<commit_message>
Update images link in spreadsheet
Co-authored-by: Lucas Macedo <lucasmacedob@gmail.com>
Co-authored-by: Felipe Moura <felipecandidodemoura@gmail.com>
Co-authored-by: Mauricio Machado <mauriciofozmmff33@gmail.com>
</commit_message>
<xml_diff>
--- a/src/utils/seed/PlanilhaFINAL.xlsx
+++ b/src/utils/seed/PlanilhaFINAL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasfellipe/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4ED486EB-6918-46B2-A620-6F1DA725D690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADA6B5AD-9102-47AD-AE48-5E12BD86FE8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36960" yWindow="3120" windowWidth="33600" windowHeight="19080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -85,7 +86,7 @@
     <t>Foto</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACOvoBAdVT_LsDOm94FyIsaa/IMAGENS-PEIXES-COMP/Acestrorhynchus%20falcatus.JPG?dl=0</t>
+    <t>https://uc473ab1d3f024f3cbbf33edbd68.previews.dropboxusercontent.com/p/thumb/ABd35-HlKek3gYJfW_-58F--BG8ejvOla5SfBjpI3pp4JgnezXwiHyrKTOkc1XZE7R7M3wnT5VrsO3ZpV7esgIbu9F_uT1sE8XUfhESBUDx-Aocld0ab_UwEPmwM6EnA-vRVepgtGjLdWctheSViJtbXYEgnAbcVFNtV4xVXMYZGnbRe-GMOgbcudYMEe7osbUBpB_ArSTyGTNJyGeHLJF6jStD02dzStybiWaTmTus81lBPVDw71XTFkp-xplaSAP1OD4KYRJLWwjLioHbpfNf4Jh7TTMqRpHABZ8kr_KM3fYIUTX4I5kwk3rHe1Ic9EAdvCDtBdyuFP-po2IlEMDaSSmHjUVacAsHqrVVLJTQrabv_i2BaybDIiuLNRAZFrkk/p.jpeg</t>
   </si>
   <si>
     <t>Peixes com escamas</t>
@@ -112,7 +113,7 @@
     <t>Não</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AABEAxtaA4Dh5nclQTWMOEDwa/IMAGENS-PEIXES-COMP/Acestrorhynchus%20microlepis.JPG?dl=0</t>
+    <t>https://ucf31c780d390a8cb66bb83d4002.previews.dropboxusercontent.com/p/thumb/ABfvSNrt2wHEshyUXbzezFx4rof0ejdFSFgV3ucUEcHYVL-kJPI_XjqCFth0gVnM3YQubDyS-roI5UiHGWUlGdCKW-VnXe4KI91oEoshW90C4hhImFx2TtHAOVo7R4AwKeDgAcAEUK8_X0YkjUN4AsMmDgDSrbRVOBiK04A-ynnOGLBBXaG1tFVdQ5OAB3PE8VLgHWG_CzG8g6B56-dxta-Gi29OU39D_5qoi-rtnt2dKBmFDF_PMuetx6oKWUss1N_73rWo08JJvQoIeLFt81jphaZAaYnZwm-_77q0AwqJRnp2LZra6BNIYw73wgmKPju7be6iKMcq_CvfoXaNiTQ23b4Dv976oSxfKZPMVhribnnMLRaI829RwExIgvU1e98/p.jpeg</t>
   </si>
   <si>
     <t>Acestrorhynchus microlepis</t>
@@ -121,7 +122,7 @@
     <t>0.23</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAC1-kwhCZ4f84-J9AKmpRVSa/IMAGENS-PEIXES-COMP/Ageneiosus%20inermis.JPG?dl=0</t>
+    <t>https://uc15704c31ef47af00a5100e660e.previews.dropboxusercontent.com/p/thumb/ABfLgn4nuKS6B58Y8iha9_NP5pFYu8UE-oBUf1XLXvpznfbTyrmqGDC12dpXEjh4pDbLug0m_XY_M8PSq-Vzqs7y01_V1FQ3PNQx_DDDy4NsrfdkPMzAr3BBDRT72xZKwC8lhFw4y3Wh1vSmyh3giSVflqfNKRiJ25RUlfNqbjl9-hr0kGCdvqoTbYfMosSKm66_EyHaA6w3OurRfp0EBQJSiOCK_fFxANOON9HICGAM21Z9YVKFj1DLFL2rS-olkazswzEtrafk0ZCXs4ed_KwDkPU0gk2LQ-nvNJdONtzJBhGtKCLWaJFH0SbohwUIEyBhNHDLyjILX8uYXHtTYS8JNiP_kfHV7uRPX97nMfUx0EMbmNZHSDMR7oLeOIMinIc/p.jpeg</t>
   </si>
   <si>
     <t>Peixes de couro</t>
@@ -151,7 +152,7 @@
     <t>Sim</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACL-fd1Tmb7cGhSrLq6k9uVa/IMAGENS-PEIXES-COMP/Ageneiosus%20ucayalensis.JPG?dl=0</t>
+    <t>https://ucc148df5b06313032c7e0f97ef7.previews.dropboxusercontent.com/p/thumb/ABf4uk6v6d7VKHC_Q-SubXtWRc9AXqFdJJkf0O3j-VkbjDRnHoqUsGIEIR_zMS1gxtxWoCyYJBUhLddJsGkagrPocSkMCYOO--qYyzRbjsms67klia86qCXAO3X2HFaj5LIgf8ZoW9T2WIO-CbLexc8Q8ItM4c4N8cQXu-FUZsOMA-o6rxf0SSD9fdC1ZF_UtdaGn24ceDYjOnNCBHQhfY01OqrW6SCr8wDibRcmjbjhz8EfVGEsQ2wO49hTuyB89SwzASNNRc3scK3A-DSpzpudBjghyvS-Lifun_iIL_OcYYTb-pgd9WfoZFlx15U7uw0mVEoXJbLXcV4RCmHNDXkgAQw0owElzn_Ma_2V6bi73bAmnR96vUlcBIr94-RmA_w/p.jpeg</t>
   </si>
   <si>
     <t>Fidalgo, Mandubé-de-ferrão</t>
@@ -178,7 +179,7 @@
     <t>26.8</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AADTl_cHBvIEp7uf8Lm3wILKa/IMAGENS-PEIXES-COMP/Aguarunichthys%20tocantinsensis.jpg?dl=0</t>
+    <t>https://uc1320008bc34c5317b6b1822d2a.previews.dropboxusercontent.com/p/thumb/ABfhKXlBCJDrVdSiBn1Qh-c_4QMP7ztUIk6Q3WH5YOHS_sAEQnCNKfyS3IBf4kQIU7UabqN0xeJp8mfu4DzWanZVwG8Xr_-GR7VSZjnNMuhex7RucKykl4BtAfOez2kpZYuX0y6IyY4RoxSGcncCjnGKguFAsfy9DN6NjNnv80fGtEABFGYk2x59mjAgStzGaGPnwL0SN0UeblOgSsGPN-hzwlJPGvByuOFcKyMbpyGLrPpy1DTUh1Fsfcno8KBytzPTsdMvNnaNprrUbJ97SOegiH9SrxrOKrtACWB_1s-4A8HlhqPNPUMNkQM0g6VswNMpJBT1uxFuuZATsVbRf_NMkdWc6h2qykTDPtHymBuSRm3zKxIRmWN9CuOVxCa8A4Y/p.jpeg</t>
   </si>
   <si>
     <t>Mandís</t>
@@ -208,7 +209,7 @@
     <t>Sim. Categoria Vulnerável.</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AABKKvS7AB0WzAzAjUbAIpNta/IMAGENS-PEIXES-COMP/Anostomoides%20laticeps.JPG?dl=0</t>
+    <t>https://uc860f724763eb5cb06b9d45f458.previews.dropboxusercontent.com/p/thumb/ABcC8X7UzVhvtB-LBC2rlqTQnbeOUXNe1CoJITGDdA-xReaPCK7GatDcmrGcRxBDKFLt4y3kk2F7bomW-OQx8b7gNC_dR3oiBreV6wrlNR0f8NygS-Sp1C6f5jBHIU1aMJvmRM4LdgKo5rMbImq3aC9zhcvN7r5wokaD0lkUH6lx9ENa01N7o9PeMcseP03BWOCzXFhht6MAmNsll1E7g_46oL6-u5l5J9NEAV7bz_8FcLbAgEjzONS2u_and9Gy7TC5Jt7jUxJ09vpFJVDgflCR7Xki8c7V-MBYupKfDQb_4x7xpylg1dtwjAkVkSg65FXiVEQMG8l0KmPHJhoxe557N-Gh1fS2r45ijMOsMD00caH4DZUUVu1y92mS_5M_VaU/p.jpeg</t>
   </si>
   <si>
     <t>Piaus</t>
@@ -226,7 +227,7 @@
     <t>Material vegetal</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AADcuOnBoEBepXsWGl4Q-ctva/IMAGENS-PEIXES-COMP/Apteronotus%20camposdapazi.JPG?dl=0</t>
+    <t>https://uccf4644f81a66fceaf58e01db71.previews.dropboxusercontent.com/p/thumb/ABcywBm5eEC3iAqGI_6-2zXII7af5ArFqPZuJZs48yenhrrXzfvhOjEyDyWKFb6UZ8P6NqaWkcZqj8YVwOkFo_7MPdaw8u_AmzOV1ig_rbycO_k9PM7zOPEg6jMMRbqK4QJlJAph3g-e06jTT78vUjJzlsuQelTCjhmxyG8UskvZWZa4rsiae041QdACjWVky1IL2hQ7KGQpE2zpV-YrcZJj2Fo8EsdWD8UfNuwR_58dx3D9tg5TMwzPAVe5VxxuH0m2GBeCmIqMlG20fXEKBskDdTCRN2Nn4e56G7waRsLrqPauFVfVUS9BpV3sUgzMnm86yWAE019rBoA7K4bUB3ew0BVIfNpnKpkKLkXAE9Q3-8A0dQHhEhNh7LX9iMxzemE/p.jpeg</t>
   </si>
   <si>
     <t>Outros</t>
@@ -247,7 +248,7 @@
     <t>Lagoas e lagos de água parada.</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACKOcO3MFPlt3G4UPEXRdTia/IMAGENS-PEIXES-COMP/Arapaima%20gigas.jpg?dl=0</t>
+    <t>https://uced6fd332230c3bf19d74637d1d.previews.dropboxusercontent.com/p/thumb/ABf-baCszaI5sdiapyAmAQj_wSZ8FROmDkmx2iOa2LQc_8IuKJguxLllpUc5KGbgUABdwPYkTGmjpZ3WisvoXMFNH69QZSxI_aE2bLfvZMJIG2EisIouZX9B9N0l0uWeStisI8tU0byxJG0o3AiF-_vgLBA4Za59rJeBdDZsElPeJ56nHtg68sXXU1TXucwIR3mpe89lTj5ni3h4a8psOA7XORzsOYNI8gvcteIue0jxISZWWU91oV3ofDpa9zd8OPV3OqHNDe78EPDYA_YQawKUT7tNZ_xCTCYLYwCRGeW2lCe466tAC2YXPvmq9M3udpXLRrB1RJnoMm5HGFaB7UVfsmcTVWJMrA0tY0p_d04ZwqpAc9KgwMM293oNDQ-EIRM/p.jpeg</t>
   </si>
   <si>
     <t>Peixes grandes</t>
@@ -262,7 +263,7 @@
     <t>Arapaimidae</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACwpkfwEnEbqcs6MYX3x7Ema/IMAGENS-PEIXES-COMP/Astronotus%20ocellatus.JPG?dl=0</t>
+    <t>https://ucaef174f583543ab756e8ff877a.previews.dropboxusercontent.com/p/thumb/ABcXBicarpH7Of3YzUoWYdgdDRi4ZjzIk0YN5dLOaxy5nUjiPbMJEGOgWmOKSmfOXdYBLyuaKe-P5xF9POuBSOa_vI0RHyz_FaZzy9dGWeJa7vtz-pL8xX46EJYqz4o6KMLIDCW7e_n5d5SsKixonXnNhMybyS1jXJcH3BT9-t2c72xb2nS-rPMgP9YuP4YuW1g3lSxTG9JuHOzm3PJGR59ne7SZaeIZFLR9aAWj2PUZm8-sKyGSwznXyAvtmnbmnaC5B_SeZBfC2_WZi9ksFS7-xIHeMqv-dK-3J0ADC3IRy1lmvWmfirxltdEZnZshLbDpo5RslmHL0w2KNyNJXByN9j856Oy6eg84Df7L5IxXdOR8ax0ozB573N9UM_f9pNs/p.jpeg</t>
   </si>
   <si>
     <t>Carás, Marianas e Jacundás</t>
@@ -286,7 +287,7 @@
     <t>1.6</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AADS59v9j932QvJo-VpizE0Fa/IMAGENS-PEIXES-COMP/Astyanax%20bimaculatus.JPG?dl=0</t>
+    <t>https://uc92cb6266affa5d3e9769dcf1fd.previews.dropboxusercontent.com/p/thumb/ABfY7l0ZYU4UOMjp5GsNhGoADEAoEL31Bp1kstAHTajUhWLGAk2tZym_3p8p2JFeFpvu3TeZccqkc0FCQsdFQNOMGhuu5_qwQgkNfeUH0ZcHCbHYWy7aTdR1bhKD7o-zWQq48ExkiI2qBqGS-oND0PRqAdCkpudaU23sL0qdha87_Q0ErZ0Wn5biWboy3JO11oUSSq87QTtCsuk3WRoy8i3hsWpXcTv-BavmQFbQw3YBeB6wigzCBxQ0fGOei1b5ZQUQSIgZikApkLs3TLmk4I1oqdiHnQMWV_eek3-o2dAIrF4XngHKhmw0qBpMAf1qIF3m9JcSj1vmihNqNkWR-mUz1zWUJALVtydoVINXTaJanN9pYETdvelkzfeMusS4Z0E/p.jpeg</t>
   </si>
   <si>
     <t>Lambarís e piabas</t>
@@ -328,7 +329,7 @@
     <t>17.1</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAAKiUGgB9LXtE3VFdUM0qkda/IMAGENS-PEIXES-COMP/Auchenipterus%20nuchalis.JPG?dl=0</t>
+    <t>https://ucbd6e7d45ddd17421102e97f896.previews.dropboxusercontent.com/p/thumb/ABeTYMw30DLWY9vkX7h4yC3ZxmdiCtNLTcS1NRSRZ6kk6JPrrFiMuseh2-P1INuo96aKCtbsPl4YbbG9wyET5BfwUxJQe3vOLwOEwC67_xCKaxCJ3uX8DBVz4CmbrwqbkUuX6ThHEvmWx-r0f0wftvnm6SCl0iRrGiCO8APA5gn_032gTSwT-kUlXgeRmNn97Vfc1emOkIWFi5Zp-vR-OdjnVofdGAVlf_i1cf_ceP56p8lD2axHWDR2SWTc4D-4EnqLxigWroC8QWxRBdAhNfX7ZqW9AiJpMiPtzMCeLQIa9b4cc2lgPdeUDZvo2f7EOihk_-iJKMa7iY79ZB17oE6CbElu4Jeu04b26SZ9_QLJj82EmiCRw_kcIKOM5s6NSYY/p.jpeg</t>
   </si>
   <si>
     <t>Bagres pequenos</t>
@@ -340,7 +341,7 @@
     <t>Auchenipterus nuchalis</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAA8uU9QkyNVZbj5tyTrp-Tka/IMAGENS-PEIXES-COMP/Baryancistrus%20longipinnis.jpg?dl=0</t>
+    <t>https://uc08263df58fceaa972604d388fc.previews.dropboxusercontent.com/p/thumb/ABd_I2DRoxRS8ST69OGSPeeADEXe02lMpiS45psSxyTjpICHJln8UASXGNUbQQXhfFGDHzf415QiE9E1EcE183v4x4FPBu9JxGUpjdzck24-7hEYbxmU3-qPa_vQUeTmArXygqCaMMDoe2gtoo7S4Jvw2U24xwJ1bSzKaZfIaCBYkG_2FC3-gaXYZTudlO3R3h3MXUtiS0TVVnKyDvCeo17F7t1XzsRHsW9aynSHgY9QeNxbIu-k-KKLAFTUxxWnSUmipBFQRsgBKm9sbluym2YVZA1c4J1IzdBQunxCu0wGempjH0tSyC04COtX1ETOKINWwDnfbFAmMt1chnV_Scj_QKAicbxSIYAHYf52UgpM5XYwdKQLtjf2QXKQ2c-ReFg/p.jpeg</t>
   </si>
   <si>
     <t>Cascudos</t>
@@ -367,7 +368,7 @@
     <t>Sim. Categoria Criticamente Ameaçada.</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAD08I99JATdNMoA2MgqpJIwa/IMAGENS-PEIXES-COMP/Baryancistrus%20niveatus.jpg?dl=0</t>
+    <t>https://ucd9a971f66696830c6121de558c.previews.dropboxusercontent.com/p/thumb/ABcLb3fcVnGTg3daAk_e_-25Eu75E8K4fDN4LGRD_Ey8PNH1dLHojua-zwbrcr2FvA1h9WVCw6QBUoevNezeUixlCbFUB-t-lSplZbzzuZPzTby7D7PlKlsBUUKDQ7O_9l5aeVdAKPlOVseDnkhBFJbZP0GnVXoekZMeq1eO5GE-cYS39vfBwCetw9-FBwnbIZakSLcSmnzkBca25zIwdr96muQjss_Ih0kUYFjiF-SFfHyxua-sJ7stxeWAWTq5ridQDfZfbhdMAk9rBFMf_G87XXnXZYsD-9a3ycsFoifNi6m98k2J0iXn_-GOGBaYUR01qua3ii9VaXiOFEWv06EXoURVp3aZ_EwzZEwn8mPKbQOIu0TyX2oz0yO3ftVZZQE/p.jpeg</t>
   </si>
   <si>
     <t>Baryancistrus niveatus</t>
@@ -376,7 +377,7 @@
     <t>0.52</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AADhhyx8HeN8kMUPE9ycHwM-a/IMAGENS-PEIXES-COMP/Boulengerella%20cuvieri.JPG?dl=0</t>
+    <t>https://uc4bb6b3c1f5228dbdb0476eebfa.previews.dropboxusercontent.com/p/thumb/ABfrkKHt4t09k2TPRjPdR44hbWooSdwJCFeG9SVmarwHBZE2eskrPCe0wTEmDm17Zugi_hK1iKWQd40HsHVUWbsny1tEtQm2KkAUd3iVPx7MNMriWrgNfIseBeVwYy2j1L11SZjwq_5OSbGnt45CNCfU1nFxHn7WwJ4RP694nTFe6if0z697J1Pb0mCPjRLPaNf8czNaFrZCBCruORTJtecpCGL7Yd676CtSAdp26tMWJrGl_ID9_6oooq7348QgoBayqVcWmzUlzNFraN2pVMIhbnY8ztBRP2QjePk1EP5KojwLtzKtWzbGjs1vXNum0TdnE9YJH1LTVV7HQ4Gxuz2MS-1Dl9b8zEU9Ae1S0oyIUlqmhf7Rjn_olkSbkXVrwWA/p.jpeg</t>
   </si>
   <si>
     <t>Bicudas</t>
@@ -391,7 +392,7 @@
     <t>Ctenoluciidae</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAD-Z6EooWtpm45HSXa8-vBza/IMAGENS-PEIXES-COMP/Boulengerella%20maculata.JPG?dl=0</t>
+    <t>https://uc19a682a333de699cffab6bd721.previews.dropboxusercontent.com/p/thumb/ABcr__zGSNirOGxergW7PZT4A3irfMOAMdQcLo0GM6ZTQ0QgZ2jjmmY5tFMmn5jOjyEL2tMUzwk12O464pv4GV28bFF7ZipcQRLajaM_kkn8vWJUDVM3mISTnG7Mx2g__lzFy0aicnxjy2vh6Ot0UarX1hWlGqf4Dh64stxSqFblcEv6udPMTzmveBgaeN-D5wWHwKQLQNukaliIh7FQ8mCxypsv7YNlG5hlLnEflCwm9wQj6-KWHiCOs_fCbHnfyZOsoWaD4kR4WwRx5jpAe25Y7lhQ16iOS24qWE-Jz9vf6ct23TpG8vXULEPiB0a0Euw7rUjKW-D-xrUfkaUv1Bkt0WujneReUTUkFauVtUNjd_F_fsCC0iy2GnI80YU_8GY/p.jpeg</t>
   </si>
   <si>
     <t>Boulengerella maculata</t>
@@ -400,7 +401,7 @@
     <t>31.9</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AABWBuirkQ7Vz462-VAmwFtUa/IMAGENS-PEIXES-COMP/Brachyplatystoma%20filamentosum.jpg?dl=0</t>
+    <t>https://ucc6da03eaf0e3e046311b662740.previews.dropboxusercontent.com/p/thumb/ABeihBhH2xERpTg2Uz6cGsbtn4cn_RR37jnaAHzr-VQAU4RmU2DkOirJWl1HCSgHZguSgK5upQLkyufQgzKetMMgw7drIknGKWMs1VwMmRBnNgDEXOXe3TAvqyDVrPCiPvXQKuBwh55PU1FjlIiMem-ZTDinb5f9VyeWxGCI57inWrDDj82OqoRdPejJw1W_sipUdcS3Q94M67_BU1SQ6KSnl93kj20TarFR2RV6bXGS7IIDv8BHfkItN8yv6UgHmKySdo3rrDCsy2A8560LBs8YRebOC8gQ4UVPCUusU1nzVA70iwgtmlgxNdBsKE3VR_8NQCwgL6O9_rEE3EEtQxvkRXFPktCrvTsS7Rdz2L_K_JgPdizHEeVmX6wiikIdAIs/p.jpeg</t>
   </si>
   <si>
     <t>Grandes bagres</t>
@@ -412,7 +413,7 @@
     <t>Brachiplatystoma filamentosum</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACl3wSuARy_frDZxJjf_Ztna/IMAGENS-PEIXES-COMP/Brycon%20falcatus.JPG?dl=0</t>
+    <t>https://uccd98bbaadc614b0d1c0421fcea.previews.dropboxusercontent.com/p/thumb/ABdFSqk-eHyqtI1aLWLS67Nlab4MZDJAPVc00G1CCLwUoxGuzEb3c5cfTx2RfmKovsMy3zENIkpZOqoSiNofvqfecnNP314HFxRs-pAgiGqLDSbj7_Yb0ma0C-cf8TDvDjR4iQyu-Eu3uJ2gd71u9qAG15OxbhlEZVjmpqlhbXlFQPJ3zwTQ7A5PZ8kRpMyVUCDkklr4kYeeexmMF0UMBlzcGSHEpBPux1kY2eKlROw6NpLrZT7TNuzFjhqdxxHGUHcwM9K2jO0s9q8BSMoC81z3-8aV_NsmdkUk83qv0Rgc9pxbNHB1UswNAjFq7Hol6ehn79JBRjTa2E81_Z8qYL5rIaCvDPqtF1qC18RgST4C-65o50r8JIsSbXgp355NoKM/p.jpeg</t>
   </si>
   <si>
     <t>Piabanha, Matrinxã e Voadores</t>
@@ -427,7 +428,7 @@
     <t>Bryconidae</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAAQgBdI7ArAzS8kpRpvGD_Ba/IMAGENS-PEIXES-COMP/Brycon%20gouldingi.JPG?dl=0</t>
+    <t>https://uc345ed5ed39e24ffd35e7e64f65.previews.dropboxusercontent.com/p/thumb/ABfjsLapW6mM5-nbh_yGcFS8YMYkM_y3Q4GAtilBJq0qltSvXO_V2wWgKtitdICgJtn7NSpvGwuHsYMVQcsYHVSTQSEF7NNEp70eoY4yaNW_WA0I5RrlXg6TmuFvD1fVoDETfJE4qRnyGbbjopXHK-o8-ZaZ4X7D483hEDfmuSG0AaZB3MMZgVebuYpR3tyZSXnToPcAatFKd7N1NTmtBLgVtu-4nWOitk6Jvx7KS8rO98eAOyYg-8sgid3bngK_hzOkZ3FqURaIh_J7R7TNqjAPXiCXbqZSnaBjTHWu1xkm9dCkqtlQMJTsQfdmudvbJyK10l9jkLguncjPoa_Kr6-O-YiduZacKHsY1TG2GDFaPLKmkN0sCVay5Jj24G28NhM/p.jpeg</t>
   </si>
   <si>
     <t>Piabanha, Matrinxã</t>
@@ -442,13 +443,13 @@
     <t>Sim. Categoria Ameaçada.</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAD701vyJ3Hm_dqfdgmgYPJ5a/IMAGENS-PEIXES-COMP/Brycon%20nattereri.JPG?dl=0</t>
+    <t>https://uc2b79bb46a20601ea0a9005caa3.previews.dropboxusercontent.com/p/thumb/ABcswFlE4ILcoEZ_zpUQGw7aESPpcjyf25nKwBuYh81bb-2VI9SVWsj80zwK4FKvM-Vu1bUKXdO2Ns4jkIaBPzcGBnPfeHCqtxcOouKmQXVFdc0afxLP7zta1pYKaEnMb2dfinHjHoA1ebEk_b_XHbYB4puqYZ_2Jw41KtGA_tZZPyGm7CWUPOUVu7ErcVp28iGCXfJAR-GdYgKtm3FHeqVr0wEyY2sDMHdzySy5o-M4GuUaGfOsKUyDRTgu9LVRPJkVNtEHnuZKu_hWIBkmzyfbpjQUA1wPAmWKh2DIfm5oaZP1ASVP5bZuhlyp0EytEhdnbAlkv3Ds9isjWTTDve1nxjOZB8dsW2VYi8L6S0IEn8tjkQ0IohivMzBDhzvZS0U/p.jpeg</t>
   </si>
   <si>
     <t>Brycon nattereri</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AABp6rgaxb35cRKhoO7tVJWsa/IMAGENS-PEIXES-COMP/Brycon%20pesu.JPG?dl=0</t>
+    <t>https://uc592eadf8510f13e4b97074faaf.previews.dropboxusercontent.com/p/thumb/ABdTq1Do4fFrME_wh2kB_HaNfWJEUdhkZAE0hpBwBAudR4zAjhEjdh0SxpUTajGjQU8U6V8uq99kNEvNuLjqgmzr6KwZQeBzCGLe-g8dLxYbtixaV6U-CnsCRm7_BdzA0NFIWXB0Te1t29WoOHWCpNQhKKf_DeC5XBV3jrrBYGEl3-7Rq3f_ok7gLh424ODNvjuqgwjjXbGCmo4JPuX371p1HflN-PDs2OcxurgbWsHwtJHrNzXV400c38jvL4bKnBaRL06gPvyzek5zB4WoQXKqYE7W-3K0qyP1Kg4RaU5-jghQAsTEwKVi1kAaaVERXpiP4rzJN0PNTF7VLjGDBmqGu5SfQom9OInZQCUcjf7fUPeQTWk0O64yxhRJ7OFp3Jk/p.jpeg</t>
   </si>
   <si>
     <t>Piaba-beiradeira</t>
@@ -460,7 +461,7 @@
     <t>Peixes e insetos</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACe1TdyNs6Ui0MLZKAQ_0F0a/IMAGENS-PEIXES-COMP/Brycon%20polylepis.jpeg?dl=0</t>
+    <t>https://uc10a0379f6ac2c632d278e42544.previews.dropboxusercontent.com/p/thumb/ABde3rEjudZrtHDZAy7eVJTZi1GUnyCEjx2YJ37u7iaPmO1iQkpIe1u1lp19cLwc6T09PC8lGZ3rf3q-GOiA4oqwB7m3ORQR8qS5UEvJVzQ0v29_J3wVV8o7M2Uqg4yETeW3tfMK8OjuixxuCXnKg2zuwY1F9kLIlAE5oy2GraFxSvEAdpwxDCkvK7Qj2fl7bhT4eMHyJhmSxnzXOvtoXp1LCjzR4K44dZ6YfxVI52Nh9Nb3ejV8pTZRnrStFaDFd_guolUrKdQfE1iFxwo--T8pi4DI2XVufjS-YMlJvvUhhIkcaa3dzQEACJT1ND1vBkaKK4bETx3K5mu8sUeNV0TU0BKVeL7K6IEK_6WuAl3EgfFkq0RaPmXEPP7pCml3Hr4/p.jpeg</t>
   </si>
   <si>
     <t>Brycon polylepis</t>
@@ -469,7 +470,7 @@
     <t>22.4</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAB1LQTY4MHrcrsvC1mAiMRpa/IMAGENS-PEIXES-COMP/Bryconops%20alburnoides.JPG?dl=0</t>
+    <t>https://uc2d44ad4a301a2ef92ff0739f7d.previews.dropboxusercontent.com/p/thumb/ABdHeAJj97hKkkZHg9NfbaDynhGw60VpuSLK-eZD9ZWdqGFuh1FfwojBAlDdq6nDlcaTZADWzihL3XR9q5jFfxC3VAFouFQpYu5HqiJ1Y_dS7cge-bKByJHZ2vuRdTtMmdQ_Xu2fQPK2twYqqB283ym1Z76zdi1-HzaAaJI9OvdlTQfJFgeixzC9Y_lXSW0cbIcIIZAAbnP_XNAALKUVY7WN7bnNKANhJ5uR4XOJ6K4e8xC9Vg-T9c03WLIoe6UYYN4Q4IopsyA4veroabFg9uzPcvDtnWq2SevNYUR7ZlYSoyTzU3qfLY7dmT3VEGSNXHgRRepG_FhpZDHMKJLC353XOF0YgVVUaY7sNNYdn0CctR1X3PKPpo8_9Wb0tsjyZOk/p.jpeg</t>
   </si>
   <si>
     <t>Piquirão</t>
@@ -478,7 +479,7 @@
     <t>Bryconops alburnoides</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAD9DJqOOHa76tfiOWazBk07a/IMAGENS-PEIXES-COMP/Caenotropus%20labyrinthicus.JPG?dl=0</t>
+    <t>https://uc5f9904111d3ea55b60b4143c79.previews.dropboxusercontent.com/p/thumb/ABfH8e1ccMfimWukD7g2Ahk8gAFcEJp-X6zPDSD17spYlpTT_vDzPs9YHsaUTKTr2M3iaYo3AGI6G_riBQqumy6YVZJCHavjD5Hbt9YV8UhiRv_Zu7Iah8fJY9FOqJ902mFlc5onL9mN1vJcsgqjw9qWL8jhJAi-ZxoUvxccIYwfrMptzLO6OK2zwPF5zvIJ2qUUkjNNvuybjrE1gsWjB5Q1NJJmyRpblNj0k0cAE7kryDEB9T7yhpXoRWt3sRsE8yJGVTtlPBbQqwWSey6k-8CIuI6dVsBbfIVzbPGAJfUzTfuaAbzjhX6_nRjhTUD89aqFdLATvY_PqJ3OCy-vTnKsUlsnItxQuhtOcSq1pqFFRw70tDThF-OqWr6QqBLww08/p.jpeg</t>
   </si>
   <si>
     <t>Durinho, Cabeça-dura</t>
@@ -517,7 +518,7 @@
     <t>27.3</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AADAZE5M321M26Z6FqVE_Ktaa/IMAGENS-PEIXES-COMP/Chalceus%20epakros.JPG?dl=0</t>
+    <t>https://uc015a5380f769f4855e21c2ee41.previews.dropboxusercontent.com/p/thumb/ABeHsHXtDdx-su1lpGhhok6ZUK8fotSjBBfvH-ONfS8Vbr-t7IAO1QYGyAZ2lDOVyeAgnEVX4aB6vrDaaw1p1JXGAceCuYQkpK_v3YQY_ssBIBXKLQxW60mILiLkbuY2F5Z05RNp8bLjyd3gr8GrZocd575bSwLj9uqn_RJuYCbKP8hPHK4YmQKeFm2oY2hVRDNVAuz1EIyMRLx7WL2EwvxoePthxQ1cqyn9v0JlOTu8LwuoTiZBSK0VFc_yCJgRDaED4VmiPQ8H6GT_sdnsMu5Bux6WD54ItYPZ5LtMP55lU01YiNkNYz4_etBLCJnfimulEV_IZxTJG1swNZjLz4x0X9Jg-qiYGtjlWF0-XiDf5j_Qn4USPvmTX_iZhKFCzvs/p.jpeg</t>
   </si>
   <si>
     <t>Rabo-vermelho</t>
@@ -535,7 +536,7 @@
     <t>0.07</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AADPobuDvJtnEqbmXW50pNfMa/IMAGENS-PEIXES-COMP/Cichla%20kelberi.JPG?dl=0</t>
+    <t>https://uc12acb66874afec202097dd4591.previews.dropboxusercontent.com/p/thumb/ABfTT9ii_MHe5YrmU_uiGP-J7ezlghj__KhpuCZZhFwnEgFjwqwhu_StH18j0Q41_uuq69AZDa11Xjpd8oxbmc8LXoX6VlAwu1LBj2EYe2bESts0xu2EA_e0QPap4oLgvbV-hochpepcCWCpzREyFu1b46tY9wThBGfaqX6YRYjNxtIwzxyOHN_1QXo4ZynPjPPvc0TD8D-kSrNM3aVkAam2gpZVhNqRx9hMDNZNtRMoXfB3DpiezxyUrSRQO_evT_RKp6MZwe6mpY_LSBfX8_X7I97JmaMAnw64zMERXWZqvMW7gGXWJZsdLhoU4auYsZlJrPrQ_tKDEVC50YbR8HJ4hhRO3JnkLgB-upREdf8__oWqtBZ4ISjfQQmSdObWynE/p.jpeg</t>
   </si>
   <si>
     <t>Tucunarés</t>
@@ -553,7 +554,7 @@
     <t>4.9</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAD93dnfwBSg4CRNg4Qj25Lea/IMAGENS-PEIXES-COMP/Cichla%20piquiti.jpg?dl=0</t>
+    <t>https://uc9d070795294239004b99a90d4a.previews.dropboxusercontent.com/p/thumb/ABen-JYsStSoO1-ysZ5YNeXxwu9wt8d2LpQPC_DNSvBXY7W_sclPq7qW_XW1X8aPvvSQhhdSrvrrJVBRykOvHTcqJHJwA_6mahaMlGPJQMEU6E2S-Aj1E4V8eADkB7gj7i06RlzDCPvqV_4JbyTMik8hrGed7Bm101hNe9lJn3IDQz_l25UjEjpWG_gZhKcKkJEEBM8f3E8FvprPfCwwbBNvD8c4XPbIFeCZyLGm0tavByEltpwZZLc419RZOB-M2UFARoksOotjBLeOIDPBU5a7FoCsknhZzPAq0WYs3D7Z-lBt6LRJlCs8Yo4gWQAPMweHdGBOpU2ufxuHCuiIEqxR8Wp_t_u0_ba4qgUbDrCyIy_Ni_I-sK6JxQOzNmiEhEk/p.jpeg</t>
   </si>
   <si>
     <t>Tucunaré-azul</t>
@@ -565,7 +566,7 @@
     <t>1.8</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AABrBaRltuJIkT8cJcysClAba/IMAGENS-PEIXES-COMP/Cichlasoma%20araguaiense.JPG?dl=0</t>
+    <t>https://uc5653b21c4bc4c0a5559d6f0a6e.previews.dropboxusercontent.com/p/thumb/ABdgl2zQ373P1oZbyF0DD1gaHUZQV74_VaLHkpZYP8i9KMLxnQjc_ti9lylW1szmqSVfryr9dBsHVwQYsRRR6u8MOcFdG5_7EVaamMk1Cq9MCRcx0VINATJvp6JdZG2CETm0AVIY0soFBKO5Webmtu_hLyLIYiU5LMiRcfbnUHWigI9a8sdu7H1CnA4OtsyNxUMfZgCT1KJPxg5DzhrzUGJ9R4eSYqyS-XyeKrT14N4VNajYTTp8VEaqNxFblyU1mxEgSf00IJeu8EghFz8cVqR2PM9gPp6HQwLJ7gjNx4cXnZJOB0g7O2BCrXP2ivkqSSoRKsGE5uSQOuHerd9Qovz7zkgLhIIjura582tyae3uFkjr1VQeQ2vJbq8tIhuZ56Y/p.jpeg</t>
   </si>
   <si>
     <t>Acará, Caroço-de-manga</t>
@@ -577,7 +578,7 @@
     <t>0.3</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAD6A-uZ3Y6yTA1F2d3gOfl1a/IMAGENS-PEIXES-COMP/Colomesus%20tocantinensis.jpg?dl=0</t>
+    <t>https://uc78db1fd14f1d1206fe0cc7167b.previews.dropboxusercontent.com/p/thumb/ABdBe2OTfsoASkyiEA8EMjaFblapWk_0Z6DVP29u1hWaSdRX3xJZrSF9rUfQX0i--QysFcuzeSxdul835MzMOoleum_dbNRPUJ3GRWRNeDrJQZglyBQIBEScLtVbevsUPUNIv-8laLRi1Q0nMpeI_kATW36XhbboTDA9kMXNrc3O5ykIxD91dnUPjtjb7-sxLvrM6RTCj96p8mfOml-pLeHzkyJD6WFBn5ABqZV3Sf1aPtOZlQ7huqqNfbB8wSukgqhr6BBTwIf69n8BPVhc-jQ1zzEcPeInqdEZqwhtybTfcpFcrIn84LBfv1f5PtkAHVtt7iatoZMXXuvijovOkc3VG0lvJ_tdAO5SkrSF548lHkS7llTHti5AujvzE24TyKA/p.jpeg</t>
   </si>
   <si>
     <t>Baiacu</t>
@@ -607,7 +608,7 @@
     <t>Crenicichla reticulata</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AADs_J7e9rNlEF17HqEJW4nta/IMAGENS-PEIXES-COMP/Crenicichla%20sp.JPG?dl=0</t>
+    <t>https://uc072b77bbb7522d0e1bae4e7a26.previews.dropboxusercontent.com/p/thumb/ABfMj6D5GnSlUv8zI7xmTY80DoA8D4-1C2KxlRqlEHLRfvx1dDJv1ujBqFNiKGN85vAE17TFN-XsfJixbjitWHNETuU2MyULJG6Yw5L1vSS0jMPkqVsbZfusnuzJ6MGJdmyRZnREPOdc6VdMdjqiJmwaN8n4o9usTFMoojYbgjfvTWgP2jlBopTNGX6vdBHbW98rmG_HFI_fhONfJs69aIzH8rSJYgmIHYOCQjmu21tgtsyNtXfXNPR3Fs-BzQCO5gqrlPwXSek2V3QCpTU10tWojQ9NrEguu5zuUGTU8qVJYWFFdgWISrgQt9FKTidSTGnKIQGrtduyPPD2zY3m16zoY58h3qcE3uU8ycTgtTUkk_yVtyFlqR3OaFYCcC3BQ6A/p.jpeg</t>
   </si>
   <si>
     <t>Mariana, Jacundá-açú</t>
@@ -616,7 +617,7 @@
     <t>Crenicichla sp</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACKkAF-OWo-AmSB7cyOv8zka/IMAGENS-PEIXES-COMP/Curimata%20sp.JPG?dl=0</t>
+    <t>https://uc96bbf2f337f688b574d6febbf1.previews.dropboxusercontent.com/p/thumb/ABc1TGuKocmlGAVpcMfBDsabwfjk7aHcgy6uy6KAE_W_aDoDxYLwBpw1U0IEkgy_9zUOEdXbIDe0JNOSlO1pGKZQ4kW9cw3AdNio5tToHa-t-UWzbtm-hOO-Cg32A5H8cckAGHYGnnAZ3_HHDwE-Hl5tQORjnvXklwJKEBN_qSzGleVdVf-jffvmnNVXZ1fkvwIbSg4pqEAO-k_Af9vq9DW8apkRA6xoLyALzvs7qLmRUscIeI2c0I_hWSwW-km8oN-WOVMEtUewb5O0aGBcyUf_3dtykWehNcF5UAwJfWRsP7KZXEEOiBMW5G5AUPcrXHBKmXN58jE_uS5I2gx1RIS6OEBx65JjR8Ij5Md2B-Ei_1NOa1MBDbLasUHdT97to9k/p.jpeg</t>
   </si>
   <si>
     <t>Papa-terras e Curimatás</t>
@@ -646,7 +647,7 @@
     <t>0.49</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AABslAzFYRzL2Z38CCTsKXPQa/IMAGENS-PEIXES-COMP/Electrophorus%20electricus.JPG?dl=0</t>
+    <t>https://uc11168f70a2fa011cec3f4582d2.previews.dropboxusercontent.com/p/thumb/ABfDJCFK_xjFZSJAI7sDp0tA1jUiKBGMJAt-xo9BN1YIbW0HnAr6Od0Mw-ME7zRwV3xyCI5qD4vCsJ-7n67V26SL5EMSs9wcz4KvKHYzLfdZI1aEr4VsVHSls-EeusRkUlKCjfflJvuCvRv1xslYpFfQVd4w9RqEc1XBjHBeT3OKRtyKylrMc49PklkJOf8TlhnWcJRQAWOwqCZFjT8WhAW3I3oF-oUi_rgD6fZGQui6SGMzCmpwkXh8Qgmu1FSR6L3MePtDprKQqq5Dj4sTd5tV53c04PorL7lev8kvtCnDVhoBegdiT5OOWEyHaWH7zCdDV4HLrzumCBB06CQF4HyCI7FITlLK3EOhT-vJOsy9c2L86KOrzOxgx3DEPQbt-5c/p.jpeg</t>
   </si>
   <si>
     <t>Peixes elétricos</t>
@@ -661,7 +662,7 @@
     <t>Gymnotidae</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAAPTZL089T3NyisVa42NbAba/IMAGENS-PEIXES-COMP/Exodon%20paradoxus.JPG?dl=0</t>
+    <t>https://ucb66a69016ce41e67c5795cfe57.previews.dropboxusercontent.com/p/thumb/ABfFC--DxJBVzIH7Om8iMME502BsMIshfLOoVNByRYyyq6HbbYaYoJZdldu8XBQ-dVzQ__RymodHLPGZRQTq47qk-DF4EwfZlheDdz1-4a1n_4HLPAY4s4y7xznXsnQ6qbSznA1kE5F5Jf_v9695uIcaqIFbVZWXPF8nVweLMxSieoxGIXtcPnbLZOVyABmMJKhik3ETSV9EJcCHHgmugvxaWg4UbaISAEj37_i22CB613cysLZPfD79mit-HvjvLHfKqH4Q2Q5cA_ylSV2Bx5ikuN4q5Q2Mz2lKN25gKcl7Oj_xc9t15ah9i52DRJOy9XPZnhikf3EOrWjll7poJOD1sFQhie3grxWfGwAVw-93V3Pgr1gCQz0EHy4iFGZq_rM6AJVKKfGIgn3Ax_xnT4kaLyE6ACZjZLkjDqgX9_vl9w/p.jpeg</t>
   </si>
   <si>
     <t>Miguelinho</t>
@@ -673,7 +674,7 @@
     <t>7.5</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAD5UGo7AKtE0FAjauJJD3bWa/IMAGENS-PEIXES-COMP/Geophagus%20aff.%20altifrons.JPG?dl=0</t>
+    <t>https://ucaf3dbc0a0373492005231719aa.previews.dropboxusercontent.com/p/thumb/ABdVP3WaxiQr5i7gh_2CAOhkwRiUiZxVOF9ktpTf2URKwTQvqW1JmKon_cEu06epgleWN1MdOeEEY9HW9nkwo413Fajjzp6JZFP3u2o_BoE6sK2C0aQC15DmCA3ulAsGSNg_Z4Eci7pZ0-GF6ZhTumP_h3Efx4sQzefPXWo3I-cEJsxgFk1sdQdku2AgGxlfmIcOfrvWBxs1cc43R-tz9xOZdIJgQroTN0O3v5caQMFrtdObThpBdZLyyhTiPh9dWOYkZXsmjbWIS3Fk47O5uw2-LqUfqeN1UViIQZo2Bg7xzlasLKxawnO9ZwgGIW9UwL64TiJ4dmhOHDTtJ4GxBR-ocqx0Zzuw_H6Y8nc3GawqqsGs2mrPSKWW-U16mHXI797IKrSLmt_FvquJY9UaCKplMBv4j7cIFQELWdqSKHX3zA/p.jpeg</t>
   </si>
   <si>
     <t>Corró, Acará-bicudo</t>
@@ -682,7 +683,7 @@
     <t>Geophagus aff. altifrons</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACyxF0bB97G23ZP6ZWvQCQWa/IMAGENS-PEIXES-COMP/Gymnotus%20carapo.JPG?dl=0</t>
+    <t>https://uc03d661ef846c2bc7cbbd75b435.previews.dropboxusercontent.com/p/thumb/ABcpNW9qaHSUHPw3Zf8H6xod8-NzabIzD7uL_zT5jHAlBEMBGthan886y3f8pGbwFp9wMcIzVkAfo6QqKyQ5dMfl0HdthnPCFVUUnhd-CxEicCZ-oe7SWwd4Imu1HfK4DxKx2nwjYq9XmcV5rroHQyTF84Zh2rCl10og-tRZdgiNjZgPnLKWUhJuby-DV2975uzjaI4WBsvoE7yRxeqlMFz1gn8fw0Yl6jL2yZUnyzwrMpGFzaTAthjeMGJqOap_G5366FJtl-3gIL_vV2gqFAo4kdoXRINWOd8vpz_TJmYo5Vw-TnO38cGYznb51yL1dIpcFGjHM1L7djcJj7jctXa-kVO93aNGMscAgv899tTC1WFFVXofXn7oNNxJDdN7z1cdelQ5aoT3V_2PwzAYjT8JSZgUYWtZgF2QHz0XSLGPlA/p.jpeg</t>
   </si>
   <si>
     <t>Tuvira</t>
@@ -694,7 +695,7 @@
     <t>1.2</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACvFn0qtcR8SZOteXKWlt5Ua/IMAGENS-PEIXES-COMP/Hassar%20wilderi.JPG?dl=0</t>
+    <t>https://uc032a835146610322780cc5f186.previews.dropboxusercontent.com/p/thumb/ABfmtClbUKIZ8VqeZDpxXG5yDfb_XyIcm3lQgqB7eNaU6dQ2mv-0CSEgHbK-V-249_4DkQqIY1N7deGVWfGIeS63ZNOrYZIRLu8sSCMdDKN4D28zWgHbu-xphMcDAvsJuHmPkFU-JQuvv4A0TaiBHfPWu3noN54yXWKuA-VIsX3JbbVSPEO1zDSKVexV0G3RMIWCLHI2O1qsSNI_tcfQujRdvf8KRM95zWI3kuispy4lFEWdmjrYnoFe8slplMciUcBxTgcCXuUvtc8SFQjkc7775B53NSuE-Jw9qC7_3-I1bXI1YPLEjH9R2WlGb15vncwUJk7-wol0W5vqjr0R9Nxw0jOnkWNZtPUdcee9bkKqGU6Uz-mQgT8p_C28PQWeGku-9RJnep2OW6weOlC3g7CtnA8DvUmceB5TTqaCUmq93A/p.jpeg</t>
   </si>
   <si>
     <t>Mandí-serra</t>
@@ -709,7 +710,7 @@
     <t>Rios de água turva.</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AABy5xWiLFJNjKCdmzmEEVe-a/IMAGENS-PEIXES-COMP/Hemiodus%20gracilis.JPG?dl=0</t>
+    <t>https://uc1f33a6f358eb8cb4fb479fdaec.previews.dropboxusercontent.com/p/thumb/ABchfz0joiYPxR6wzc0xUaQZm2sgs0D4o-ujq1MRjxcdmapkM0w_T2svIEy-XeEGAeA5T1WwsxoJEFNPqzCDg0izXPlee5mxEMT60OX3B2M1YNJj6xBvjXx7cBnj_F5rqgfD6xhaBrjMPD8us-6Ha2wRiE2d1lBKL-BWF7OObQXbo_S1HLm-nfq30bXm0Qv9u39T9xNwdukWbMoP88bAgU14ZB8vzYEVMwNcKmkht0_E6VPkjQentV1O7n76H3z8TS3vSe_VV6-7Ch4Fg9TYCmx5fnvak9VWzrNKJKvY1XQYMAUDj8mxUo-W-oacRBtlux12QUfzb13VAe7NejgR0IO7rfelr47R1kqDCBhkEl-fThc7Mbr8KUBoCNso2ouAPr4vcL_OBlTJltjGEy7yXFttcErr84vjECSVOxRpQWtOdQ/p.jpeg</t>
   </si>
   <si>
     <t>Voador-rabo-vermelho</t>
@@ -724,7 +725,7 @@
     <t>Onívoro</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AABUnwolVY9GhjMAyojHPbKYa/IMAGENS-PEIXES-COMP/Hemiodus%20microlepis.JPG?dl=0</t>
+    <t>https://ucec514f2625e7a4aba72b101c7f.previews.dropboxusercontent.com/p/thumb/ABeSpvtqHI0zqtgulFq0rYChM-_ampMAgUGpgr8pwrg-3iVIBdfIMT2J9uT46-ZJc9vUM66HHLRM9EoHsPdj9iL2YOTmHseY7jMOG8U5EuBQRoj-pBKPPpIWG_UHsjWU2814f7q__61AWNECXk-Q74imXeEEiZvs27t8SU2ntz9CCTXtS8xzRTCcX_VmdZBVUa3NN1-lG5pIzgf9_4qDj_PVtZtyp7IXxnJszFWNEIJIQjedlS8F9fRkGoFGCT9w_tecgnXBQeHAO8f60jn2YTrMy1VxeooesBImTc7ecQXoSEY8lR63Q7rTIX8xYQONCF24LHUCcP7fw4rA7AXNAxo11cL9GbqkftDG3gGFmRg1CsJ33023TaONJb4hEbaSHA3EbdTKFyG_BDar4VqjGM-bWvNayx6EUzuQ2lH-h-iuLg/p.jpeg</t>
   </si>
   <si>
     <t>Voador-escama-fina</t>
@@ -733,7 +734,7 @@
     <t>Hemiodus microlepis</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACw9JqM6vmBv2F4YvKUSmYTa/IMAGENS-PEIXES-COMP/Hemiodus%20ternetzi.JPG?dl=0</t>
+    <t>https://uc034b5b8de8b2771327a68b2ff4.previews.dropboxusercontent.com/p/thumb/ABejOCRrQW2VG9yOfC1IyZv6ovfjmviwOMuY5qw3r2uMlmCxw50dT_5RH1Dgm5SZL8oanu35EhcrTakf8Uq8CePgGTPGn98UxxnQ2U4k38htTUTBvE9n8NbVVgeMJfBIx0edDssRwvKgEiQqI7FYGvW3hwCOdsQmRGvVcOjHCivSCc3HD6dg0woGylc_fsp4EqW7vcA88JojMTBNzyLwhrXbr2lz8WDXHIdkhhVOJlFH5yGR0GJV4LmvMKQ5E5ZYaa_kHbTD3cywOits-Lu-vu-TQHAAI-stNs2lPoP4_otl-Yer4jWjHaDnBp-6YvEIutYR06iYxxRtI73EV6P9iyJgKDdTh9TaYmSItwQSAD39nkfn8xkWLNNhtHI49XUpdp0-gYw-okzjY4FU3FMNd3CHCZUkzJd1RmjWuKPtf4x5_Q/p.jpeg</t>
   </si>
   <si>
     <t>Voador-vermelho</t>
@@ -742,7 +743,7 @@
     <t>Hemiodus ternetzi</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAB9hl9dPO4i78jhP6SwGCr3a/IMAGENS-PEIXES-COMP/Hemiodus%20unimaculatus.JPG?dl=0</t>
+    <t>https://uc4c1ddbc7cd58ae881d4fd284b9.previews.dropboxusercontent.com/p/thumb/ABd9QpLsOOMxRZqhuSpbY_KZDxOay5CdrC5buopt1llrFDQE52ZCH6LM4jH0MFb1x77azVkA8yzv5tJV4_C6c8wws-hDwDoHTK74_BSye70368Bf4k69VTGRkND6s2d0s6I_5aB0deM4MY1e_BRLCNq7UG0_bMNuMhyocTfqLvR28UhqMPDF3v0toaj7zB7iGL6SUFRTAPIK5rfa1NtSzZ3a0YkQC6ClY9QDDJhkGH30gjLQPdSNvweT-ZkE2wTqxZ5_gssOdymGu_kOhSowSAmMf5BU5-6gv4ofzPutBrVy_BMq4DPkF-DnK_dDzDK8PRpF9Xw0yv30byZBz-sm8SVbaxKOp_hBQFfsaD_-v-5MmrLHVqp2mHKtiUBQzYo5ga24NjxRgImoQpGz2k5SWOoPd50xap1UHcTwQE4rA2ZOQg/p.jpeg</t>
   </si>
   <si>
     <t>Voador-escama-grossa</t>
@@ -751,7 +752,7 @@
     <t>Hemiodus unimaculatus</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AABxEhZzVhRJc_uonaH4T2S8a/IMAGENS-PEIXES-COMP/Hemisorubim%20platyrhinchus.JPG?dl=0</t>
+    <t>https://uc0e3e8967bf06a15c3fa3773d43.previews.dropboxusercontent.com/p/thumb/ABdc5-k1PIbBaEjEvNdW5FO1AJ8GfQSg9JIfouEyzhnGwugP1EAiLX53nED6Dt5GFGWTSHWOaiQnTE_gV6kjDaSZSFiFJ8F-W_PTtM2EuFlHuwT0dmBy9XUykwlWDSkYK9dKNa_-YPTY--h7cGNLhs4e1fW_pCX79JeLC1zYB30tIEk8DZVHODMfhkxq2-bS15gD_11DINOk8a6MVyLPjDGShkr9bRRXrvy2MPJBYCCnJJgYft3uBMSqaWQXtQBkmdkZaJSOgcY6gDnG6Zk7C32reZgS55M2OjPqd-JVcSYAaDbi5uSdVwX224cgfHWQeIJHHjo_56c0c55wTMrnhabQkbG3HWyIi1gy5Edm2KVf3PIOOhA5kp7NEEgzSFPCSMfU4UtjcKDpoEWI-EFgksG7UBY7r7avdfvDj11nx21a7Q/p.jpeg</t>
   </si>
   <si>
     <t>Jeripoca, Jurupoca</t>
@@ -763,7 +764,7 @@
     <t>2.7</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACKZvAChnWh44wd9UiRNKQwa/IMAGENS-PEIXES-COMP/Heros%20efasciatus.JPG?dl=0</t>
+    <t>https://uc656b29d690f8216279c80811d0.previews.dropboxusercontent.com/p/thumb/ABcdyCdBMjehqr7JUqoXAUzZliwX-4LBiYsIxL6YXvze2g_8QFSsB9ti8e-MKv9hnp3wHMd49i6vImtIObrb77ZWiBgXpxxG-B1JJEhAZuFgU61HbphcHQGRvWB3PaA65x09qSsSUhkQS1YXtrW3Usi4tnglYysuMdrJe0_nUvoPEBz6mimK4BNf3IgphbfE4l2MCtl3Rqr8rgQCphu0KfJkURf-Jed07XQTaGDdlSf1-6n9BZtRSYLP7Hxz-Yj-At3X1zs5ZDbCm_rF3tFZIcPqhGGPv5ULSckOAn-YneftIgYYmnqr_ev8XOhq2qD3y7XH6J3qbLso6D5tpY13kSQ7aI56LbhTObPJ8tFx3yG0vw_25LCxTX7VA6ipalXYHiUumXRWwlkZWRGRDNJLf5n-vyjxqgCFeXqWnkxP4KUd6w/p.jpeg</t>
   </si>
   <si>
     <t>Acará-folha</t>
@@ -787,7 +788,7 @@
     <t>Ambientes com água parada.</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAABZk7jKM3_8JTEkjDVTDn7a/IMAGENS-PEIXES-COMP/Hoplias%20malabaricus.JPG?dl=0</t>
+    <t>https://uc3c868bf0f6f47a0eea0eb045c8.previews.dropboxusercontent.com/p/thumb/ABfvKyncm0ZMnbXO0KlzkATSYszJrVT1PKESgPrSQX6W-dqCRjCyM4tFTUISjMbUcbo7KJ19dNJj3UCjqeQ_OPGbrDyHGm6w48QzLsYpl4sYcosjZLFZdn6Y4xLRCIXiSliFc2-QgWLYTN3MYm00Gb-7lpRMfOtuuuOPY8_arTzkz1uDJ7mC8sSbLrKnIknCQqB9uu81oWtXdESEwyyOr7oSMsTQzSts9p4If9iIJZAJm3pR9-SQqdERj21yWSYFL3-EcpYGEnypXggItMZy73d_d0PK56o0KRoZthnJ3XOgv6p2ANvCKJoGM_2HUIc5XSFdqyAqu66IFTwaU1LiRQGhbKSsV3yEImDP-qnMAXis1NXS6vVc7ZtjQM4Ecwl_pmy7RxejHr3aPGlqsOVA3BW-BcAoruVW1aIc2MpicXrx8A/p.jpeg</t>
   </si>
   <si>
     <t>Traíra</t>
@@ -799,7 +800,7 @@
     <t>3.8</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAB-Lp_cQv_zQ2n7eVTyKxjJa/IMAGENS-PEIXES-COMP/Hoplias%20curupira.JPG?dl=0</t>
+    <t>https://ucb4fbc484a655eef8c73cbf7c30.previews.dropboxusercontent.com/p/thumb/ABcZDNLim83J0K-hVA_vWZoiqrDgpmkXdNNR2QIpwCa1YOxCmva8G_yjzM03zTyVt73NptDzOnUyKvnhxv62g3_aYkVd_gLU4il_yaO057hCrqKcynFTFSZqtMfHrtoN1DRudiY_-GvkYytKNBOVkLnST8Kw4dtLBTYG-NE6TT-otto8Nj-yWGy-S4gqwTYkqlQwZXZ_XhoGqB1HlaUSoMQV957-6h1DReGfBz7Ry63J3b4zR60OAoKAlnQh4Iz3vE8O4Cf5bygKEBmcedtruGEwwwpN5f6W__85LISxc0lJFf485_oZ1j8hWGtqgsCUnkIo8fyqaew3fjQT8fLHWhwdTSA7s8kKQYOvSPfpomjJJWfOe9ZHu0ohYU25EhTP2epplyUo4kzJCZ5zuOqvVkWCVE7t8eaLU4uE4Fa1QxuchQ/p.jpeg</t>
   </si>
   <si>
     <t>Trairão</t>
@@ -808,7 +809,7 @@
     <t>Hoplias curupira</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACz2Fldo2VKXjDZV54CRW8xa/IMAGENS-PEIXES-COMP/Hydrolicus%20armatus.JPG?dl=0</t>
+    <t>https://ucc78c6e58bdebc65eb75b4a15f9.previews.dropboxusercontent.com/p/thumb/ABeGuajVtgU7dybJwHogODzIMUhS0eHT4bw4tX_reFiPGvcDCLQpHheZIt-OdOF2CDMVmKpCl6XbE5dyYBC-ES96zuUfxLLAkbctGQBUGh2XlW5nHnuezoiItQdEulwkDS0N_TgmVa-U4ZeavJT2fjWHhVXHoKQo3WUNLhp3YlDQ7g1O9mBY3GhjnHoJtEDyjiYk0hLbJmYFbQfl2DUsQ-CkyWfDNK_26ckb14CPbIVzOI8H7TlP8sn2VokJ9tt9WRKW349JzAQ6M2NTQwp3A0kN27oEiynUMp2Xv8xckzDxgDx-dB6v4G3qgk8Q2PPitC1aIHogYOGhppw28L4WLtPdQpkJTs6KJIbN0YkK5QuS5nIZRXkCFz8xYR52SWdqKaVIWxQj_6HhPLugDOhk8MYLU2SINGeZkEfr18yq0d6NMA/p.jpeg</t>
   </si>
   <si>
     <t>Cachorra-larga</t>
@@ -826,7 +827,7 @@
     <t>Hydrolycus tatauaia</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AABcOIol9ut7_EFrMcF8cU_ma/IMAGENS-PEIXES-COMP/Hypophthalmus%20edentatus.jpeg?dl=0</t>
+    <t>https://uc13cc8d5a399d899796296d326c.previews.dropboxusercontent.com/p/thumb/ABe6DU0UGxC02G73DIkI0PWQj7pOR26NvgF1rHvkDf9uKA1sRH7ZcHYjEJ_ij7bhCrljskpNdyhB6loEny_XMj0A12mso2goCjcm5XbLbNzlQvJyl-pn0kktj3QIpZfm_Br20edmV9eCdyj1ZJF7bViD1y88bA4KzDtd-08BJ5I4iJRg2C1hz2hxR8XItBhebkAoiYpu1K7WJHpNycF3br9QkDmZfm2zwSemBB0pKf5WHfWFdFMD-F9K3Pig2QHfZEwpP_neNdZSp9uQng9MNDTg1HzJodQjwzV8JNr6zi0koymkEcHX08eCWOLLMpaYngxeak-LuP-4G6JJVqfqnyxmsU-QsMRIkxnjrYKQLrVAKmDf-U8BD_NhVnabBgRAVVMTtj-nOEGfEZ9AoeIMu69mY9HGFGr1k6ExIoQVlpVBAg/p.jpeg</t>
   </si>
   <si>
     <t>Mapará</t>
@@ -844,7 +845,7 @@
     <t>1.3</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACmO9IbOGmdgafHxqFokh0Ua/IMAGENS-PEIXES-COMP/Hypselacara%20temporalis.JPG?dl=0</t>
+    <t>https://uc4b48c815b9eefb1571c0018181.previews.dropboxusercontent.com/p/thumb/ABeMJXnmSi5Dd6xaeeeKDrZB7akeJOY9tH7ZiUy70zr3RWc1fcIA9Dj02AkLsMlRi_M7kLeLK4YMcOh47HOYl142lfTMZBryzO8X7Walol4I2CNf3rfONH2WWfXynLALaRn6WmzB1Ji3SKG4F3YWQvW8eN-C5mXfs4yoyNan2LqPCzefqA_cn3ZPpzzUeuUXPpqz25ZN3UAaC9YKMxEAOdUr2J66ixtYpR8XphxDiilhHfiaHYimIIAAKTjM53U1gBQWBNJihM-TX-rcbZg-UOMz5S5rdUlIzC5Eq8NY5bBUfZj8rFTVcJTcqtJJMA_rIsZ9YWDavS7J9TNSKrhOhdxPDCi06i7pfY0ScKTFi9t41m6KWVz-Xj84ijVgHgYTeCTfkOB0z4eoFTGpQ6qNxC_bnR45yWGcQPy8aYLRLUB4IA/p.jpeg</t>
   </si>
   <si>
     <t>Acará-roxo</t>
@@ -859,7 +860,7 @@
     <t>Leporacanthicus galaxias</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AADhhYZ1RU5Qpl3hgucksodwa/IMAGENS-PEIXES-COMP/Leporinus%20affinis.JPG?dl=0</t>
+    <t>https://ucbf64dfc33a0d3f30fceb766e73.previews.dropboxusercontent.com/p/thumb/ABc0KNZ9jcREKi7dfJA7AJq8vlYHBjfzLpezZIOSIqIQ4ranqbWqOW1a4EQfKVhgE08W227vWrbVZgWAhzzp4BvF0f1Blzd7G-VveIzVaA2CrbJ_d69nDE7bt4Y17e2LNdCB88OANoSe7BVgjN5TeUf6xHyaI6mItxZ7YYmhCwZLw3lnOpvJhQwjageeOa64Ww8g7WKb5QS3SUj_xqbWDMAavwNxTJcOIr8axxykF2uYrPZ2cBwcf3P5ub6a71FdmMWt_jVXLjcB6EGv18EB0vpfzYq8LTAQkvPRc40NYqjMTi2yL_Ivt0rTrEHlwo9NQk7sj5Qo5xGXBeBCyicDhU77Nw0q7AOC3HhboDJ7vL55lXeVhwbD_bM80zX5xN9XPmSpnkG69kizRw7a0ugCxrnu-i4gdeKc7yQx1Tpm-tHGQA/p.jpeg</t>
   </si>
   <si>
     <t>Piau-flamengo</t>
@@ -868,7 +869,7 @@
     <t>Leporinus affinis</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AABaN1jywFzFPpUWpgEShzxPa/IMAGENS-PEIXES-COMP/Leporinus%20friderici.JPG?dl=0</t>
+    <t>https://uc30eec35611120bbb7c4913d0a1.previews.dropboxusercontent.com/p/thumb/ABdlzNu9zWpKNyZ8bLj7b1cBkB-qvd5IovokMHMDQrdgy6oQuRazxTRNv4QCtfRb0ia0QBbgXxbsGg4XwxyQ4l3CGVxfou7CxOZWemJnk1q8x_msQ8OClAy7Y7I_ANOJhByKTPRzpeltMrFrzCesCbn3qgb_TmX_i27eXjlK48SnGfeMWNQDvvV4-VnPBoiAM1VGOAlexn5fBV-GL6d-FztISgNt3W4-q14jQVst5lB5ivNPFOJpyCYqBbJ56pHlBjwmBJ4KFX8iomcbJCBGy1yfpMsxtXZos7M8YFz4--h5IpFP98-FuWCKdYpm2Ds5WuNbezjhAsux5TqMNTCd13vqV6LL2k3hG7inVmGT_k-vI_B1sbUe4TJ8trV8YEvPhfu3bsg4xoO7rYj6MMNfdh3yXpLhFkUhHql9wAjk5iUePA/p.jpeg</t>
   </si>
   <si>
     <t>Piau-comum</t>
@@ -880,7 +881,7 @@
     <t>1.5</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAAv8lOH1KpwZtclwQ6T4AQ7a/IMAGENS-PEIXES-COMP/Lycengraulis%20batesi.JPG?dl=0</t>
+    <t>https://uc3df08688d681b3b2e338c47b9d.previews.dropboxusercontent.com/p/thumb/ABfSQmyTVbrAy4ZCkFCFd5BxLUF9A1vB77IHVgc1cCjqA2W_m7IJJNzmS_h_UQ8gxfxBEJ1cUu7UzrVWGjdUKqtYa1A_1jcTi79NqH2jSepjyCQis3lPCWp5W8sFtPWxgXsigqAzyTN6MTlJTME6GTDc0y_3f0jn5IHfbgfRRJzn_ane9xOOQx2LtTuljRPwaYOzoIyvtkSh4GWZJ3sz8NA_hsxC9Gx4IwPK4sA_TkPxWfA-Yhatw9Okz2OX6sUmZRdKqge_lyvNzw7dQrReeGvlWIHEg80jUbayvtez1q4WDD22AOpQ64ZE9FYHVX5sb7yYcoJa-ZDj5jDQmIqLQiWejtIxS-DfaTfDtYkr032oOZrw0j_iO3msLaaeRsN9KFyFkIVqEuBFcC9Sh7p4_hlw1DIWDf4siM9OUZf9JT9AqA/p.jpeg</t>
   </si>
   <si>
     <t>Sardinha-de-gato, Manjuba</t>
@@ -892,7 +893,7 @@
     <t>Engraulidae</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACSJrf9ZJ-i8bm_RKJR94zYa/IMAGENS-PEIXES-COMP/Megaleporinus%20trifasciatus.JPG?dl=0</t>
+    <t>https://ucdf3a59536b5f7df87755759b8a.previews.dropboxusercontent.com/p/thumb/ABfC8hr1u13kCvZE9yONgSxQJJ_OOj3R9Ehii2qhaoKeFAkmDDw6S74H_notSlLTW5UknU00ECxUTHf1b4lqjLls3S2bI9Wdd4qkOODyOg4T_6PjMQY6zQYosld50s6uGsyTCWHyGCrjKwDYsKyIhcMdz3lgtqrDCQysh67hgbmkKp4VUkDNT9IgEwYDbtYg4I3PBBkvx6v1gbtzHpGt65KUI4Zm2AjiDkqK4QZadydVzPOZfAi8FJRkWQ6-ta1isyGDiYj_CqLWjFPIdDVQi7x-eTYH9mWilnCEB1u9BHQPvgUGv2XhwmrJVT6UcmK07v8JSk1Ac2AcYZq2nbvQKrJj-NDjtsLLo-IiidM3j3OAV9N6ND2wGyXoQqNeSSfmdHBBlpav-9WlLrYdwvxJSI4rhwnJVjk0T2dntLh7Vd6ulw/p.jpeg</t>
   </si>
   <si>
     <t>Piau-cabeça-gorda</t>
@@ -904,7 +905,7 @@
     <t>2.2</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AABycH01-jWguDoS9hV6A11aa/IMAGENS-PEIXES-COMP/Moenkhausia%20dichroura.JPG?dl=0</t>
+    <t>https://uc7b0406223bf1daec0413cca967.previews.dropboxusercontent.com/p/thumb/ABdfMztxLH15j68nBwphpOaudt-KQehuDvZ_lIxW55GDQq5jKAntatU8nfDBLaKkTkIOCy-EKk6zbZfVvP-93hkYEOVKQ3zZYiJYA-OBwyDobkZbXH-_O2EQd8LY84HN_XgKTEn-9HSJyX622wS3zd7n9hm7sS4yk1w6dCkqq_HkqEHbGK1V9i22xhsElubbo9oI9OOpZfWU2gtcc1imtKXuvwe63FtCaVPRZZO9hNHBjWlKDjHjsu3CZatRzTfpWSHdKq28apCOGQ5uE5n9QLhRY7NBp8jHYMQc4BoN142RDsFQR7n9cc-vz0044gO090PwQ5mD2Kwo6nrXhAUzG79RalIcnzO3O1IywGPA0k7RlNvM4L-jqxRnKL7mq2CssbsECnJH1Bayb3FIwAozLISu3-BCAWOFU7YUIzdBJJReYg/p.jpeg</t>
   </si>
   <si>
     <t>Mandí-prata</t>
@@ -913,7 +914,7 @@
     <t>Megalonema platycephalum</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AADuWRBNEs3KZ7aRoxZTnR0Oa/IMAGENS-PEIXES-COMP/Mesonauta%20festivus.JPG?dl=0</t>
+    <t>https://ucfd7523b16bcad4d01f1e2adbd7.previews.dropboxusercontent.com/p/thumb/ABeNL8tVlZ88lepY1u5lXFU5ocbfzmDCthEmuuYuyMUhRqIjAxVoNlOj5AMrX2cyfbrGcYQdHik25LzaS6HieLs2PSFuDBLN_g1PgBU2SSg5a2b1gInW6QRzIwphLwkA0EP2V4RssZaPEDLhQ3bx1bt8uceBPogmo4YCdh-m95RsP0FhdTiSqj8VVt-CNDy-6GvTlK10xDZkpufjoOF6yuoOj1bvq292NLRs9VnycMA1YSV_eZNlbHo94H0-hr3glqHzPJSqkzYhWp7CsmhTs50SZENEmzgXPqqjBkttIpm3SmjU2rvUpIGqsiGsyUErw7MBaKGn88UWi3e3nbXn7iCxlECQN9WyWVsNaHpiLJwVHBu5SOxPP-FF0UC6v25gD5NwChV3xrjyVEU3D1p0bfrQK8B_vtLPSg-NfETeGlPrLQ/p.jpeg</t>
   </si>
   <si>
     <t>Acará-festivo</t>
@@ -937,7 +938,7 @@
     <t>10.5</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACjM2baghwdzyGn-9v0yxD_a/IMAGENS-PEIXES-COMP/Moenkhausia%20oligolepis.JPG?dl=0</t>
+    <t>https://uc868df3f7362fb41d16e17eec8c.previews.dropboxusercontent.com/p/thumb/ABeU7JGZKxbX-yq_Nv_T8MnKcWzWxSOqrxS2m9RFCCdbylPAXtpBO3EKnsvy_ycwljblQB9isyR_x68m3Q8lBVEUXlAg7YOAKA7P_haG-R2EOCePgoYWWqyl0IXwV5sZ4ezJ-WwpIUR1MgdOGyrdpOPiThkjt04lpAobOqVUIFeM4_GgeKwCZRdXY4uoOqnCAEeCYpdRKuurFJr5R9-PLhFRgV4Aae7JEtEXIDN5UqVjN4icZatYZfjiFqXjxc3UyJZdO6b8IEvXsYA77Fc9PX0yoCAC1iuWMTfzv8RBi2jbJ9eLaTsEadhPeZeBQTiozzg-KE3HOY2EOAk-_Ijt2kMD-zpwXoOeaMRR3T_zYGbyrBKfV6hvByxhB8AB-FIliCKJszAzpVbw0hlrBU-UY_aSQlYZ3A0MK8ze7MHF2R2xJQ/p.jpeg</t>
   </si>
   <si>
     <t>Lambarí-rabo-de-ouro</t>
@@ -946,7 +947,7 @@
     <t>Moenkhausia oligolepis</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAC5_329wbAk1r6Q8iAvEr2Ua/IMAGENS-PEIXES-COMP/Mylesinus%20paucisquamatus.jpg?dl=0</t>
+    <t>https://uc3b2151db4e51f764f5f098b2b1.previews.dropboxusercontent.com/p/thumb/ABfE0fFqsUXHOB6ILGSY9BJXeHlJa7jNYNVXfl3Ifvjy7RQQnr_MEQ5o1RPRK6XSlKi3C7gNmIwF3cnVIwdnHQ9iQNilsoAnh8XWhXfZhdIgDlENbKPtu4B9KJVRxAMudXqWaNiA7JICgKyjbtmnuLGHxJMuc5QPaa58fpCmdsSfigzPUBn4hHxK5mBvQKbtcBQ2C12M7XGSP0iGN2c4qYa5CdhjuZLUfDo1YfFJG-gkJFB34Zz_m62t-AXdAzo0MddvI0gJwO7MG893NkjPLkCsYA8kVo5aWdmL-B7A2bAGSnyV-nfCBcXSM81pffW3PHuZR8nDFR3yuyOIxF7U1c1cY-QemPFJnqiYwQefIYBbtc1M7wt4MntOrCtEiRGzOlrQT9E-MjkA5O6Tv1szuBqwHzgWjFwxYpKlMxzm7Q94Yw/p.jpeg</t>
   </si>
   <si>
     <t>Peixes redondos</t>
@@ -970,7 +971,7 @@
     <t>Myleus setiger</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAD_2ol5WCDh0Bo448NTyo1Ja/IMAGENS-PEIXES-COMP/Myloplus%20schomburgkii.JPG?dl=0</t>
+    <t>https://ucf9e4f04a38eddaa75371ce841a.previews.dropboxusercontent.com/p/thumb/ABfk_UYOLIgf_w2dxAXzDyqEjFn7C6JQPnfluWZzUCfwZB-TI2DZPWR2arFvigcaFpn35i2m4wL68VuSQmO60U8nEMiMvyNO2KTbjA6oJOt1Ozt1zTxrTc5Yk0qpSa_anktE1fWhhwprqPaThBxZUPMce7QJaRudPg52_7dcvMDQ1lHUVeu4GLY5x-lyhnTFsXUA53Rm4J_ituFipHzGGgt1lDD3Q9MA6HLMnlFRdl8-yGScTGohLeoTzDldSa6TnRWT2VrxmfzC3-Lw2qynb-7pqx52KosKxsAuvmf2Sk1HiiuTdyceeY7VOqyE5Ecqjf-gCgKvkxHWk5cMmB73t5f8tKCjhwnhbdbZiy_I1X-NoMRqZ8q51hTHbMVPIKY87qED3iVtbuU-8uhVht0qA0HOyGVY9WcDWGwjHpOMgTLUjg/p.jpeg</t>
   </si>
   <si>
     <t>Pacú-ferrado</t>
@@ -991,7 +992,7 @@
     <t>Mylossoma duriventre</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACPuoB9Gfbu2WUYhd0ZCDIya/IMAGENS-PEIXES-COMP/Oreochromis%20niloticus.jpg?dl=0</t>
+    <t>https://uc7513b31a13f14f67ba48e8063d.previews.dropboxusercontent.com/p/thumb/ABed6XjhcDRDoXDMfIVjErksm_GhvHZVTcf2Ghc3LZAaTBCDal67pkj70NqxH19y6pjuvXYJxwfG8OTcVFDnVThfQ_y4u8ZIMBwCOqMpSikyOZu8K2kRDVOHHoOn-wYZ82ZKiGIn99c_8MIyJRi7Jkc4X3o8qHOmEslZATLYi42QtKo3DQ6XT2yBLQRHR1FShZESX9pnY1LUua_0OpjGuuHN3qUp4eV0y4k9NrCwJXxTgjp4Fd9cYOVQizU0qCzyJJsY7iKLaRvWph5TUL7mooXbCvKqQzKX_vVGAwYhtYBtlPPKsg4qtLfzUbUxLmkCRqWxy9g1Vb-3yMwPv7LQQrtTpXeuVjjCdSgmeYYDrTESa9OD7Ts86CuhxIz1OHkr8nQ8BH8riPQ2043WUGTyFz_CjQp8TUr54Nv4XIo7udS08w/p.jpeg</t>
   </si>
   <si>
     <t>Peixes médios</t>
@@ -1006,7 +1007,7 @@
     <t>4.3</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AABYrbhZdKIIyyLqPZk7KFAua/IMAGENS-PEIXES-COMP/Osteoglossum%20bicirrhosum.JPG?dl=0</t>
+    <t>https://uc83429968c20a3cc962d81543c5.previews.dropboxusercontent.com/p/thumb/ABfxmJEsKSkHKbCQuOWFGaJUHZzDebP1lzd4nvZ73ZPEyPPZyOtD0EWpoWIyG01NSg2JN_9eAaZjuYAm8rcOXRX_bUDw_T0lta6QQ0hb315P055bPhzmyVwT2FZNZbesa46nqGwxFkZffu9sr47_pY0qBXbyAY5aRM8QWetWM3MuZSoqTMly3X1O7Y-y2ywIwG_LcwaQaCZyTg-gM3-D44dtGHh65WboYM0R8oJJqbVy-gxmUw2qkwOTx086t--PazStvTTCM9Y8xUSU_3MpdGZYl2FGdIbn_kfKSGUHe8GRvIKBBgnYTI2CqLnk2R5iUMCllkgaWKuTZy61SU4EUkuBeQSOi8MuzOykRYWcinCAQ_fY5-fuEfQwcNLq5uEeN4Jd2uG6inmlX3o-cURRtYkQIFPK1zHu5RMeShXsxs02EQ/p.jpeg</t>
   </si>
   <si>
     <t>Aruanã</t>
@@ -1024,7 +1025,7 @@
     <t>Oxydoras niger</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAAILsq4uAUI0FNcSqI_mhDCa/IMAGENS-PEIXES-COMP/Pachypops%20fourcroi.JPG?dl=0</t>
+    <t>https://ucffc5d1d3c28063252b38135a46.previews.dropboxusercontent.com/p/thumb/ABd8S709hRA9CtfqWfm9xZDyRWGDEXgAFOiC1xyTB1Z0yJ4KlmesqVmswB2NstQEK6LhzqShmeh5B5ZvNMYg3vEawPYo5XS8JcdkWHtOzb6zqEHsAEJ4yzG5NOuZezrVgHuiqQ1ntMFqP8wQ3VkWbQQmzvPTijO3KgrQo5PwIWBxzmK7g0AHTBB9-Tbrb0a6eFc_BPTnNq6WtaJjHt3TyI9i7MoyFOGJbSDtnZ9cFsrn3JxcSLZvKOhsyTO-sb4ZFpcEXufnGO5YuaX2DsVhDE_OAaQrBmNR2BVmt5R8RsjzdIJ14sc88M8wQswJPwGg9YsHJ1ZqMPvNVQgGJt_DEBU5fGqOc5bPZv7cCEUhSH82MrV8QZQB_6vq2WEGmTlRA2NVRec61djc3OccU-4WlQzNafzkq5m2jjM6SwICrdW09Q/p.jpeg</t>
   </si>
   <si>
     <t>Corvinas</t>
@@ -1039,7 +1040,7 @@
     <t>Scianidae</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AADYA8fAuVQ-F8NooDSlVZ9xa/IMAGENS-PEIXES-COMP/Paratrygon%20aiereba.jpg?dl=0</t>
+    <t>https://ucc5ee67eec19705a1aa38e681bc.previews.dropboxusercontent.com/p/thumb/ABf0fZnYSwzeVbF_LH-KJA90rofrmSF-gM6aGDFrqwy7zRp9U772ygqHGU-Faouv10eyRb68Q-YyQzVtGrPeGQO0tp-FI0k7qKImzKfVypst6c1k4v4XiXjdqDtoUMYrGjDkCn1s0ADV-JkdK38o8coNuTghJoC7TaCcUztBvssEqnvWIJyk-SLhdhX2Tfvp-5QmtBnlT98NoUNS0Ag9uG88YGT7GntBejVCK7XjWfYrIJGMG8lghn8tFSaJlI7wqqpJ3E112lWeXCxE40bDOOLuIvXOlV_qjFfzcxZXyz_44LroXZyMtxrzAFLQRr6n_2KAGDb7YY0W6TnSGRQYfKkLo2xg4NTWi1YodU4Wq5hLB59QPd9eZMjx0QKUOVvdo0_HYiRUSwnAVAqutpzQ7He659CqBv70bKetuF3uB6FQ_A/p.jpeg</t>
   </si>
   <si>
     <t>Arraias</t>
@@ -1060,7 +1061,7 @@
     <t>Endêmica da Amazônia.</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAABdMCI8HIJPV8GaxwtrG2Wa/IMAGENS-PEIXES-COMP/Pellona%20castelnaeana.JPG?dl=0</t>
+    <t>https://uc788feaa3a8a2b39def5a66043e.previews.dropboxusercontent.com/p/thumb/ABdkZuoZ-OKV2d-EkXZlAU6-XX6qDOk63QBaNAzXEQGNJryviIG826oPvh66KRDyaTZvJiPKLJ9jwoAqG9zSAg1hbKMzhQJRU8bUU_JX8fjTbzN-3rjvMNNGWK6vaoNkWkxCvcxLNae11S242bYUBhvaKVT-tTTW3ZiBWSO0gLiL_x8LTzzP8v_A5tm_IkpbvJ-83OEjKVDbdrH9pitom_8DSrdwNqw92ZBlYM5Z_VE219dOWaNVHcNAgY5iPvezp-xeHj9H16qy6XzEamIZv9HginStARybbcXB3iUJN3Do9J_3WvwoIIW6YG5OdwQLlwb-LWVTxf8mrl_ABK99p_nhKb-T8WzHpwY3YLYz9RyqiZe57FVs8j_TX78hxOvvliBX9IU3mG4u6Ffi-rUKtuBvt1vUzZYBcgky_eLGmAijsg/p.jpeg</t>
   </si>
   <si>
     <t>Apapá, Sardinhão, Pescada-amarela</t>
@@ -1075,7 +1076,7 @@
     <t>7.1</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAAvnWSee1KqapbMyokPyCdFa/IMAGENS-PEIXES-COMP/Pelona%20flavipinnis.JPG?dl=0</t>
+    <t>https://uc29275d8d46bb13a1594645a0f5.previews.dropboxusercontent.com/p/thumb/ABfQEjwNklcgoQhRMZE_EUyzxzcj_q1HmnIclR3K7g5nuD_9SZ5WwdAQC4_-mjw8aP1Y9DBFCGIR5SVSLYVOE2ZF3-Gzf4y0zc9HR6XBbvy-zo72KOBp_4sKRTAIGO6jsh2ODxGWu32N-zjaRpukAlRR3wY4wxMErZgh7DfoTSEMbxfBhUHCnr9REtkJ2r8TjSdcSsYRJ54Ajkp4YNxbO3Y7nu01Mh1iufmY8VmGF8xAafJOFva_B8w-mBhVnRR1fHnnP8uW1R--_fKFxgbKhTLRkRSgFspf_jIQ-U63ht_vLxVbPoHJ3pIykGmOQT4w8xm5B-klR55rYCbq_-QriJsGkWvTlS4eR5JNYY4ntt2bKzjev05pvnYFKj_nrJanWbGCeHuXm42wpNR8akbfwzayCpw9m9uR0r2MASaBTSUr5Q/p.jpeg</t>
   </si>
   <si>
     <t>Pescada-branca</t>
@@ -1084,7 +1085,7 @@
     <t>Pellona flavipinnis</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AABlrH8XfldL2BARz2B05FLga/IMAGENS-PEIXES-COMP/Phractocephalus%20hemioliopterus.JPG?dl=0</t>
+    <t>https://uce2b7795785b131a9a6b15b4b6c.previews.dropboxusercontent.com/p/thumb/ABdWPwp7XVja9_siOWp6A3EsFIDGBPyiTy93pj9ZuXiJFK910QOkliRPYzSdqCmArcJURZ9iEBnOlG2DT4DO4q26s2MtRWn3Cd3pKzYhAGZ3Q38YcnLfWwnVkXeuUeFvQNOWhKqfTzMxaympAP5nalOrwGFVmqrslXT9mC8lA_p0gh6f5J_mef6lrpKkOyS6Xzn3kiiPR1w9XUStt10cnH2HEduu_nS8WGv1Ov6HTSQvBiRxI0oY0e9zqxxzIms_BSu50DiISTIqZ-vSenmaTzGVty2fHYeTwrDFY7ng5GlWhyHQUF5AUUPX5OWa1KqKCXbViyga5ZSGJ62QXr4CFkG7ymR06kNNYQURiJdjyFoe7dq6F_tkrzFLFo7IN5o_oEmn24SRU2QFiov0gY2IjW32CcoVjV9kl7dAHwuoBk9jnw/p.jpeg</t>
   </si>
   <si>
     <t>Pirarara</t>
@@ -1096,7 +1097,7 @@
     <t>44.2</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAALnzyfV5l2cjp8y0cXQPgMa/IMAGENS-PEIXES-COMP/Piaractus%20brachypomus.JPG?dl=0</t>
+    <t>https://ucbc454bf97b12d7ceb293031874.previews.dropboxusercontent.com/p/thumb/ABejEvOrfugnqEOOcEyGcUm22-EILJ2zaSSFdhaRkYQAcn8ueCMXci5SxjyGzZkLwbSdsT38-vbtKnMTaDb0VR7tah3GD2PL2aATxLxJdNh7xmR2g-Wvjtfwo2tGoPfHNbW0vKKdCidL3nrq-0RufqtTs2rjXUwonsHlCx0YmQugIDNPFjJehAKZvmTQtRWaBfvHLa5a5UNM_F3jedcIKXMv-qs5XcwzFS0kIYtrZhsA58FD6Ov5MseY2cgIcrL4EIBpO0mzkjPrULXKmbyOthcKCB0Q3cJltK2RaJBs-creg7Nfzk7b_j9OI_1JtbIYdJSL_jb75cdEIUvMeVfNON3kkUZbNIyhUAo6gUauKas7rOYQtLxWgmeegqm0divORPwv8tU--JU06FOwC60oIyQoY6Ck2VkcUTD6ibZKR_o-1w/p.jpeg</t>
   </si>
   <si>
     <t>Caranha, Pirapitinga</t>
@@ -1117,7 +1118,7 @@
     <t>Heptapteridae</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACzXEvj6FW0ylRrCpLtpgCja/IMAGENS-PEIXES-COMP/Pimelodella%20gracilis.jpg?dl=0</t>
+    <t>https://uc21c0d12b07380bacad6c136c4c.previews.dropboxusercontent.com/p/thumb/ABef8aEkanJmpzSbx9kzrBCtjeQutvQvi2p_1xFVw92WTqRaw7XkECXgSjd34kocghctzYH5jWQGHjMDKVyl_5xLfVeNEOxpK3ZktPeD6epWfiKTlSldGhGHycSdOcNVfgdZzAAtM1bmFRIgdkuuDSckKbce2TM-W5Bu_bgsLCFLW4z5DcBJTtpEquxVrio0BTFE2OzdsAPTzprmhhQzDjWmqG-0QDH2lzXMY0QvFdVYjHyk_gZZhq_fAhdQ1AYDjRxhm_0b09z95lpCA6VgJM5YYol4x_uxuQKjPcTuiwz8nAAzKV_P25js2A-BBznbReeYCym7zZby-O1IVeQ70IOxXV0S55f4fBFi5BERB3x4q1ou15h-E7CE6XFTol1t-NEe6zvgstyjZjVMlB_cY05FtziJ173_UTptFvSAwGQjnQ/p.jpeg</t>
   </si>
   <si>
     <t>Chorão-de-faixa</t>
@@ -1135,7 +1136,7 @@
     <t>Canais de grandes rios.</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAA7iDN4mU2L43grTlFyexvoa/IMAGENS-PEIXES-COMP/Pimelodus%20blochii.JPG?dl=0</t>
+    <t>https://uc8469c499b4878b9ba8a6a46aa1.previews.dropboxusercontent.com/p/thumb/ABf7mn6t39xyvDMWdhHGUJ8ZRHFtUFWi5BUieJMNa7pq8I1g7Gu2cyRMZJ6Vp9cLlo6Lqwt9yJdTqSeTHVuO8Ix-icIoz0d20XyTS2EsqpjwR6xSku_tYJP3s5wgM10_ljE5pjcLD-x-OjZmYoLXoYhR85L7UW6X0isoD-SzBRmrWSGCMTVjrwpo-DYwPVloLHfRqRNXBLvY90fEsVM6wmrjjQLsYyC8MLQ0f-ot6GuWgYLbQNuRgfRvc-pbJ_yaK-5JJewd0e1zl8geEGbj0aaC9Ve40OWf3_o3U9n8cnQIFjxAwSNf_YRTV0xIImtHEBHJjpitaewEKys6mGAOmMjdytBHWattQGUikO_u5w3UZNVSqW4benEHmaISoCncipNTyiN9jx5Ez5N4S8RE66xaGJZIidyMRnBMz-zT-Xj6JA/p.jpeg</t>
   </si>
   <si>
     <t>Mandí-amarelo, Mandí-cabeça-de-ferro</t>
@@ -1144,7 +1145,7 @@
     <t>Pimelodus blochii</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAAY-25ybeXXyYdwQoNAIM9Ra/IMAGENS-PEIXES-COMP/Pimelodus%20ornatus.JPG?dl=0</t>
+    <t>https://ucee90d2ec2fcd89db947f4786ff.previews.dropboxusercontent.com/p/thumb/ABcEYrLFQ5tiU_cXBC_x660m-i2mbuVy9oNi8jPbXL7vx5Qvza2V-4x1MKrNfLVA3VdtybHgOC5fECT6f7BXzxBCz7iM7TI18dn2BkncCdxJLFUUsa9_QsxOzCoEnxI3ArkESr7JxI10mtkO24dqOZWXanX-33-ZkmFrjdLYOrt5zrs6W17kBC0hML_tKLcOeygbefF8YPswO2SvxHEvdOhPaIpQSQJEPWWy8FU6FjDUsRR-IiLTEjy5djdztd3CrrcLnTSZ0L-vRWedDQAayPR4GF-BZu7cc_8a6c2Dyi5o0NLI-gDAU1hjGOgRxJzsmss92RqiCT2LWws-wTmIXoGZUSPpOaI6mVtNBq2tYuasQ6dp87xEpx2DTDvYej68I1aCQgMdFyYsnchvETDpgfF01qMYhCDUKf3OOrQEJlYzTQ/p.jpeg</t>
   </si>
   <si>
     <t>Mandí-guarú</t>
@@ -1153,7 +1154,7 @@
     <t>Pimelodus ornatus</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AADoMJzwzl979lGkcl1COGZ3a/IMAGENS-PEIXES-COMP/Pinirampus%20pirinampu.JPG?dl=0</t>
+    <t>https://uc4e9f43815ce453f6302cace789.previews.dropboxusercontent.com/p/thumb/ABeiv-O7IOLMwziwR6zBgbiKUsC92D-ktVaPoUM4UoKmpDchvtJnub4HAHt2NKgHgl-3Jsmc53-cgr3kB0ooRz1_yx0MtYSQqulAqjboUpkXrMSk9g0KqAVLpN8WNlGEuaaxU6VJfX9hz3xKSRow4Qd4sosWpWVU7fUaKMjby3pt8EXYkor7VoW7srpIJwzOS894xoRfO3_R7bXeH5hhwSAAkKVpUAuI9I7sdh9RZsD0HynTtr5dv9l_Lxk5egxdwPbV9NU4BPmGtje535lE4Om4qieDGMSycHF8CaOS_3ic3tM2FbhC6T5iznVHeIr7Gk97IsoKWPq47Fuv-T3ZGkPxYLxmzMJcHKbRytDxTVjibJBXtJ1mL9TL_qMXa8q8wEecwI-bIuPVom__hnQXMYFXOD2mGDqkS4VBUBUBdcitIg/p.jpeg</t>
   </si>
   <si>
     <t>Barbado</t>
@@ -1165,7 +1166,7 @@
     <t>7.7</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACfNh7tCn1JZmXGEQcLoqRAa/IMAGENS-PEIXES-COMP/Plagioscion%20squamosissimus.JPG?dl=0</t>
+    <t>https://ucb53aa7d567a677ff7621919f85.previews.dropboxusercontent.com/p/thumb/ABcRp9azTRbl07Aw7DfUmyJOaiF9j_siFqhDAYCal9_Ri2S9zXth_vxjNPendvdFlrZORvxVPeuBgbYj3Vng1dOHGtuw-pWkl5uZUfS7G_avlj-5xLVf368_R4FhAc-cjjwx8JcumFyNUA-FVSx4vzffdVv801d41POGYM-9gnUYKy6iysg5OsEebjmx43qJrrbazitMgUCQrrRt0H43m3EYjLzkQ4zrscwgfKxmQh_UT5x9lVOJTMyIE6C-viMDmLqQXcIUHkq_Dnjl7aCra7qxipj0Wpfzo9_CzhobygwvT8vkqswFh9mJIHHIyt54bue4UHdXBUnI0MQH1hMK6GZLN01tzlYNmClWe5ESFG7VDpuYkMiNkM0xUPVVWhum36Dc2OwsHEHbP4Mi_5GUexhM4IOOa9Lswq3Av_1O58-73Q/p.jpeg</t>
   </si>
   <si>
     <t>Corvina</t>
@@ -1177,7 +1178,7 @@
     <t>4.5</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAAcbuE7Wu4XjnSXPja0xuDGa/IMAGENS-PEIXES-COMP/Platydoras%20costatus.JPG?dl=0</t>
+    <t>https://uc39ace3b8238f7870dda6fe3546.previews.dropboxusercontent.com/p/thumb/ABeZbrg-gwG7sh_59zcmQ4WSVsPeU8sEKZ-K4MsurCtuxbVcTBIgFh_15o2F67B1q7SoX5El57eQ96-ntdLuvPiIeSkd4pvr8s39VPaioBmLGEiJoYiSzJu0n5PpInGidp35Ob-UHSdBykNp_g_g5H6i5JLd3F4SkQABSlttlygwi9dHqz7kYW2FBw-yd2dzD7Gf6diIpo6hopuHoCPDk6b2CI1TnKScF9Kp9r47f2x5FJA-ZK0_DT7u8lwD-cVBVRPYQnVs-nNiAURCnVPXhMJD0pkzPlDU8DjEQ3zYjka0n_bjYH35D669TVF_XeTvQlpp6kdgRRqXYS2qBOPdppRv_Y2asj3llI6vofRqGo85Gq8VZm7sGCo4Mq3l4GZ1mS-0CYKZb77ypSOhJ4mYUcP65TYk2S3AZjltvkivaNHIIA/p.jpeg</t>
   </si>
   <si>
     <t>Bacu-rebeca, Cascudo-rebeca, Cascudo listrado</t>
@@ -1186,7 +1187,7 @@
     <t>Platydoras costatus</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACy6WMl-PXOK-C5lJwnd4e_a/IMAGENS-PEIXES-COMP/Platynematichthys%20notatus.jpg?dl=0</t>
+    <t>https://ucd000e2a95820e6afc400d76825.previews.dropboxusercontent.com/p/thumb/ABdjM1ehD_u320U9zM9FDKMtdLF9q9S2pVERjmoLxjcHn1bM8tqIWo8GpCHkEL2uvKbtsEcR38nLKmWF_E2awuqfCrAp6jHHS46M8S8iL0NpzkA-u5aTGkXEke4zyoxQFpLainG1afM5N_Cwm7YAZBYSL0g8EpyaESDbdsa39If2luFE5l39puCJ4_bBb8AqYOvqUjCF0xhGLmZv7wD9a4XW5JhofsXGs8stQMM1Z0jkUEjylpNZ6sVTYEhyQDSE_-aP8WQZkBR7T21hEwF8S1sRdVc_z-_50nACvjFe3D_eF9JIPOun54ExtLSU6q6rinySL36N09xXDsbJyGylo2io6X3SXIW7clRhtSEPT4lTQwS9pfkPrYEePsUQnsCsfuXUkIcHeQR9nZs7deYIWU075GdsPT63TjjOKUpEafJ8hw/p.jpeg</t>
   </si>
   <si>
     <t>Coroatá, Piranambú, Surubim-de-corredeira</t>
@@ -1204,7 +1205,7 @@
     <t>10.2</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AABbLiTuIFay_XaYb-O1qprSa/IMAGENS-PEIXES-COMP/Potamorrhapis%20guianensis.JPG?dl=0</t>
+    <t>https://uc96b9aff1e347771330ddb7d5d5.previews.dropboxusercontent.com/p/thumb/ABcrKpRblMJ1LAhez72-JeBwtjwp8tLEUgy6Rwe9Hr21TIe38GAcD5PsvdTPNWSDYWIcuqt-4_JQEXQd4Uv9IbPBFY-52NnzuKW7NY2Zh9GwaQbB4ydnJgqM_bB2dltIBH3mf_XX3x3a4NWwjLICcegFnVtmmLYm630PxQ7rAnkI5QlGmNvHsn6Fo4bZzqTogolXvArSx3sGr6AO6FCdzqh2jv34YMIvbD2fIIOpR7HXIDwDIRrfZOHuqzejnuS32-miv5uUNkoGF-5fH08kE5e3dxQ7O20urvKJkrnf7U2Wow9C37K1IQAcEIFBzjHvdQHyzyPSABE7IiIb8qVQ3VLMeiEa67oAVzlMsfdOsAuZLVa9KM4W1DuFHZw_-7-_DgylXnd9jRRau8WTkc5STI8ZfGFKWAuXZqHnQLr_idG1hQ/p.jpeg</t>
   </si>
   <si>
     <t>Bicuda-agulha</t>
@@ -1246,7 +1247,7 @@
     <t>14.5</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AADcBEMuZ477MtbZrHaGm4Pla/IMAGENS-PEIXES-COMP/Prochilodus%20nigricans.JPG?dl=0</t>
+    <t>https://uc8bd7896662a8fbe079bbcb02c5.previews.dropboxusercontent.com/p/thumb/ABfbKWCtZazIAAxFUR-JbHcmfj8bJBKRb5UkRTEaiaHdSDKitydpPb4RL9cP9rBugCSum0XRqO2Xbd34gd_g64pSYH9oSjw9MT03AqHU8-wr63kO8r86ba2TM77IgAK9cb0Kb4m8f1SgSiO1iP1KoNEUsfAX55oEfMccTBU2za5KmfX1LhwFQrl6-zRoeAxWmynC-5dJlAli0COpKn9eQe2eGlvhAXhweOVJFMiMPrIp4rDeUJRSVHQXzGQ1A03sAxsDbNG0eDOWYf9OKXvwCXMT1ig7iqLGxvD-UYA4tJdd2ZmEJWIqR0ZpFHJrWbCVVDyNCyzmdiy8Nii9VdBEdtidRwTvgY-fJrND-tzP2FEiZJU4eVZXPGHumGQLrBsKf9K6NM9KJnngJsVwwBCPSjsqqeQ8IYxllnMqTFUGg6NPKQ/p.jpeg</t>
   </si>
   <si>
     <t>Papa-terra</t>
@@ -1258,7 +1259,7 @@
     <t>Prochilodontidae</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACNL0_62R878dYkHK_SZptda/IMAGENS-PEIXES-COMP/Psectrogaster%20amazonica.JPG?dl=0</t>
+    <t>https://uc74fba5b81091e184fb23167601.previews.dropboxusercontent.com/p/thumb/ABfG-qciPGtY3e4C91HIEHOtHDxP3gSugijkd-ZWYfbg5hFRpvDbxJSMsf7Vai1fYhUX0By4t4aiZWZi67x4iq-vE30dYCMhlrLPgE_1GkmHqTfIV_hK2vwgosycysm7sZ1FH_atnsnlALqQ9MEyVMnqvNHm64WlQilZqqP1FAXAKHh85VE1wiXQb2CNqVqIk7XZhDvlsShsQqhw3TmOBM2GnkB_QquayV3TrrcQFYHAHDJYx2lmovJOpX-0wTBw3pqSbkttXtY7PVlBrcO1kgIDaTXTlEBjiMTXaIksApjuKgui6sPTjB2EYA7E0cbKR2ZUNvZjJD67WgS11vmISZgV7sw1sLt6WbhreFoUPWDfRNEZRQpPAiGuOZlYIs3j4VkqpClm_oprTkS3BdzolZGr1eckzWGfPVmBCBnDLALs1A/p.jpeg</t>
   </si>
   <si>
     <t>Branquinha-cascuda</t>
@@ -1270,7 +1271,7 @@
     <t>0.2</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAD9ZDjhfNB6V6gWvFcmiFcua/IMAGENS-PEIXES-COMP/Pseudoplatystoma%20fasciatum.JPG?dl=0</t>
+    <t>https://uc7e90520245e3c6974300e8e7cf.previews.dropboxusercontent.com/p/thumb/ABfQJwjz0ndBca77lwbHjTw6CXW7n34JlZYOK-2NLX13NKEdVQuOlqcf_jCFl21M1y0D-JGoB14nnI_XWv4OjzaoW64dpHwAADKrMW3imdPjapxQCIswFqqO03PDsDYNihEjp0krNKZ9bt6kDfrpBcSpgWrX7fbpWx8xAbYLnioZht53R9AgAbBQmwnfHmz-U-zQq0LTrE2jVMIsFelQVxaGjtLcIe8oLznIL97KHSGEfh_jh-2M_XeXbH7OaF0ywA6WPtbk_XH8gwRqaI3ls30DSS7_FdqcZzCZuC5zwQBtPh7IINEOrnFFZPhKwgvCleRZ0EiHKP6-cHlyRUwjV7g7sQPcM_Fe0uMqX-RRQgvC53kVzrKLXwq0NSPv9iXC0wvMJ6RmGxt8i-g3oj_RCEaoZgdycE1rfgiMtsXN5EnGwA/p.jpeg</t>
   </si>
   <si>
     <t>Surubim, Cachara, Pintado</t>
@@ -1291,7 +1292,7 @@
     <t>6.5</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAC6F3IwgPnSC65H90tdGsCOa/IMAGENS-PEIXES-COMP/Pterygoplichthys%20joselimaianus.JPG?dl=0</t>
+    <t>https://uccc3a26dca8001df60984dd46e0.previews.dropboxusercontent.com/p/thumb/ABdHyIJdJWfVK1QfIBOTkE6g1iw-P41KDeuYrpTaWVKyvIogoBI1-NcnCOQczF8FjGGWqrb66vAlS3n1WfRNJi8U3QsBDg7BtO9m6k4cq3Igq0rQH-IT1gy6_2V9x_vCUsAc4VjWqETZWUoJQHTluLek_lCcwhzaxCSmYsg4Y5uVsMnzbVYW4Z2gq202hfULKV2TZJ65HIVg0930WeAU8QqDaS13f1k_-CT9Tt43Ze-ul27oEq9LiJC7gJaRwMUYylBfhd6bejvt6A7eK8yU6GjXG-xlGHBOViI9FwXmUyvihKzNOcTv0Lnr6rrB-bXW2mH5CSnVPeETILpNg--0PkZ5ODm22IO4HP0iorBdniRqehpvKFpte6sdUB0msVJVYtOVyjQn_uiYnIWwcIq5KUpY3j8rLOlq7dblJISc6Gi7qQ/p.jpeg</t>
   </si>
   <si>
     <t>Cascudos grandes</t>
@@ -1306,7 +1307,7 @@
     <t>39.5</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AADWsSa9ePO4Cu_WQJkzTn-2a/IMAGENS-PEIXES-COMP/Pygocentrus%20nattereri.JPG?dl=0</t>
+    <t>https://uc0450cdde5830db8d628e12afa1.previews.dropboxusercontent.com/p/thumb/ABeLYrLuMZxMKXbR7rHoBxX_pqEPJ-q1cn6adAb-qINNp-4JrioC-FDLhQqzNriEr-hkgzONFVdFBD3dM_PTX9Tf3FbNWMB5ZeYxItSuNEGs-zA8Fdwma0if8mTcxdCQRZzIWx4s8Qoke1hw9TX1fCclSzUnRfi6BBCbhuqmx1vzDX5ykDTri3X34P43R4acMZZ1JeqZ2ZDMMK51paT3SgNQZrGDTNH19A9Ftba4Cah41YPZA-oVUXL57HNpsPMrNodnTGsyE1zb2zj-lHokTmJvxHZBgqjwmukBJjzpi34bM9cuWIdr7vY-xtWd-KPGN3G6HkRHM5GUawllUYYvkdsLSnXgbh54tf8PmcYG818EtrL63kX4VauW18YfVH8xviu5GTs1gNLHQAsk6JlAG5npe8euvhjv94hNyPAsSRvZ1g/p.jpeg</t>
   </si>
   <si>
     <t>Piranha-vermelha</t>
@@ -1318,7 +1319,7 @@
     <t>3.9</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AACz1lvaNE4ola6s5HDBk3kOa/IMAGENS-PEIXES-COMP/Rhaphiodon%20vulpinus.JPG?dl=0</t>
+    <t>https://uc7cbaa023146e7d14fc365bf5fd.previews.dropboxusercontent.com/p/thumb/ABfwTQkaNioWE1_B5dKGm7WWjXQspOw0CJFvSL0A9t8yVQHOFuTwyUvxahluqW7llo_iB-6TJEhZGWnIuGiE70J7j_A7MEzZNs0V5KrP_NrcuPlkyA0Yy7Cr_sVo_b_O6c1RYJnEEHFcA3QDgzYrptgnc7_w3nxukkN412DDKouFvuJ561-R7drOexSwwA8hB6FWRVi9f7O6fugIGsY2Ss8rzsOtDVA6EvEiK_Ykjl3xEK3YoP_Hhn9tUDOCz9PchhA688AH-kn3rqQKWgJd8JRssWJFeP9_PFFfmLdy352e6UCqEqooAu2sxo5ijrgu8rspYt38SGy8MOPtjcCwvimHwuvoIJosHrUd3IyziBDJv5iFj_1WQOXpJ0EEPUb9dB1i_3fMMeLe0oOmdGc5OPBmn2LWr2Z-CWK0n8Qbkm9x8g/p.jpeg</t>
   </si>
   <si>
     <t>Cachorra-facão</t>
@@ -1330,7 +1331,7 @@
     <t>2.1</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AADq0APo6MtUrzQ6Bn34YGTVa/IMAGENS-PEIXES-COMP/Rhamdia%20quelen.JPG?dl=0</t>
+    <t>https://uc561b3ba606cb2a8e43f284220c.previews.dropboxusercontent.com/p/thumb/ABc5kFfI1d6Rr09uwi4UpPZ1HHBk-n1A8yCctr7gv1E_wk63KfT8nBu-JsUsAbgq_Pet0REKr51ixL0qyCRS0FulRc2ldfLl4yGHovv4aTDao4mpBRW03LWSQMuOgLLHi5hyfZKrbdgLbd6LkxswOM4S4I9WRaHenc4ZuZojgaA2TE0IIPlwaHoQgm_uQlCb5Isfshu_jksD8K94TXjarfpcjjbVbOZEyT5svUc9p5NsvPRcvK69O9w0WQJBS9PJlJLMq2CyDmfcDJt-2adrVGkOJD9D_TW5wyCbKipSbnos8w8bzjPDMX6eZix_MR0wHT3FoY9Dj0kSCnItW8lXSzPYwmGsYeHloho8NnpXZT_D0xy2UdhACKOQw3iTGCJCANFrGNvwEW2zmYPQjmOVmB35mBqfQOhsu1xpckn7aqkbxw/p.jpeg</t>
   </si>
   <si>
     <t>Jundiá, Bagre, Lobó</t>
@@ -1345,7 +1346,7 @@
     <t>47.4</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAD64t33d_lYTf0Ot0d1Gyv9a/IMAGENS-PEIXES-COMP/Salminus%20hilarii.jpg?dl=0</t>
+    <t>https://uc24ee82e6b0dd0b3f1a452135ac.previews.dropboxusercontent.com/p/thumb/ABdwNaEKHKUmrs0LphOhNJCwnhiGqTmBDsZPYFp_sLo3WsQWVk-_ZuFH-uRGsNHhgfHau73xC8xngYWnSvajBnj9hzVO2kqEw2F2Igm2V8QXPqb11eHOiT2i9LCdNOxp91Xupa4MnOab7jZqzhjFDkNfTU28Kp7g1-GcxxzScYcslI8dIUeK6Jaip39Y1ES-JxUnynLKgBJmzMFoHU8um6mjTBm9vZiOsdUFRO4a8JY0iqx96Du2_7rg2S3vto3Zx2nkEtkIZiN6rSIq-xt-7CyPOwutJ4F6lGDTDJNwLgvXflhSlpbph1wfIboVyo0kFbAf2Nt6UBo452CSs7CJ5dVO-A18LC6jt6ufg4O8EEIRMmB7TPU7x7VTnhAuJh7Q1h1iglNn6vGrrsvbwjgE5iWVxEXlDaVjnQLouXJ_Z5kR8w/p.jpeg</t>
   </si>
   <si>
     <t>Tubarana, Tabarana</t>
@@ -1357,7 +1358,7 @@
     <t>1.1</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAC2EQYX64NdzWNCuWAuDrcVa/IMAGENS-PEIXES-COMP/Schizodon%20vittatus.JPG?dl=0</t>
+    <t>https://uc940cf153674f0ce4aefd03eeca.previews.dropboxusercontent.com/p/thumb/ABe9r_X4Q8puGuNyktisc-OtZjdiygrZzSvPlWEpSef9P0zU_aZjAhC-6YjGqlJO74kluz-uhMTaFWfcX3tMT2yjqqAuUaN1dDPs5HM6T8iUt-buoIdnGrHf31HtzS_3otRNdNXtoFOwTVrpbNItHGg7a8AInPEi2lmHEA5EwO-WRCzL5Yu328rVeAFKnjdVKZaDK3Ea0aaDM_FEgltUPQp7UtfSz7U_KOLiwsngvW2BURdU1p4TkC5nHkfdJXpZdLgsO1_uNIBM_Dmcl3tBRfH_0Sd-1lAmlA5Ki4CfT2gfTVDRuX1Qjm38OefRiyi0iiey3i4QpAor3bMYkymVHVAqB1Zdg7yw1YzeunMJBSAiqQ9j-Zpqfu12uGNMRIVkYCUWW1CoNCaPjAMV7eCTIADtJdHngFqG-MFnA49yN6zvAw/p.jpeg</t>
   </si>
   <si>
     <t>Schizodon vittatus</t>
@@ -1372,7 +1373,7 @@
     <t>2.6</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAClkk-O0h17qx0oWtn-CTwXa/IMAGENS-PEIXES-COMP/Serrasalmus%20eigenmanni.JPG?dl=0</t>
+    <t>https://uca556c15aacf9c2baf478338fc7.previews.dropboxusercontent.com/p/thumb/ABd0UCMWdNhEgmzdJ3-vL3p79Rt3CLIYmTJ7a-va9Ptz4LYEIgLJ2XZiCi1CgI01vdmYE1RiafNJaJdkO3dK10s0h5BiGf-H5Z-fx0YRmQqLNPClgrTY_EHrZ7j2DT5clyM6NBrTmnwQMZSWepx6mjsFW16XriLSZYnxor9Lrj8CX2LYh6iK88IzMRkxKGjMvK-eD32xLbOHxzzzBoFeJnEmSPpN0jx7xMqbzMCuzdZczuwepfK2yavxHWUxjmrXUxky59F7gGhUTrUr-JYfPCQp7zIKVS-06qgYzt6G1lumzNnHtTI0xRVgqKdhIzSHSdY87kmMcsIv0zmPb6bnzwbap_nKHkBZYHqFAiNNNpuymCy14anOYkrZKKMtvSAg7r1YqnxCwVdBMz6AdDUmehcGvzOhp15wBqimlsiV6RIw5Q/p.jpeg</t>
   </si>
   <si>
     <t>Piranha</t>
@@ -1381,7 +1382,7 @@
     <t>Serrasalmus eigenmanni</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAC9sHLOxqvoEZIvRND0hhZ3a/IMAGENS-PEIXES-COMP/Serrasalmus%20rhombeus.JPG?dl=0</t>
+    <t>https://uc214cd81079fa3f5be4ee0e0fdb.previews.dropboxusercontent.com/p/thumb/ABc2cU7FcMIc31ShVHnOM8Sf7TKr35brVrCwYH4-mbALsQxhL5g1u-qJbYtnNCa57eyTqKo8TWOQGd3lEhmdJYwfSJKgUBAmUwlVOioksNoNlUj82WHG6JdihgVfUR4nFtOI08nCBJ_UOia4-bfChHt3VfBwbXtP76etO5JiJjBJpvJ5ab_bnABbSdLMJYiTtdpm8lkCfjifWQhxqZcLMjdhmFrqg4p8fpK4Ip_mIGxz3DX19aK8idMyy0hcAZr49EMa45sJ5Y1ZaMOXIYM_eDRGXoPfRgGSgvgbMzh1o-PPoIEDcvnkp12txpvB-h72AdmJhZFNtJNLo729M4ySQ-d1hc9qjZ8f1yb6tCVBLrVgaVyacoy9V4InNcw8mHPmJ_IkzxvF6lXkxD1vR5bulWNgayGBGsTfgdMIpro41SNW8w/p.jpeg</t>
   </si>
   <si>
     <t>Piranha-preta</t>
@@ -1393,7 +1394,7 @@
     <t>41.5</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AABdJLNMq8Nqbbga9VjZfaSUa/IMAGENS-PEIXES-COMP/Sorubim%20lima.JPG?dl=0</t>
+    <t>https://ucc3f474c2861fb01650641440dc.previews.dropboxusercontent.com/p/thumb/ABcHtE7dOTUZJkWRd_6zz9qXsxHQf4_0ubdFjeNJdTMVr4hsdGkmDc5NweRXSgsFAPD_aAiKeeus4RaLNW7CCdMaHMxskCaSyZve2r_DAQT9opYKoRo5gPHL3mBhwcz1BTnSNR6uVqwiQ4GndVoZjaNm6OC3A_xnyLY9MZvfN7nKns66ufXhzTM1q4oyFxXxlCFG6VUZLwDX3GormtTj_0KCEXEwmxVRCyLmyYLzVw-uDx29tTgG1TwGH5c4lEv21kxJGtoruY0tENqfUUz4M0IzM5zH3p5fyrcqU2gKT-23MGi_CgdTtwT9MHF8G2cvkaMM0LInIloson-Qu5ZKp5k-ebPWXYiqAatPFIb6kTWyaNR1NvWQ-wyK3sOCEX5gNWGsjR0xmsgNoabu7-ZeWWTlfUoEAm0ghcuDv1pklw6z5Q/p.jpeg</t>
   </si>
   <si>
     <t>Bico-de-pato, Jurupensém</t>
@@ -1405,7 +1406,7 @@
     <t>54.2</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AABmepXnrKV7MWeYHXOu6Geja/IMAGENS-PEIXES-COMP/Sorubimichthys%20planiceps.JPG?dl=0</t>
+    <t>https://uc7e58b0df394520ffb96a31b712.previews.dropboxusercontent.com/p/thumb/ABcgkRnFag0DXx0Tnjz_7wga1u9AmYLrMBNGmPROP8pu9NU0LZ0TD8dCEH6iuZsvmWUlyFx08hjXGJ-lUEWl_E4be0xivy5qDGHI-w6sxEbN6BaiHHhVdSw_mB5ObS-tES6kj2zDK5MfWUwgFhSub8qJ-YXynF4ltFsnxemxiulknjGzspsVyuyk89dclXz90pjZ-g0dlTLz6DgYoInb_WBhZcnIWjrwgMCTllM-1Jh9YyZ_Pu561dmnHESg6Jr3gLIcXbRpvZcx1HBsJshpsIcbfAQ8eBNg-iKPinio7VpXJma5HDEwekDRPtjC1FXeW8Z04TioftDh0SDStNavOzfAwHl6rhpz3O5U4nGu-96H6uJHToM1FWspqicnv87VPRBmkaKDiMR-bCjSmjH8t3hzeTDZSIZxWKpYU7wa-oWTsQ/p.jpeg</t>
   </si>
   <si>
     <t>Surubim-chicote, Bargada</t>
@@ -1429,7 +1430,7 @@
     <t>Synbranchidae</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AADbgGlZQyvj0KdS8BGwRJ1ra/IMAGENS-PEIXES-COMP/Tetragonopterus%20argenteus.JPG?dl=0</t>
+    <t>https://uc468eb4491bea3902454a023f08.previews.dropboxusercontent.com/p/thumb/ABcCz1iBA6elQb5edj2fL_x9MUyPj2UJ6wglAaeZ8mB0Zq9byVrsSwOzSjoRrGcciZ6vFx1BWrdAbpAzUgfrx1FYKulqaMpwdpMvU7HIyB-SVotjad5RxEXqGuh2Z_ohPXVZbttSdVaf0fsU8IFiHo110O3cWrX13ZF6VNT_NJgkRPiqosJvLfmKx-vqe6JXF7gEaseB-hOEDTFwWtbwXUQylqz4GIR61YHyEHbdWLWxBJ3MbUIsZCKa2VygdD5hSRwfK43g3biT3L9PZDujVlZgVo7CAxQOpkNw7UXgruTJjYndQwAyWkqEGe-nPpDxhtcbFGUUddOspw-_g19NeXk5I2o2qtnUxDmzRiVqKbswps12B_4dpeH0JKObFJnQvZ544l8S_IDRpAlDkrUeDkVYv-C4oUeasN-sgQAkPw7-5A/p.jpeg</t>
   </si>
   <si>
     <t>Pataquinha</t>
@@ -1438,7 +1439,7 @@
     <t>Tetragonopterus argenteus</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AADnlkGtA7fiF7o81dZslO3Pa/IMAGENS-PEIXES-COMP/Trachelyopterus%20galeatus.JPG?dl=0</t>
+    <t>https://uc49fa0cbdb0be62073bcd6f37ec.previews.dropboxusercontent.com/p/thumb/ABf1Kpuxlbn7Dhd1H6AA0ahGqFH0aBb-uk7Vhpg4P3HihaiexEvfZo1mKOs20Fp0OVN8Q3llsC0_XnNU94t5oWA-c3hXGhmBYo5HHPRzyt3LXmd5myqUdXosEC4wrWVkzLcz2aIHTeR2-WKlK9V0LCiucUmU2kKA9EXnlYdJJ0AUmc91BDWXB-7rewc4qy9483DUOZPizK3DL91m7pGct7oMW51fIReNeJ4-ebMMt3PrVr3A5-P-EEQ84FmvQJfVRzRxOODyhpaCEFDI6MS9_wsplbW5W4ZAk5tKKk822uVfZZBevrp2F0BvgDim9LpDVhkitvEjLxMPO3c6f1LpLi1iJKy56WAdNH5aOQskOXcm4s1OBlQwIzU-7su3t6xEn93jGMlIGHLfNx0IPvCCKi6Ci78EjszHJnq8JdBQ4v5QFw/p.jpeg</t>
   </si>
   <si>
     <t>Cangatí, Cachorro-do-padre</t>
@@ -1447,7 +1448,7 @@
     <t>Trachelyopterus galeatus</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAA_KSDc8TQ9IhRf6LLb7L7da/IMAGENS-PEIXES-COMP/Triportheus%20albus.JPG?dl=0</t>
+    <t>https://uc589611219f1960daf2097896e7.previews.dropboxusercontent.com/p/thumb/ABcsSMMY8yQn0SebALghdta5kA1G93Hz_K9oAb4gsspClegxItpTOnrP5MbR57w8_pdOysunCj-_ajn0rZkPJfYxBM3tfxxJraj7vthDMtCFwxxk3OK3naNqM3jvSbwzz1TwdP9_b85G-ZsCaI66LO_bP62Hbgz9Whnt1ScO8enHCNi2GD2kvcZayYZ4qPmXVIcSeqZ-7Bq5H5C_hmruj7SFdypbNw4FP83tJ8nM8Lfjy-leBC5MKjaRRLDw9tsqmQBOVhFjFhMQWUfCH5I4Qif-b7FqEKG94zsMW7wwv1XNmis1cd83hjKaUSOdQ16ZczrRSgsiF4uVVaLiS5iI7OKAw5nbIP5fF9D8_DetkPmUsVM_j7rNP9QPcHHMmGtorLdid0eF9g9E5v7y18i9BzYtMiJbpx-k7Joit2OAmJxHvg/p.jpeg</t>
   </si>
   <si>
     <t>Sardinhas</t>
@@ -1462,7 +1463,7 @@
     <t>25.7</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAAQGRq3z7ED4QDaq6H6y3vga/IMAGENS-PEIXES-COMP/Triportheus%20trifurcatus.JPG?dl=0</t>
+    <t>https://uc9b2ddc0c78a7155fb0ed01917b.previews.dropboxusercontent.com/p/thumb/ABdEGLF7egd0G2pM5dX7AGfo5FHhA9z3-BeHeQ5MOL8t-21T0VP5sDaixagumCtk_MlBgdy_0tvf9MaX1YNQA7EABMowbeo-rHDQMw9VgpgKGD1xDY3bZhWOqbtQ738Spy4x19ptCkfO4Wwv43oW7XqBbFtm9Tm6sKDl-NBbrD7_4x7-Gh8fS8xiQfcME881MUrn7D66XfSMy22Tq94cFhoJ651n-QK0aojgxLnRs2_Ti0mEzcEqomrUfZhUvQ2XVBb9nXBP-hS9-adzeododwbM6rJhdyn7p-C5vhZbKcZ87E4JfOPqa6toQLyV-VjMSJXlDeRY-PoV1RTgfcj1JG0ntpZfDkGH156rOgqUYUQEmczkiSRIEkPaHEwia9v7BDNPXtd5pwLTOayDvO_jhv8-QaWnwEiF65Nr7rlEuooG1w/p.jpeg</t>
   </si>
   <si>
     <t>Sardinha-papuda</t>
@@ -1474,7 +1475,7 @@
     <t>16.5</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AAA7NxFhV1XWPolav1l8Ra9Xa/IMAGENS-PEIXES-COMP/Zungaro%20zungaro.JPG?dl=0</t>
+    <t>https://uc18f08d002c9a613a28a0086fad.previews.dropboxusercontent.com/p/thumb/ABfd58-PPmiYUdNAlDEe6h_B6IiaQf-oEHlirhQvWpX-XKGSgCDDuDKtOoCxJOPRdu7xvqUL_erXsTKizY6z17GZL1x_teTKqjTEJZkaNxemRCKNT04YurJnLG2vu_M45BvRdKE2bQfFrkxkLmYjzPjlww8mnvF5xyEEotaHy8BjossG4W17EvII383240-B5YjOaDkrpQv04tHxXpNLNyGmPbes2icuc7oanqagd8eQzgrnL72v0qa4kpS7vkpZ4T5fHAiYrJlEWb73Fnm-S-oVKbfV72NuLw7tXv3Dq8SqSs1Y_rtdVVK6WiSj10iKMZw6ZVsvC4rk9DOAbGunSFGea9m20NOm4SxPS_Rp4jjD26BmgrhSHWG5i_D1LUS9tCqlA-VAOPIQFA4NR1IyGWrgQivItcfAAg2ox9luhuo2uQ/p.jpeg</t>
   </si>
   <si>
     <t>Jaú</t>
@@ -1483,7 +1484,7 @@
     <t>Zungaro zungaro</t>
   </si>
   <si>
-    <t>https://www.dropbox.com/sh/yacowjkdclxiyp9/AABZndaVIQjC6xaMcxRajZ9pa/IMAGENS-PEIXES-COMP/Leporellus%20vittatus.JPG?dl=0</t>
+    <t>https://uc0c68e868d69f568916df4f9c30.previews.dropboxusercontent.com/p/thumb/ABdadMC-x1JdIQE6azcIAnUZxoHQfS7DLvWVp_TG-CYvSWhO7mxYUAWvRjLTvPNtwet5zTvcWxSHIqHZThrF7C7uNZFEA0bb9xnhn9NM4UXlMs4sN6yGwkjmTqKyMXkhedfseiT1h3FfQIeGHwND8N9_G1AoKryRlBL29SJbrQcb0VauWEaeAhy5wQS0ZKKN-VpGLv6jm64kByGsCxnxvPj_mE4zg94e071cAO-55WTXgYWj58gOwls9oFJy9uvBvgkEA2fktpI58AF5jVilDZNR4YJhNU4-UdgJdjZXwZQoZQCFNuGq-fidKh5bsPrUzBuUpX272pE61eOlaI7jCDRx5oEMWdqpvK_T0R7h2Ras8sK7UlGBst59CxFjQMi_nT9koBAHvtd7vexzlF0rWJXQAWtoJ1Z7cYdP6ijrMR0pow/p.jpeg</t>
   </si>
   <si>
     <t>Peixes de escama</t>
@@ -1857,8 +1858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:X118"/>
+    <sheetView tabSelected="1" topLeftCell="O94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X104" sqref="X104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -1880,6 +1881,7 @@
     <col min="18" max="18" width="0" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="137" customWidth="1"/>
     <col min="23" max="23" width="3.28515625" customWidth="1"/>
+    <col min="24" max="24" width="27.7109375" customWidth="1"/>
     <col min="31" max="31" width="41.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7057,190 +7059,192 @@
   </sheetData>
   <autoFilter ref="A1:O1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="S118" r:id="rId1" xr:uid="{08A3F25F-0414-4A0F-A719-72B022F2E356}"/>
-    <hyperlink ref="S116" r:id="rId2" xr:uid="{FA043706-2418-432F-B7FE-CD4917F577EF}"/>
-    <hyperlink ref="S115" r:id="rId3" xr:uid="{9B08E448-A33F-4876-8B2D-80E23B551D54}"/>
-    <hyperlink ref="S2" r:id="rId4" xr:uid="{42BCB43A-A740-4362-9343-018B8DAFFD31}"/>
-    <hyperlink ref="S114" r:id="rId5" xr:uid="{0D168D68-FFA1-4886-8A0B-DB218F59AE1C}"/>
-    <hyperlink ref="S113" r:id="rId6" xr:uid="{C22B599C-F442-4501-A9F9-6A8400F6172C}"/>
-    <hyperlink ref="S112" r:id="rId7" xr:uid="{0F8FF7E4-C11D-43EB-A495-B509DB231213}"/>
-    <hyperlink ref="S109" r:id="rId8" xr:uid="{459A5495-4787-4D8F-B703-4AFBBD4034D8}"/>
-    <hyperlink ref="S108" r:id="rId9" xr:uid="{C330ABE3-972D-4081-AAC3-C63501B0F5C2}"/>
-    <hyperlink ref="S107" r:id="rId10" xr:uid="{5277B38A-204B-4B87-9040-A744AFC25530}"/>
-    <hyperlink ref="S106" r:id="rId11" xr:uid="{6ED5A6FC-2B11-4300-AF1C-41821F8AB203}"/>
-    <hyperlink ref="S104" r:id="rId12" xr:uid="{2F7B420F-24FC-4CCA-8AEA-29E61AF1ECD6}"/>
-    <hyperlink ref="S103" r:id="rId13" xr:uid="{0308509F-1F94-49E7-A457-BA1A2A654AB9}"/>
-    <hyperlink ref="S102" r:id="rId14" xr:uid="{1DF4DD8D-5377-4193-AE41-2B8277ACBDEB}"/>
-    <hyperlink ref="S101" r:id="rId15" xr:uid="{A0AD95C2-9571-47B5-B12F-F459C414E925}"/>
-    <hyperlink ref="S100" r:id="rId16" xr:uid="{F9288155-8FF7-4E08-8181-3714D1F4AAE5}"/>
-    <hyperlink ref="S99" r:id="rId17" xr:uid="{46D99794-CF13-4DCB-B26D-67035C8C2141}"/>
-    <hyperlink ref="S97" r:id="rId18" xr:uid="{BCEC2863-A25D-454A-A7DD-050F6C31238C}"/>
-    <hyperlink ref="S96" r:id="rId19" xr:uid="{23DDFA23-4E47-4469-B38E-BDC9BAE646A2}"/>
-    <hyperlink ref="S95" r:id="rId20" xr:uid="{B267C1DE-294D-442D-954D-0CB23BF7FE57}"/>
-    <hyperlink ref="S91" r:id="rId21" xr:uid="{684E1A62-CE22-4299-8956-8EB927260FF8}"/>
-    <hyperlink ref="S89" r:id="rId22" xr:uid="{74DFAD5E-15A5-4F5D-A7DC-F051F4DB143B}"/>
-    <hyperlink ref="S88" r:id="rId23" xr:uid="{B45807E6-7392-4AD2-9F08-022937B69378}"/>
-    <hyperlink ref="S87" r:id="rId24" xr:uid="{4D7DD7B5-1489-4282-86D7-96E75FFB7B63}"/>
-    <hyperlink ref="S86" r:id="rId25" xr:uid="{E7E937AD-BBF5-4986-B89A-53E905853B98}"/>
-    <hyperlink ref="S85" r:id="rId26" xr:uid="{FC6A2171-7CC2-4E0F-858C-D70AE62BCD49}"/>
-    <hyperlink ref="S84" r:id="rId27" xr:uid="{2AF5EBD7-1F31-431C-A2F0-F38F2CF2EAEF}"/>
-    <hyperlink ref="S83" r:id="rId28" xr:uid="{64863B1C-44EC-4D8B-9E8C-08CA16AAA5C5}"/>
-    <hyperlink ref="S82" r:id="rId29" xr:uid="{3C55DEBF-3646-48AA-9074-10179AE8018B}"/>
-    <hyperlink ref="S80" r:id="rId30" xr:uid="{6C29BEEB-9380-4475-833C-4EC3C7791646}"/>
-    <hyperlink ref="S79" r:id="rId31" xr:uid="{F1A4DB3E-C837-46CD-8853-637CE70E4625}"/>
-    <hyperlink ref="S78" r:id="rId32" xr:uid="{D2D46AB3-F33E-42B3-AF6D-9CC5D7FE9DA7}"/>
-    <hyperlink ref="S77" r:id="rId33" xr:uid="{6684545E-95B7-4D76-B123-007EC36D247C}"/>
-    <hyperlink ref="S76" r:id="rId34" xr:uid="{9E89D255-5C13-4C5C-81FA-3B908D4FD707}"/>
-    <hyperlink ref="S75" r:id="rId35" xr:uid="{5932A081-90C7-4C9E-8007-1735043537FC}"/>
-    <hyperlink ref="S73" r:id="rId36" xr:uid="{1D081D37-D3D6-4B6D-94E7-B150C41DB62E}"/>
-    <hyperlink ref="S72" r:id="rId37" xr:uid="{D21EE40B-43F0-4267-ACCA-8410E8A90238}"/>
-    <hyperlink ref="S69" r:id="rId38" xr:uid="{3D8DCC6E-A185-4F3E-9CF0-523F4B53695D}"/>
-    <hyperlink ref="S67" r:id="rId39" xr:uid="{E2B468C6-38E2-4F50-B521-D7873935576C}"/>
-    <hyperlink ref="S66" r:id="rId40" xr:uid="{6A7AD920-F7E9-4B9C-A793-D35F4D695E6A}"/>
-    <hyperlink ref="S63" r:id="rId41" xr:uid="{27FE5FEC-D381-4D2E-BD24-B0A183EAC1D0}"/>
-    <hyperlink ref="S61" r:id="rId42" xr:uid="{9F35053B-AFFE-47B5-A05D-216185E4DB51}"/>
-    <hyperlink ref="S62" r:id="rId43" xr:uid="{B7BE9BE8-F682-4C1A-9B73-74956E1BFB50}"/>
-    <hyperlink ref="S60" r:id="rId44" xr:uid="{8C51B5C6-E1F6-4F4D-B258-2E00C10F816D}"/>
-    <hyperlink ref="S59" r:id="rId45" xr:uid="{36F4343C-DB8A-45A6-BBAC-0088882378A9}"/>
-    <hyperlink ref="S58" r:id="rId46" xr:uid="{820A12A8-022D-444D-981C-135311FD60C3}"/>
-    <hyperlink ref="S56" r:id="rId47" xr:uid="{EE1E2092-AC87-468B-8185-F8CC3AACACE4}"/>
-    <hyperlink ref="S1" r:id="rId48" xr:uid="{9ECB1404-B45D-4AFC-816E-26036A3FCBBB}"/>
-    <hyperlink ref="S11" r:id="rId49" xr:uid="{33D3FA1D-DC37-4FDF-A096-69C2D2324395}"/>
-    <hyperlink ref="S10" r:id="rId50" xr:uid="{EC53894E-6532-4B09-861D-B6EE7DC6A583}"/>
-    <hyperlink ref="S9" r:id="rId51" xr:uid="{9CDDFEA1-8012-4701-BAC5-2D7225E170F5}"/>
-    <hyperlink ref="S8" r:id="rId52" xr:uid="{4B3F45E0-42DF-4E9E-9C80-2F0C3EEEBAF8}"/>
-    <hyperlink ref="S7" r:id="rId53" xr:uid="{EC8768B4-E6BE-40DD-9C77-E3A425D4B0FB}"/>
-    <hyperlink ref="S6" r:id="rId54" xr:uid="{60261B18-2BCC-49FD-88BE-A28704D0A89F}"/>
-    <hyperlink ref="S4" r:id="rId55" xr:uid="{AFDBFE02-5199-40BE-901F-5A390252797D}"/>
-    <hyperlink ref="S3" r:id="rId56" xr:uid="{70DEF3EC-7056-4B17-8850-C1CE31B288FB}"/>
-    <hyperlink ref="S14" r:id="rId57" xr:uid="{F80EA165-40A2-490E-B378-8667EDB1CF82}"/>
-    <hyperlink ref="S15" r:id="rId58" xr:uid="{AB3D87C9-7D0F-4032-9690-F550082C465F}"/>
-    <hyperlink ref="S16" r:id="rId59" xr:uid="{5E73B485-8D4E-406B-8E01-9A24198B6989}"/>
-    <hyperlink ref="S17" r:id="rId60" xr:uid="{1C216117-3EA3-4DB1-9344-5A878188703E}"/>
-    <hyperlink ref="S18" r:id="rId61" xr:uid="{24A2721C-1EE4-4619-AF54-6A980028DC39}"/>
-    <hyperlink ref="S19" r:id="rId62" xr:uid="{D14E1F61-D584-443D-B8F9-469505A35F52}"/>
-    <hyperlink ref="S20" r:id="rId63" xr:uid="{BB7C0591-AED2-4C94-A813-DD979708BA14}"/>
-    <hyperlink ref="S21" r:id="rId64" xr:uid="{F13F8704-8289-41EA-A3A6-659480185842}"/>
-    <hyperlink ref="S22" r:id="rId65" xr:uid="{A5389021-867F-4831-B886-1C614F4D4754}"/>
-    <hyperlink ref="S23" r:id="rId66" xr:uid="{091CB816-BEA2-4F12-A75A-DD98A837D23E}"/>
-    <hyperlink ref="S24" r:id="rId67" xr:uid="{384C6749-AB5C-4DBD-B525-B4C6D8B88403}"/>
-    <hyperlink ref="S25" r:id="rId68" xr:uid="{22333AE4-0388-4368-B086-4E3B48650CD3}"/>
-    <hyperlink ref="S26" r:id="rId69" xr:uid="{827731C5-3AE8-40B2-BC57-FE841C69DAEF}"/>
-    <hyperlink ref="S29" r:id="rId70" xr:uid="{A7E47F32-F209-4CDF-ABEA-539DA5D4A66C}"/>
-    <hyperlink ref="S30" r:id="rId71" xr:uid="{D9B893A6-989C-40E2-BD5D-FD5F18683B13}"/>
-    <hyperlink ref="S31" r:id="rId72" xr:uid="{504959EF-916C-4300-8F03-4AC31162701F}"/>
-    <hyperlink ref="S32" r:id="rId73" xr:uid="{2EEEAE0B-6781-49AD-AC40-A5610FF1DAA4}"/>
-    <hyperlink ref="S33" r:id="rId74" xr:uid="{4177EAB0-9D3C-4DB2-943A-C88B49F0A04E}"/>
-    <hyperlink ref="S36" r:id="rId75" xr:uid="{FDAC5791-2B05-4B1F-B329-E7A655CECDC6}"/>
-    <hyperlink ref="S37" r:id="rId76" xr:uid="{03628202-D11F-4A5F-BE71-DE2A5AD97B71}"/>
-    <hyperlink ref="S39" r:id="rId77" xr:uid="{6C294763-D096-4B9C-B1FD-4DB5E5C9934A}"/>
-    <hyperlink ref="S40" r:id="rId78" xr:uid="{DC7E5C5D-3291-4BE2-A97F-B05603CB0686}"/>
-    <hyperlink ref="S41" r:id="rId79" xr:uid="{91D38BF0-A6C2-4871-BCD4-69E399FCFB24}"/>
-    <hyperlink ref="S42" r:id="rId80" xr:uid="{E9D4D0E1-8BFE-4EF4-89B8-0FDDEEAE3BCF}"/>
-    <hyperlink ref="S43" r:id="rId81" xr:uid="{DA64F217-2099-46D6-8846-3DF0D87ED1C2}"/>
-    <hyperlink ref="S44" r:id="rId82" xr:uid="{45A27B6B-B9EC-4F35-84B7-CE9A211662C0}"/>
-    <hyperlink ref="S45" r:id="rId83" xr:uid="{2F4D4E24-8D85-4DC3-A68F-C8835A8C8CC8}"/>
-    <hyperlink ref="S46" r:id="rId84" xr:uid="{9A9466B3-7C2C-4C04-9C42-C6F95183D15A}"/>
-    <hyperlink ref="S47" r:id="rId85" xr:uid="{42A7F6EA-BA09-490B-AEA0-932EB36AECAB}"/>
-    <hyperlink ref="S48" r:id="rId86" xr:uid="{EB6BF247-0D37-4FEE-B8BB-3FD000029744}"/>
-    <hyperlink ref="S49" r:id="rId87" xr:uid="{CBB9CFE0-32A8-4560-A6E6-23C5B2B59FAD}"/>
-    <hyperlink ref="S52" r:id="rId88" xr:uid="{7932744B-D63D-4C1F-844E-6D281C4BBBD3}"/>
-    <hyperlink ref="S53" r:id="rId89" xr:uid="{B4543D33-6DE6-48F7-BF92-D2ED31FFFF12}"/>
-    <hyperlink ref="S55" r:id="rId90" xr:uid="{31F44A9D-D9C5-4F49-B2D2-2FB243B3B396}"/>
-    <hyperlink ref="S64" r:id="rId91" xr:uid="{2DDF491D-2026-47BB-9E85-949DF05C3A0F}"/>
-    <hyperlink ref="S51" r:id="rId92" xr:uid="{638ADFD7-425E-4B69-B8F4-37E94BCDF139}"/>
-    <hyperlink ref="X118" r:id="rId93" xr:uid="{6D409CB9-5472-4B12-AB8A-2ECA29EABD0A}"/>
-    <hyperlink ref="X116" r:id="rId94" xr:uid="{B5E30B03-9A75-4020-81B4-37EE7E15797E}"/>
-    <hyperlink ref="X115" r:id="rId95" xr:uid="{03AFE4C2-3B07-4229-9B2E-C15CA0A9308F}"/>
-    <hyperlink ref="X2" r:id="rId96" xr:uid="{EB45551D-7971-49EC-8D6A-AF3B58D00971}"/>
-    <hyperlink ref="X114" r:id="rId97" xr:uid="{1BC5E21F-4285-4B68-AD86-30E2029F7332}"/>
-    <hyperlink ref="X113" r:id="rId98" xr:uid="{2F5EA629-1D29-4BF8-B584-8B7AE44AAA1E}"/>
-    <hyperlink ref="X112" r:id="rId99" xr:uid="{ABC8FE78-1BE3-4F98-A3A5-73B412639C20}"/>
-    <hyperlink ref="X109" r:id="rId100" xr:uid="{98C1F4C7-AC30-4864-94C3-2CB6A8C41519}"/>
-    <hyperlink ref="X108" r:id="rId101" xr:uid="{F2CBD225-22EB-4034-8AD5-78D7D75E80E0}"/>
-    <hyperlink ref="X107" r:id="rId102" xr:uid="{75DAE6E6-9ABE-4B5C-BF24-EAF030DAC930}"/>
-    <hyperlink ref="X106" r:id="rId103" xr:uid="{AC80106D-754F-47EC-B13E-5A5080A54E6D}"/>
-    <hyperlink ref="X104" r:id="rId104" xr:uid="{B6E73C6A-3D6E-4544-B3CB-ADB615F6CAA6}"/>
-    <hyperlink ref="X103" r:id="rId105" xr:uid="{38994A13-6852-4FD3-A857-6ED4DC355081}"/>
-    <hyperlink ref="X102" r:id="rId106" xr:uid="{1D74813C-AB57-4444-B881-583079BBC2E6}"/>
-    <hyperlink ref="X101" r:id="rId107" xr:uid="{0E50AC8A-5A9A-4BDF-81BF-D086861800A4}"/>
-    <hyperlink ref="X100" r:id="rId108" xr:uid="{9D52EDE2-B0A8-4B2F-916F-07502724F846}"/>
-    <hyperlink ref="X99" r:id="rId109" xr:uid="{0D50A806-8EFA-4C54-9932-4484A25AA005}"/>
-    <hyperlink ref="X97" r:id="rId110" xr:uid="{6BBC3CF1-4A21-44F1-844F-FC36656709F5}"/>
-    <hyperlink ref="X96" r:id="rId111" xr:uid="{C0A42781-30F1-4830-BB1E-E90C775F3548}"/>
-    <hyperlink ref="X95" r:id="rId112" xr:uid="{C245D737-DA87-4947-8C7C-CE08CB088C3E}"/>
-    <hyperlink ref="X91" r:id="rId113" xr:uid="{0D41F64C-1AE8-4FB8-BEBF-3B81C22926ED}"/>
-    <hyperlink ref="X89" r:id="rId114" xr:uid="{34BEC296-A515-4369-BC36-FCBF09DA281F}"/>
-    <hyperlink ref="X88" r:id="rId115" xr:uid="{642B7C7F-DE89-4383-959C-70D6BB231B36}"/>
-    <hyperlink ref="X87" r:id="rId116" xr:uid="{1554FEF3-48C2-4DE8-9C2C-57D63B0D1605}"/>
-    <hyperlink ref="X86" r:id="rId117" xr:uid="{74D60557-DBF8-4857-96F2-E6218E61D890}"/>
-    <hyperlink ref="X85" r:id="rId118" xr:uid="{CCF2BA8E-8137-4F02-8CA0-043FB1C64B96}"/>
-    <hyperlink ref="X84" r:id="rId119" xr:uid="{65E533D8-D9FF-470A-BB35-DAD642242C1B}"/>
-    <hyperlink ref="X83" r:id="rId120" xr:uid="{89C6A5EF-ECF1-470C-8CA6-A9A2471EF6DC}"/>
-    <hyperlink ref="X82" r:id="rId121" xr:uid="{A4C8BCDE-D903-4281-A8C6-F601170FF3DC}"/>
-    <hyperlink ref="X80" r:id="rId122" xr:uid="{285A8B4C-9D0E-4D53-A96A-6CAEF87E4621}"/>
-    <hyperlink ref="X79" r:id="rId123" xr:uid="{4D547B67-7B2E-4E8C-9B2E-9AB10A7E6A58}"/>
-    <hyperlink ref="X78" r:id="rId124" xr:uid="{00AC5DC8-0B1A-45EE-B8EE-C98A4AEE2FF1}"/>
-    <hyperlink ref="X77" r:id="rId125" xr:uid="{1B988C9B-4D0C-47EB-85D3-5AE14F84627F}"/>
-    <hyperlink ref="X76" r:id="rId126" xr:uid="{546BAB12-6ADC-4D1D-9AEF-7C7920102954}"/>
-    <hyperlink ref="X75" r:id="rId127" xr:uid="{BB7F7443-717D-4F39-8D02-74FFACE5AFB6}"/>
-    <hyperlink ref="X73" r:id="rId128" xr:uid="{3857EA5C-17B9-4571-9CE0-7B0CEF4FC475}"/>
-    <hyperlink ref="X72" r:id="rId129" xr:uid="{CCF3758A-352F-45DE-83F2-047816B61DF6}"/>
-    <hyperlink ref="X69" r:id="rId130" xr:uid="{E6C8D17C-7D0D-49E9-9DFE-23B6BE4A1FBA}"/>
-    <hyperlink ref="X67" r:id="rId131" xr:uid="{3C29B990-AAC6-44D3-9E66-35CB94D6BD5E}"/>
-    <hyperlink ref="X66" r:id="rId132" xr:uid="{CFEEFB24-004C-473B-9B72-98FAAA155687}"/>
-    <hyperlink ref="X63" r:id="rId133" xr:uid="{5216637B-649E-4233-80A0-B3FD95D343E4}"/>
-    <hyperlink ref="X61" r:id="rId134" xr:uid="{9DF42FCD-D729-49DD-8EDE-2D164570355B}"/>
-    <hyperlink ref="X62" r:id="rId135" xr:uid="{2549495B-9440-4D5F-864C-40657C65F12D}"/>
-    <hyperlink ref="X60" r:id="rId136" xr:uid="{6EA73B25-4314-43BF-84D7-C1025B828710}"/>
-    <hyperlink ref="X59" r:id="rId137" xr:uid="{39F5AAE0-DE83-4426-819B-DFC4D88E77C8}"/>
-    <hyperlink ref="X58" r:id="rId138" xr:uid="{A261690A-FB58-48A4-83CD-7EE23CAAFE11}"/>
-    <hyperlink ref="X56" r:id="rId139" xr:uid="{DA9991D4-4218-46E6-943F-5D6F0851211D}"/>
-    <hyperlink ref="X1" r:id="rId140" xr:uid="{AADE2FCC-FBE9-4037-9A44-091744B115F9}"/>
-    <hyperlink ref="X11" r:id="rId141" xr:uid="{3D833E68-F0B4-41D0-B8DD-882B594775B4}"/>
-    <hyperlink ref="X10" r:id="rId142" xr:uid="{E813F73D-2B9A-4D9E-833E-71C17EB2CD05}"/>
-    <hyperlink ref="X9" r:id="rId143" xr:uid="{9C51DBCD-54CA-4278-8636-9E592E346E87}"/>
-    <hyperlink ref="X8" r:id="rId144" xr:uid="{BD00D2D9-AAFD-45CB-8E97-97CBDCA599C4}"/>
-    <hyperlink ref="X7" r:id="rId145" xr:uid="{EB192115-710B-4EF7-A9E0-2C418ED41823}"/>
-    <hyperlink ref="X6" r:id="rId146" xr:uid="{9DD78B19-34F6-4676-B349-10181322B59D}"/>
-    <hyperlink ref="X4" r:id="rId147" xr:uid="{0859B299-8675-4EBC-AB58-25A7041F4C22}"/>
-    <hyperlink ref="X3" r:id="rId148" xr:uid="{7BB9ABBF-C981-4B72-B29C-F4929C395D0A}"/>
-    <hyperlink ref="X14" r:id="rId149" xr:uid="{3281EE27-6A9E-4970-B235-18B2FF6E361E}"/>
-    <hyperlink ref="X15" r:id="rId150" xr:uid="{7FDB7AD3-9180-454D-8331-E5B39498F82F}"/>
-    <hyperlink ref="X16" r:id="rId151" xr:uid="{144A7458-1627-4CAB-9F25-D4DC5DF60CA7}"/>
-    <hyperlink ref="X17" r:id="rId152" xr:uid="{FC7FC384-EC8E-41B0-9333-6D4EDE50377D}"/>
-    <hyperlink ref="X18" r:id="rId153" xr:uid="{BC4A0553-028C-440C-8ECA-087CAC548267}"/>
-    <hyperlink ref="X19" r:id="rId154" xr:uid="{A61BB485-6385-47CF-BEDE-BE09C085031A}"/>
-    <hyperlink ref="X20" r:id="rId155" xr:uid="{636BEE57-B70F-4AFC-A1D6-6C3607546AD4}"/>
-    <hyperlink ref="X21" r:id="rId156" xr:uid="{A077AF0B-86E2-4686-AC25-703C709EBC36}"/>
-    <hyperlink ref="X22" r:id="rId157" xr:uid="{3DAEFE40-F37C-4A48-BF56-18B8FB8DB98D}"/>
-    <hyperlink ref="X23" r:id="rId158" xr:uid="{E8ACC0DE-2352-4BED-91E6-CDFA5BED5775}"/>
-    <hyperlink ref="X24" r:id="rId159" xr:uid="{6664C09B-126F-45DB-BD80-01D27874200A}"/>
-    <hyperlink ref="X25" r:id="rId160" xr:uid="{83643440-1DE9-4326-BEE1-0B7A4ACFBA34}"/>
-    <hyperlink ref="X26" r:id="rId161" xr:uid="{24EE32A3-F255-4971-92BD-B18CA60224BB}"/>
-    <hyperlink ref="X29" r:id="rId162" xr:uid="{114E0B9C-AD21-4E30-AB64-24ACC63DBF12}"/>
-    <hyperlink ref="X30" r:id="rId163" xr:uid="{833FC9A2-7290-4372-83AD-6982DD0E071E}"/>
-    <hyperlink ref="X31" r:id="rId164" xr:uid="{3FA93865-D042-4302-9F45-2CFB4616C346}"/>
-    <hyperlink ref="X32" r:id="rId165" xr:uid="{51824781-FB27-4A5E-9457-C7E3D5374224}"/>
-    <hyperlink ref="X33" r:id="rId166" xr:uid="{B5AA74E8-6217-480B-8E47-A644AF763483}"/>
-    <hyperlink ref="X36" r:id="rId167" xr:uid="{FDAD1893-CA96-4E0C-98EC-36165CFFADDC}"/>
-    <hyperlink ref="X37" r:id="rId168" xr:uid="{257195C3-BF96-43FA-A695-D523EE129800}"/>
-    <hyperlink ref="X39" r:id="rId169" xr:uid="{14C704B5-52F4-491F-879B-80EAF36E3AF6}"/>
-    <hyperlink ref="X40" r:id="rId170" xr:uid="{BC7FA5BA-4280-4344-88D2-41B05882DB26}"/>
-    <hyperlink ref="X41" r:id="rId171" xr:uid="{AB22EDB3-64EA-4DD4-B31F-56BDD8989C95}"/>
-    <hyperlink ref="X42" r:id="rId172" xr:uid="{BE1EE722-4DE5-41BC-92EC-7C8540DE2DC2}"/>
-    <hyperlink ref="X43" r:id="rId173" xr:uid="{4B024BC0-3294-4DAA-BC9D-2F5E646BEC9C}"/>
-    <hyperlink ref="X44" r:id="rId174" xr:uid="{862B6BA6-4841-44B1-8CA6-3D1794390896}"/>
-    <hyperlink ref="X45" r:id="rId175" xr:uid="{F9FDD8E6-98F9-48A3-A0D1-969A3052A5AE}"/>
-    <hyperlink ref="X46" r:id="rId176" xr:uid="{08C35F6C-2863-40AE-AF11-D0EECE8271CD}"/>
-    <hyperlink ref="X47" r:id="rId177" xr:uid="{B8FC9862-2CC0-4AD9-9AEA-548FA23D328B}"/>
-    <hyperlink ref="X48" r:id="rId178" xr:uid="{365AC08C-7659-4C0A-A4C6-A44A9C2F13E3}"/>
-    <hyperlink ref="X49" r:id="rId179" xr:uid="{07BAD4B4-E92A-4291-922E-2C88CE2A49D2}"/>
-    <hyperlink ref="X52" r:id="rId180" xr:uid="{ED8ECEDF-EFA9-4B28-82DE-741895D31E84}"/>
-    <hyperlink ref="X53" r:id="rId181" xr:uid="{D6E91280-C98F-4584-8D1C-FE041B71DE43}"/>
-    <hyperlink ref="X55" r:id="rId182" xr:uid="{90EE6D7B-BD16-4B99-B583-46F219D804D5}"/>
-    <hyperlink ref="X64" r:id="rId183" xr:uid="{D18B9D5E-05E1-49AD-8D43-0D1A92B5DFC2}"/>
-    <hyperlink ref="X51" r:id="rId184" xr:uid="{4C5BD6FA-A3E8-4947-9ACF-8D658A40CB8F}"/>
+    <hyperlink ref="S118" r:id="rId1" display="https://uc0c68e868d69f568916df4f9c30.previews.dropboxusercontent.com/p/thumb/ABdadMC-x1JdIQE6azcIAnUZxoHQfS7DLvWVp_TG-CYvSWhO7mxYUAWvRjLTvPNtwet5zTvcWxSHIqHZThrF7C7uNZFEA0bb9xnhn9NM4UXlMs4sN6yGwkjmTqKyMXkhedfseiT1h3FfQIeGHwND8N9_G1AoKryRlBL29SJbrQcb0VauWEaeAhy5wQS0ZKKN-VpGLv6jm64kByGsCxnxvPj_mE4zg94e071cAO-55WTXgYWj58gOwls9oFJy9uvBvgkEA2fktpI58AF5jVilDZNR4YJhNU4-UdgJdjZXwZQoZQCFNuGq-fidKh5bsPrUzBuUpX272pE61eOlaI7jCDRx5oEMWdqpvK_T0R7h2Ras8sK7UlGBst59CxFjQMi_nT9koBAHvtd7vexzlF0rWJXQAWtoJ1Z7cYdP6ijrMR0pow/p.jpeg" xr:uid="{08A3F25F-0414-4A0F-A719-72B022F2E356}"/>
+    <hyperlink ref="S116" r:id="rId2" display="https://uc18f08d002c9a613a28a0086fad.previews.dropboxusercontent.com/p/thumb/ABfd58-PPmiYUdNAlDEe6h_B6IiaQf-oEHlirhQvWpX-XKGSgCDDuDKtOoCxJOPRdu7xvqUL_erXsTKizY6z17GZL1x_teTKqjTEJZkaNxemRCKNT04YurJnLG2vu_M45BvRdKE2bQfFrkxkLmYjzPjlww8mnvF5xyEEotaHy8BjossG4W17EvII383240-B5YjOaDkrpQv04tHxXpNLNyGmPbes2icuc7oanqagd8eQzgrnL72v0qa4kpS7vkpZ4T5fHAiYrJlEWb73Fnm-S-oVKbfV72NuLw7tXv3Dq8SqSs1Y_rtdVVK6WiSj10iKMZw6ZVsvC4rk9DOAbGunSFGea9m20NOm4SxPS_Rp4jjD26BmgrhSHWG5i_D1LUS9tCqlA-VAOPIQFA4NR1IyGWrgQivItcfAAg2ox9luhuo2uQ/p.jpeg" xr:uid="{FA043706-2418-432F-B7FE-CD4917F577EF}"/>
+    <hyperlink ref="S115" r:id="rId3" display="https://uc9b2ddc0c78a7155fb0ed01917b.previews.dropboxusercontent.com/p/thumb/ABdEGLF7egd0G2pM5dX7AGfo5FHhA9z3-BeHeQ5MOL8t-21T0VP5sDaixagumCtk_MlBgdy_0tvf9MaX1YNQA7EABMowbeo-rHDQMw9VgpgKGD1xDY3bZhWOqbtQ738Spy4x19ptCkfO4Wwv43oW7XqBbFtm9Tm6sKDl-NBbrD7_4x7-Gh8fS8xiQfcME881MUrn7D66XfSMy22Tq94cFhoJ651n-QK0aojgxLnRs2_Ti0mEzcEqomrUfZhUvQ2XVBb9nXBP-hS9-adzeododwbM6rJhdyn7p-C5vhZbKcZ87E4JfOPqa6toQLyV-VjMSJXlDeRY-PoV1RTgfcj1JG0ntpZfDkGH156rOgqUYUQEmczkiSRIEkPaHEwia9v7BDNPXtd5pwLTOayDvO_jhv8-QaWnwEiF65Nr7rlEuooG1w/p.jpeg" xr:uid="{9B08E448-A33F-4876-8B2D-80E23B551D54}"/>
+    <hyperlink ref="S2" r:id="rId4" display="https://ucf31c780d390a8cb66bb83d4002.previews.dropboxusercontent.com/p/thumb/ABfvSNrt2wHEshyUXbzezFx4rof0ejdFSFgV3ucUEcHYVL-kJPI_XjqCFth0gVnM3YQubDyS-roI5UiHGWUlGdCKW-VnXe4KI91oEoshW90C4hhImFx2TtHAOVo7R4AwKeDgAcAEUK8_X0YkjUN4AsMmDgDSrbRVOBiK04A-ynnOGLBBXaG1tFVdQ5OAB3PE8VLgHWG_CzG8g6B56-dxta-Gi29OU39D_5qoi-rtnt2dKBmFDF_PMuetx6oKWUss1N_73rWo08JJvQoIeLFt81jphaZAaYnZwm-_77q0AwqJRnp2LZra6BNIYw73wgmKPju7be6iKMcq_CvfoXaNiTQ23b4Dv976oSxfKZPMVhribnnMLRaI829RwExIgvU1e98/p.jpeg" xr:uid="{42BCB43A-A740-4362-9343-018B8DAFFD31}"/>
+    <hyperlink ref="S114" r:id="rId5" display="https://uc589611219f1960daf2097896e7.previews.dropboxusercontent.com/p/thumb/ABcsSMMY8yQn0SebALghdta5kA1G93Hz_K9oAb4gsspClegxItpTOnrP5MbR57w8_pdOysunCj-_ajn0rZkPJfYxBM3tfxxJraj7vthDMtCFwxxk3OK3naNqM3jvSbwzz1TwdP9_b85G-ZsCaI66LO_bP62Hbgz9Whnt1ScO8enHCNi2GD2kvcZayYZ4qPmXVIcSeqZ-7Bq5H5C_hmruj7SFdypbNw4FP83tJ8nM8Lfjy-leBC5MKjaRRLDw9tsqmQBOVhFjFhMQWUfCH5I4Qif-b7FqEKG94zsMW7wwv1XNmis1cd83hjKaUSOdQ16ZczrRSgsiF4uVVaLiS5iI7OKAw5nbIP5fF9D8_DetkPmUsVM_j7rNP9QPcHHMmGtorLdid0eF9g9E5v7y18i9BzYtMiJbpx-k7Joit2OAmJxHvg/p.jpeg" xr:uid="{0D168D68-FFA1-4886-8A0B-DB218F59AE1C}"/>
+    <hyperlink ref="S113" r:id="rId6" display="https://uc49fa0cbdb0be62073bcd6f37ec.previews.dropboxusercontent.com/p/thumb/ABf1Kpuxlbn7Dhd1H6AA0ahGqFH0aBb-uk7Vhpg4P3HihaiexEvfZo1mKOs20Fp0OVN8Q3llsC0_XnNU94t5oWA-c3hXGhmBYo5HHPRzyt3LXmd5myqUdXosEC4wrWVkzLcz2aIHTeR2-WKlK9V0LCiucUmU2kKA9EXnlYdJJ0AUmc91BDWXB-7rewc4qy9483DUOZPizK3DL91m7pGct7oMW51fIReNeJ4-ebMMt3PrVr3A5-P-EEQ84FmvQJfVRzRxOODyhpaCEFDI6MS9_wsplbW5W4ZAk5tKKk822uVfZZBevrp2F0BvgDim9LpDVhkitvEjLxMPO3c6f1LpLi1iJKy56WAdNH5aOQskOXcm4s1OBlQwIzU-7su3t6xEn93jGMlIGHLfNx0IPvCCKi6Ci78EjszHJnq8JdBQ4v5QFw/p.jpeg" xr:uid="{C22B599C-F442-4501-A9F9-6A8400F6172C}"/>
+    <hyperlink ref="S112" r:id="rId7" display="https://uc468eb4491bea3902454a023f08.previews.dropboxusercontent.com/p/thumb/ABcCz1iBA6elQb5edj2fL_x9MUyPj2UJ6wglAaeZ8mB0Zq9byVrsSwOzSjoRrGcciZ6vFx1BWrdAbpAzUgfrx1FYKulqaMpwdpMvU7HIyB-SVotjad5RxEXqGuh2Z_ohPXVZbttSdVaf0fsU8IFiHo110O3cWrX13ZF6VNT_NJgkRPiqosJvLfmKx-vqe6JXF7gEaseB-hOEDTFwWtbwXUQylqz4GIR61YHyEHbdWLWxBJ3MbUIsZCKa2VygdD5hSRwfK43g3biT3L9PZDujVlZgVo7CAxQOpkNw7UXgruTJjYndQwAyWkqEGe-nPpDxhtcbFGUUddOspw-_g19NeXk5I2o2qtnUxDmzRiVqKbswps12B_4dpeH0JKObFJnQvZ544l8S_IDRpAlDkrUeDkVYv-C4oUeasN-sgQAkPw7-5A/p.jpeg" xr:uid="{0F8FF7E4-C11D-43EB-A495-B509DB231213}"/>
+    <hyperlink ref="S109" r:id="rId8" display="https://uc7e58b0df394520ffb96a31b712.previews.dropboxusercontent.com/p/thumb/ABcgkRnFag0DXx0Tnjz_7wga1u9AmYLrMBNGmPROP8pu9NU0LZ0TD8dCEH6iuZsvmWUlyFx08hjXGJ-lUEWl_E4be0xivy5qDGHI-w6sxEbN6BaiHHhVdSw_mB5ObS-tES6kj2zDK5MfWUwgFhSub8qJ-YXynF4ltFsnxemxiulknjGzspsVyuyk89dclXz90pjZ-g0dlTLz6DgYoInb_WBhZcnIWjrwgMCTllM-1Jh9YyZ_Pu561dmnHESg6Jr3gLIcXbRpvZcx1HBsJshpsIcbfAQ8eBNg-iKPinio7VpXJma5HDEwekDRPtjC1FXeW8Z04TioftDh0SDStNavOzfAwHl6rhpz3O5U4nGu-96H6uJHToM1FWspqicnv87VPRBmkaKDiMR-bCjSmjH8t3hzeTDZSIZxWKpYU7wa-oWTsQ/p.jpeg" xr:uid="{459A5495-4787-4D8F-B703-4AFBBD4034D8}"/>
+    <hyperlink ref="S108" r:id="rId9" display="https://ucc3f474c2861fb01650641440dc.previews.dropboxusercontent.com/p/thumb/ABcHtE7dOTUZJkWRd_6zz9qXsxHQf4_0ubdFjeNJdTMVr4hsdGkmDc5NweRXSgsFAPD_aAiKeeus4RaLNW7CCdMaHMxskCaSyZve2r_DAQT9opYKoRo5gPHL3mBhwcz1BTnSNR6uVqwiQ4GndVoZjaNm6OC3A_xnyLY9MZvfN7nKns66ufXhzTM1q4oyFxXxlCFG6VUZLwDX3GormtTj_0KCEXEwmxVRCyLmyYLzVw-uDx29tTgG1TwGH5c4lEv21kxJGtoruY0tENqfUUz4M0IzM5zH3p5fyrcqU2gKT-23MGi_CgdTtwT9MHF8G2cvkaMM0LInIloson-Qu5ZKp5k-ebPWXYiqAatPFIb6kTWyaNR1NvWQ-wyK3sOCEX5gNWGsjR0xmsgNoabu7-ZeWWTlfUoEAm0ghcuDv1pklw6z5Q/p.jpeg" xr:uid="{C330ABE3-972D-4081-AAC3-C63501B0F5C2}"/>
+    <hyperlink ref="S107" r:id="rId10" display="https://uc214cd81079fa3f5be4ee0e0fdb.previews.dropboxusercontent.com/p/thumb/ABc2cU7FcMIc31ShVHnOM8Sf7TKr35brVrCwYH4-mbALsQxhL5g1u-qJbYtnNCa57eyTqKo8TWOQGd3lEhmdJYwfSJKgUBAmUwlVOioksNoNlUj82WHG6JdihgVfUR4nFtOI08nCBJ_UOia4-bfChHt3VfBwbXtP76etO5JiJjBJpvJ5ab_bnABbSdLMJYiTtdpm8lkCfjifWQhxqZcLMjdhmFrqg4p8fpK4Ip_mIGxz3DX19aK8idMyy0hcAZr49EMa45sJ5Y1ZaMOXIYM_eDRGXoPfRgGSgvgbMzh1o-PPoIEDcvnkp12txpvB-h72AdmJhZFNtJNLo729M4ySQ-d1hc9qjZ8f1yb6tCVBLrVgaVyacoy9V4InNcw8mHPmJ_IkzxvF6lXkxD1vR5bulWNgayGBGsTfgdMIpro41SNW8w/p.jpeg" xr:uid="{5277B38A-204B-4B87-9040-A744AFC25530}"/>
+    <hyperlink ref="S106" r:id="rId11" display="https://uca556c15aacf9c2baf478338fc7.previews.dropboxusercontent.com/p/thumb/ABd0UCMWdNhEgmzdJ3-vL3p79Rt3CLIYmTJ7a-va9Ptz4LYEIgLJ2XZiCi1CgI01vdmYE1RiafNJaJdkO3dK10s0h5BiGf-H5Z-fx0YRmQqLNPClgrTY_EHrZ7j2DT5clyM6NBrTmnwQMZSWepx6mjsFW16XriLSZYnxor9Lrj8CX2LYh6iK88IzMRkxKGjMvK-eD32xLbOHxzzzBoFeJnEmSPpN0jx7xMqbzMCuzdZczuwepfK2yavxHWUxjmrXUxky59F7gGhUTrUr-JYfPCQp7zIKVS-06qgYzt6G1lumzNnHtTI0xRVgqKdhIzSHSdY87kmMcsIv0zmPb6bnzwbap_nKHkBZYHqFAiNNNpuymCy14anOYkrZKKMtvSAg7r1YqnxCwVdBMz6AdDUmehcGvzOhp15wBqimlsiV6RIw5Q/p.jpeg" xr:uid="{6ED5A6FC-2B11-4300-AF1C-41821F8AB203}"/>
+    <hyperlink ref="S104" r:id="rId12" display="https://uc940cf153674f0ce4aefd03eeca.previews.dropboxusercontent.com/p/thumb/ABe9r_X4Q8puGuNyktisc-OtZjdiygrZzSvPlWEpSef9P0zU_aZjAhC-6YjGqlJO74kluz-uhMTaFWfcX3tMT2yjqqAuUaN1dDPs5HM6T8iUt-buoIdnGrHf31HtzS_3otRNdNXtoFOwTVrpbNItHGg7a8AInPEi2lmHEA5EwO-WRCzL5Yu328rVeAFKnjdVKZaDK3Ea0aaDM_FEgltUPQp7UtfSz7U_KOLiwsngvW2BURdU1p4TkC5nHkfdJXpZdLgsO1_uNIBM_Dmcl3tBRfH_0Sd-1lAmlA5Ki4CfT2gfTVDRuX1Qjm38OefRiyi0iiey3i4QpAor3bMYkymVHVAqB1Zdg7yw1YzeunMJBSAiqQ9j-Zpqfu12uGNMRIVkYCUWW1CoNCaPjAMV7eCTIADtJdHngFqG-MFnA49yN6zvAw/p.jpeg" xr:uid="{2F7B420F-24FC-4CCA-8AEA-29E61AF1ECD6}"/>
+    <hyperlink ref="S103" r:id="rId13" display="https://uc24ee82e6b0dd0b3f1a452135ac.previews.dropboxusercontent.com/p/thumb/ABdwNaEKHKUmrs0LphOhNJCwnhiGqTmBDsZPYFp_sLo3WsQWVk-_ZuFH-uRGsNHhgfHau73xC8xngYWnSvajBnj9hzVO2kqEw2F2Igm2V8QXPqb11eHOiT2i9LCdNOxp91Xupa4MnOab7jZqzhjFDkNfTU28Kp7g1-GcxxzScYcslI8dIUeK6Jaip39Y1ES-JxUnynLKgBJmzMFoHU8um6mjTBm9vZiOsdUFRO4a8JY0iqx96Du2_7rg2S3vto3Zx2nkEtkIZiN6rSIq-xt-7CyPOwutJ4F6lGDTDJNwLgvXflhSlpbph1wfIboVyo0kFbAf2Nt6UBo452CSs7CJ5dVO-A18LC6jt6ufg4O8EEIRMmB7TPU7x7VTnhAuJh7Q1h1iglNn6vGrrsvbwjgE5iWVxEXlDaVjnQLouXJ_Z5kR8w/p.jpeg" xr:uid="{0308509F-1F94-49E7-A457-BA1A2A654AB9}"/>
+    <hyperlink ref="S102" r:id="rId14" display="https://uc561b3ba606cb2a8e43f284220c.previews.dropboxusercontent.com/p/thumb/ABc5kFfI1d6Rr09uwi4UpPZ1HHBk-n1A8yCctr7gv1E_wk63KfT8nBu-JsUsAbgq_Pet0REKr51ixL0qyCRS0FulRc2ldfLl4yGHovv4aTDao4mpBRW03LWSQMuOgLLHi5hyfZKrbdgLbd6LkxswOM4S4I9WRaHenc4ZuZojgaA2TE0IIPlwaHoQgm_uQlCb5Isfshu_jksD8K94TXjarfpcjjbVbOZEyT5svUc9p5NsvPRcvK69O9w0WQJBS9PJlJLMq2CyDmfcDJt-2adrVGkOJD9D_TW5wyCbKipSbnos8w8bzjPDMX6eZix_MR0wHT3FoY9Dj0kSCnItW8lXSzPYwmGsYeHloho8NnpXZT_D0xy2UdhACKOQw3iTGCJCANFrGNvwEW2zmYPQjmOVmB35mBqfQOhsu1xpckn7aqkbxw/p.jpeg" xr:uid="{1DF4DD8D-5377-4193-AE41-2B8277ACBDEB}"/>
+    <hyperlink ref="S101" r:id="rId15" display="https://uc7cbaa023146e7d14fc365bf5fd.previews.dropboxusercontent.com/p/thumb/ABfwTQkaNioWE1_B5dKGm7WWjXQspOw0CJFvSL0A9t8yVQHOFuTwyUvxahluqW7llo_iB-6TJEhZGWnIuGiE70J7j_A7MEzZNs0V5KrP_NrcuPlkyA0Yy7Cr_sVo_b_O6c1RYJnEEHFcA3QDgzYrptgnc7_w3nxukkN412DDKouFvuJ561-R7drOexSwwA8hB6FWRVi9f7O6fugIGsY2Ss8rzsOtDVA6EvEiK_Ykjl3xEK3YoP_Hhn9tUDOCz9PchhA688AH-kn3rqQKWgJd8JRssWJFeP9_PFFfmLdy352e6UCqEqooAu2sxo5ijrgu8rspYt38SGy8MOPtjcCwvimHwuvoIJosHrUd3IyziBDJv5iFj_1WQOXpJ0EEPUb9dB1i_3fMMeLe0oOmdGc5OPBmn2LWr2Z-CWK0n8Qbkm9x8g/p.jpeg" xr:uid="{A0AD95C2-9571-47B5-B12F-F459C414E925}"/>
+    <hyperlink ref="S100" r:id="rId16" display="https://uc0450cdde5830db8d628e12afa1.previews.dropboxusercontent.com/p/thumb/ABeLYrLuMZxMKXbR7rHoBxX_pqEPJ-q1cn6adAb-qINNp-4JrioC-FDLhQqzNriEr-hkgzONFVdFBD3dM_PTX9Tf3FbNWMB5ZeYxItSuNEGs-zA8Fdwma0if8mTcxdCQRZzIWx4s8Qoke1hw9TX1fCclSzUnRfi6BBCbhuqmx1vzDX5ykDTri3X34P43R4acMZZ1JeqZ2ZDMMK51paT3SgNQZrGDTNH19A9Ftba4Cah41YPZA-oVUXL57HNpsPMrNodnTGsyE1zb2zj-lHokTmJvxHZBgqjwmukBJjzpi34bM9cuWIdr7vY-xtWd-KPGN3G6HkRHM5GUawllUYYvkdsLSnXgbh54tf8PmcYG818EtrL63kX4VauW18YfVH8xviu5GTs1gNLHQAsk6JlAG5npe8euvhjv94hNyPAsSRvZ1g/p.jpeg" xr:uid="{F9288155-8FF7-4E08-8181-3714D1F4AAE5}"/>
+    <hyperlink ref="S99" r:id="rId17" display="https://uccc3a26dca8001df60984dd46e0.previews.dropboxusercontent.com/p/thumb/ABdHyIJdJWfVK1QfIBOTkE6g1iw-P41KDeuYrpTaWVKyvIogoBI1-NcnCOQczF8FjGGWqrb66vAlS3n1WfRNJi8U3QsBDg7BtO9m6k4cq3Igq0rQH-IT1gy6_2V9x_vCUsAc4VjWqETZWUoJQHTluLek_lCcwhzaxCSmYsg4Y5uVsMnzbVYW4Z2gq202hfULKV2TZJ65HIVg0930WeAU8QqDaS13f1k_-CT9Tt43Ze-ul27oEq9LiJC7gJaRwMUYylBfhd6bejvt6A7eK8yU6GjXG-xlGHBOViI9FwXmUyvihKzNOcTv0Lnr6rrB-bXW2mH5CSnVPeETILpNg--0PkZ5ODm22IO4HP0iorBdniRqehpvKFpte6sdUB0msVJVYtOVyjQn_uiYnIWwcIq5KUpY3j8rLOlq7dblJISc6Gi7qQ/p.jpeg" xr:uid="{46D99794-CF13-4DCB-B26D-67035C8C2141}"/>
+    <hyperlink ref="S97" r:id="rId18" display="https://uc7e90520245e3c6974300e8e7cf.previews.dropboxusercontent.com/p/thumb/ABfQJwjz0ndBca77lwbHjTw6CXW7n34JlZYOK-2NLX13NKEdVQuOlqcf_jCFl21M1y0D-JGoB14nnI_XWv4OjzaoW64dpHwAADKrMW3imdPjapxQCIswFqqO03PDsDYNihEjp0krNKZ9bt6kDfrpBcSpgWrX7fbpWx8xAbYLnioZht53R9AgAbBQmwnfHmz-U-zQq0LTrE2jVMIsFelQVxaGjtLcIe8oLznIL97KHSGEfh_jh-2M_XeXbH7OaF0ywA6WPtbk_XH8gwRqaI3ls30DSS7_FdqcZzCZuC5zwQBtPh7IINEOrnFFZPhKwgvCleRZ0EiHKP6-cHlyRUwjV7g7sQPcM_Fe0uMqX-RRQgvC53kVzrKLXwq0NSPv9iXC0wvMJ6RmGxt8i-g3oj_RCEaoZgdycE1rfgiMtsXN5EnGwA/p.jpeg" xr:uid="{BCEC2863-A25D-454A-A7DD-050F6C31238C}"/>
+    <hyperlink ref="S96" r:id="rId19" display="https://uc74fba5b81091e184fb23167601.previews.dropboxusercontent.com/p/thumb/ABfG-qciPGtY3e4C91HIEHOtHDxP3gSugijkd-ZWYfbg5hFRpvDbxJSMsf7Vai1fYhUX0By4t4aiZWZi67x4iq-vE30dYCMhlrLPgE_1GkmHqTfIV_hK2vwgosycysm7sZ1FH_atnsnlALqQ9MEyVMnqvNHm64WlQilZqqP1FAXAKHh85VE1wiXQb2CNqVqIk7XZhDvlsShsQqhw3TmOBM2GnkB_QquayV3TrrcQFYHAHDJYx2lmovJOpX-0wTBw3pqSbkttXtY7PVlBrcO1kgIDaTXTlEBjiMTXaIksApjuKgui6sPTjB2EYA7E0cbKR2ZUNvZjJD67WgS11vmISZgV7sw1sLt6WbhreFoUPWDfRNEZRQpPAiGuOZlYIs3j4VkqpClm_oprTkS3BdzolZGr1eckzWGfPVmBCBnDLALs1A/p.jpeg" xr:uid="{23DDFA23-4E47-4469-B38E-BDC9BAE646A2}"/>
+    <hyperlink ref="S95" r:id="rId20" display="https://uc8bd7896662a8fbe079bbcb02c5.previews.dropboxusercontent.com/p/thumb/ABfbKWCtZazIAAxFUR-JbHcmfj8bJBKRb5UkRTEaiaHdSDKitydpPb4RL9cP9rBugCSum0XRqO2Xbd34gd_g64pSYH9oSjw9MT03AqHU8-wr63kO8r86ba2TM77IgAK9cb0Kb4m8f1SgSiO1iP1KoNEUsfAX55oEfMccTBU2za5KmfX1LhwFQrl6-zRoeAxWmynC-5dJlAli0COpKn9eQe2eGlvhAXhweOVJFMiMPrIp4rDeUJRSVHQXzGQ1A03sAxsDbNG0eDOWYf9OKXvwCXMT1ig7iqLGxvD-UYA4tJdd2ZmEJWIqR0ZpFHJrWbCVVDyNCyzmdiy8Nii9VdBEdtidRwTvgY-fJrND-tzP2FEiZJU4eVZXPGHumGQLrBsKf9K6NM9KJnngJsVwwBCPSjsqqeQ8IYxllnMqTFUGg6NPKQ/p.jpeg" xr:uid="{B267C1DE-294D-442D-954D-0CB23BF7FE57}"/>
+    <hyperlink ref="S91" r:id="rId21" display="https://uc96b9aff1e347771330ddb7d5d5.previews.dropboxusercontent.com/p/thumb/ABcrKpRblMJ1LAhez72-JeBwtjwp8tLEUgy6Rwe9Hr21TIe38GAcD5PsvdTPNWSDYWIcuqt-4_JQEXQd4Uv9IbPBFY-52NnzuKW7NY2Zh9GwaQbB4ydnJgqM_bB2dltIBH3mf_XX3x3a4NWwjLICcegFnVtmmLYm630PxQ7rAnkI5QlGmNvHsn6Fo4bZzqTogolXvArSx3sGr6AO6FCdzqh2jv34YMIvbD2fIIOpR7HXIDwDIRrfZOHuqzejnuS32-miv5uUNkoGF-5fH08kE5e3dxQ7O20urvKJkrnf7U2Wow9C37K1IQAcEIFBzjHvdQHyzyPSABE7IiIb8qVQ3VLMeiEa67oAVzlMsfdOsAuZLVa9KM4W1DuFHZw_-7-_DgylXnd9jRRau8WTkc5STI8ZfGFKWAuXZqHnQLr_idG1hQ/p.jpeg" xr:uid="{684E1A62-CE22-4299-8956-8EB927260FF8}"/>
+    <hyperlink ref="S89" r:id="rId22" display="https://ucd000e2a95820e6afc400d76825.previews.dropboxusercontent.com/p/thumb/ABdjM1ehD_u320U9zM9FDKMtdLF9q9S2pVERjmoLxjcHn1bM8tqIWo8GpCHkEL2uvKbtsEcR38nLKmWF_E2awuqfCrAp6jHHS46M8S8iL0NpzkA-u5aTGkXEke4zyoxQFpLainG1afM5N_Cwm7YAZBYSL0g8EpyaESDbdsa39If2luFE5l39puCJ4_bBb8AqYOvqUjCF0xhGLmZv7wD9a4XW5JhofsXGs8stQMM1Z0jkUEjylpNZ6sVTYEhyQDSE_-aP8WQZkBR7T21hEwF8S1sRdVc_z-_50nACvjFe3D_eF9JIPOun54ExtLSU6q6rinySL36N09xXDsbJyGylo2io6X3SXIW7clRhtSEPT4lTQwS9pfkPrYEePsUQnsCsfuXUkIcHeQR9nZs7deYIWU075GdsPT63TjjOKUpEafJ8hw/p.jpeg" xr:uid="{74DFAD5E-15A5-4F5D-A7DC-F051F4DB143B}"/>
+    <hyperlink ref="S88" r:id="rId23" display="https://uc39ace3b8238f7870dda6fe3546.previews.dropboxusercontent.com/p/thumb/ABeZbrg-gwG7sh_59zcmQ4WSVsPeU8sEKZ-K4MsurCtuxbVcTBIgFh_15o2F67B1q7SoX5El57eQ96-ntdLuvPiIeSkd4pvr8s39VPaioBmLGEiJoYiSzJu0n5PpInGidp35Ob-UHSdBykNp_g_g5H6i5JLd3F4SkQABSlttlygwi9dHqz7kYW2FBw-yd2dzD7Gf6diIpo6hopuHoCPDk6b2CI1TnKScF9Kp9r47f2x5FJA-ZK0_DT7u8lwD-cVBVRPYQnVs-nNiAURCnVPXhMJD0pkzPlDU8DjEQ3zYjka0n_bjYH35D669TVF_XeTvQlpp6kdgRRqXYS2qBOPdppRv_Y2asj3llI6vofRqGo85Gq8VZm7sGCo4Mq3l4GZ1mS-0CYKZb77ypSOhJ4mYUcP65TYk2S3AZjltvkivaNHIIA/p.jpeg" xr:uid="{B45807E6-7392-4AD2-9F08-022937B69378}"/>
+    <hyperlink ref="S87" r:id="rId24" display="https://ucb53aa7d567a677ff7621919f85.previews.dropboxusercontent.com/p/thumb/ABcRp9azTRbl07Aw7DfUmyJOaiF9j_siFqhDAYCal9_Ri2S9zXth_vxjNPendvdFlrZORvxVPeuBgbYj3Vng1dOHGtuw-pWkl5uZUfS7G_avlj-5xLVf368_R4FhAc-cjjwx8JcumFyNUA-FVSx4vzffdVv801d41POGYM-9gnUYKy6iysg5OsEebjmx43qJrrbazitMgUCQrrRt0H43m3EYjLzkQ4zrscwgfKxmQh_UT5x9lVOJTMyIE6C-viMDmLqQXcIUHkq_Dnjl7aCra7qxipj0Wpfzo9_CzhobygwvT8vkqswFh9mJIHHIyt54bue4UHdXBUnI0MQH1hMK6GZLN01tzlYNmClWe5ESFG7VDpuYkMiNkM0xUPVVWhum36Dc2OwsHEHbP4Mi_5GUexhM4IOOa9Lswq3Av_1O58-73Q/p.jpeg" xr:uid="{4D7DD7B5-1489-4282-86D7-96E75FFB7B63}"/>
+    <hyperlink ref="S86" r:id="rId25" display="https://uc4e9f43815ce453f6302cace789.previews.dropboxusercontent.com/p/thumb/ABeiv-O7IOLMwziwR6zBgbiKUsC92D-ktVaPoUM4UoKmpDchvtJnub4HAHt2NKgHgl-3Jsmc53-cgr3kB0ooRz1_yx0MtYSQqulAqjboUpkXrMSk9g0KqAVLpN8WNlGEuaaxU6VJfX9hz3xKSRow4Qd4sosWpWVU7fUaKMjby3pt8EXYkor7VoW7srpIJwzOS894xoRfO3_R7bXeH5hhwSAAkKVpUAuI9I7sdh9RZsD0HynTtr5dv9l_Lxk5egxdwPbV9NU4BPmGtje535lE4Om4qieDGMSycHF8CaOS_3ic3tM2FbhC6T5iznVHeIr7Gk97IsoKWPq47Fuv-T3ZGkPxYLxmzMJcHKbRytDxTVjibJBXtJ1mL9TL_qMXa8q8wEecwI-bIuPVom__hnQXMYFXOD2mGDqkS4VBUBUBdcitIg/p.jpeg" xr:uid="{E7E937AD-BBF5-4986-B89A-53E905853B98}"/>
+    <hyperlink ref="S85" r:id="rId26" display="https://ucee90d2ec2fcd89db947f4786ff.previews.dropboxusercontent.com/p/thumb/ABcEYrLFQ5tiU_cXBC_x660m-i2mbuVy9oNi8jPbXL7vx5Qvza2V-4x1MKrNfLVA3VdtybHgOC5fECT6f7BXzxBCz7iM7TI18dn2BkncCdxJLFUUsa9_QsxOzCoEnxI3ArkESr7JxI10mtkO24dqOZWXanX-33-ZkmFrjdLYOrt5zrs6W17kBC0hML_tKLcOeygbefF8YPswO2SvxHEvdOhPaIpQSQJEPWWy8FU6FjDUsRR-IiLTEjy5djdztd3CrrcLnTSZ0L-vRWedDQAayPR4GF-BZu7cc_8a6c2Dyi5o0NLI-gDAU1hjGOgRxJzsmss92RqiCT2LWws-wTmIXoGZUSPpOaI6mVtNBq2tYuasQ6dp87xEpx2DTDvYej68I1aCQgMdFyYsnchvETDpgfF01qMYhCDUKf3OOrQEJlYzTQ/p.jpeg" xr:uid="{FC6A2171-7CC2-4E0F-858C-D70AE62BCD49}"/>
+    <hyperlink ref="S84" r:id="rId27" display="https://uc8469c499b4878b9ba8a6a46aa1.previews.dropboxusercontent.com/p/thumb/ABf7mn6t39xyvDMWdhHGUJ8ZRHFtUFWi5BUieJMNa7pq8I1g7Gu2cyRMZJ6Vp9cLlo6Lqwt9yJdTqSeTHVuO8Ix-icIoz0d20XyTS2EsqpjwR6xSku_tYJP3s5wgM10_ljE5pjcLD-x-OjZmYoLXoYhR85L7UW6X0isoD-SzBRmrWSGCMTVjrwpo-DYwPVloLHfRqRNXBLvY90fEsVM6wmrjjQLsYyC8MLQ0f-ot6GuWgYLbQNuRgfRvc-pbJ_yaK-5JJewd0e1zl8geEGbj0aaC9Ve40OWf3_o3U9n8cnQIFjxAwSNf_YRTV0xIImtHEBHJjpitaewEKys6mGAOmMjdytBHWattQGUikO_u5w3UZNVSqW4benEHmaISoCncipNTyiN9jx5Ez5N4S8RE66xaGJZIidyMRnBMz-zT-Xj6JA/p.jpeg" xr:uid="{2AF5EBD7-1F31-431C-A2F0-F38F2CF2EAEF}"/>
+    <hyperlink ref="S83" r:id="rId28" display="https://uc29275d8d46bb13a1594645a0f5.previews.dropboxusercontent.com/p/thumb/ABfQEjwNklcgoQhRMZE_EUyzxzcj_q1HmnIclR3K7g5nuD_9SZ5WwdAQC4_-mjw8aP1Y9DBFCGIR5SVSLYVOE2ZF3-Gzf4y0zc9HR6XBbvy-zo72KOBp_4sKRTAIGO6jsh2ODxGWu32N-zjaRpukAlRR3wY4wxMErZgh7DfoTSEMbxfBhUHCnr9REtkJ2r8TjSdcSsYRJ54Ajkp4YNxbO3Y7nu01Mh1iufmY8VmGF8xAafJOFva_B8w-mBhVnRR1fHnnP8uW1R--_fKFxgbKhTLRkRSgFspf_jIQ-U63ht_vLxVbPoHJ3pIykGmOQT4w8xm5B-klR55rYCbq_-QriJsGkWvTlS4eR5JNYY4ntt2bKzjev05pvnYFKj_nrJanWbGCeHuXm42wpNR8akbfwzayCpw9m9uR0r2MASaBTSUr5Q/p.jpeg" xr:uid="{64863B1C-44EC-4D8B-9E8C-08CA16AAA5C5}"/>
+    <hyperlink ref="S82" r:id="rId29" display="https://uc21c0d12b07380bacad6c136c4c.previews.dropboxusercontent.com/p/thumb/ABef8aEkanJmpzSbx9kzrBCtjeQutvQvi2p_1xFVw92WTqRaw7XkECXgSjd34kocghctzYH5jWQGHjMDKVyl_5xLfVeNEOxpK3ZktPeD6epWfiKTlSldGhGHycSdOcNVfgdZzAAtM1bmFRIgdkuuDSckKbce2TM-W5Bu_bgsLCFLW4z5DcBJTtpEquxVrio0BTFE2OzdsAPTzprmhhQzDjWmqG-0QDH2lzXMY0QvFdVYjHyk_gZZhq_fAhdQ1AYDjRxhm_0b09z95lpCA6VgJM5YYol4x_uxuQKjPcTuiwz8nAAzKV_P25js2A-BBznbReeYCym7zZby-O1IVeQ70IOxXV0S55f4fBFi5BERB3x4q1ou15h-E7CE6XFTol1t-NEe6zvgstyjZjVMlB_cY05FtziJ173_UTptFvSAwGQjnQ/p.jpeg" xr:uid="{3C55DEBF-3646-48AA-9074-10179AE8018B}"/>
+    <hyperlink ref="S80" r:id="rId30" display="https://ucbc454bf97b12d7ceb293031874.previews.dropboxusercontent.com/p/thumb/ABejEvOrfugnqEOOcEyGcUm22-EILJ2zaSSFdhaRkYQAcn8ueCMXci5SxjyGzZkLwbSdsT38-vbtKnMTaDb0VR7tah3GD2PL2aATxLxJdNh7xmR2g-Wvjtfwo2tGoPfHNbW0vKKdCidL3nrq-0RufqtTs2rjXUwonsHlCx0YmQugIDNPFjJehAKZvmTQtRWaBfvHLa5a5UNM_F3jedcIKXMv-qs5XcwzFS0kIYtrZhsA58FD6Ov5MseY2cgIcrL4EIBpO0mzkjPrULXKmbyOthcKCB0Q3cJltK2RaJBs-creg7Nfzk7b_j9OI_1JtbIYdJSL_jb75cdEIUvMeVfNON3kkUZbNIyhUAo6gUauKas7rOYQtLxWgmeegqm0divORPwv8tU--JU06FOwC60oIyQoY6Ck2VkcUTD6ibZKR_o-1w/p.jpeg" xr:uid="{6C29BEEB-9380-4475-833C-4EC3C7791646}"/>
+    <hyperlink ref="S79" r:id="rId31" display="https://uce2b7795785b131a9a6b15b4b6c.previews.dropboxusercontent.com/p/thumb/ABdWPwp7XVja9_siOWp6A3EsFIDGBPyiTy93pj9ZuXiJFK910QOkliRPYzSdqCmArcJURZ9iEBnOlG2DT4DO4q26s2MtRWn3Cd3pKzYhAGZ3Q38YcnLfWwnVkXeuUeFvQNOWhKqfTzMxaympAP5nalOrwGFVmqrslXT9mC8lA_p0gh6f5J_mef6lrpKkOyS6Xzn3kiiPR1w9XUStt10cnH2HEduu_nS8WGv1Ov6HTSQvBiRxI0oY0e9zqxxzIms_BSu50DiISTIqZ-vSenmaTzGVty2fHYeTwrDFY7ng5GlWhyHQUF5AUUPX5OWa1KqKCXbViyga5ZSGJ62QXr4CFkG7ymR06kNNYQURiJdjyFoe7dq6F_tkrzFLFo7IN5o_oEmn24SRU2QFiov0gY2IjW32CcoVjV9kl7dAHwuoBk9jnw/p.jpeg" xr:uid="{F1A4DB3E-C837-46CD-8853-637CE70E4625}"/>
+    <hyperlink ref="S78" r:id="rId32" display="https://uc29275d8d46bb13a1594645a0f5.previews.dropboxusercontent.com/p/thumb/ABfQEjwNklcgoQhRMZE_EUyzxzcj_q1HmnIclR3K7g5nuD_9SZ5WwdAQC4_-mjw8aP1Y9DBFCGIR5SVSLYVOE2ZF3-Gzf4y0zc9HR6XBbvy-zo72KOBp_4sKRTAIGO6jsh2ODxGWu32N-zjaRpukAlRR3wY4wxMErZgh7DfoTSEMbxfBhUHCnr9REtkJ2r8TjSdcSsYRJ54Ajkp4YNxbO3Y7nu01Mh1iufmY8VmGF8xAafJOFva_B8w-mBhVnRR1fHnnP8uW1R--_fKFxgbKhTLRkRSgFspf_jIQ-U63ht_vLxVbPoHJ3pIykGmOQT4w8xm5B-klR55rYCbq_-QriJsGkWvTlS4eR5JNYY4ntt2bKzjev05pvnYFKj_nrJanWbGCeHuXm42wpNR8akbfwzayCpw9m9uR0r2MASaBTSUr5Q/p.jpeg" xr:uid="{D2D46AB3-F33E-42B3-AF6D-9CC5D7FE9DA7}"/>
+    <hyperlink ref="S77" r:id="rId33" display="https://uc788feaa3a8a2b39def5a66043e.previews.dropboxusercontent.com/p/thumb/ABdkZuoZ-OKV2d-EkXZlAU6-XX6qDOk63QBaNAzXEQGNJryviIG826oPvh66KRDyaTZvJiPKLJ9jwoAqG9zSAg1hbKMzhQJRU8bUU_JX8fjTbzN-3rjvMNNGWK6vaoNkWkxCvcxLNae11S242bYUBhvaKVT-tTTW3ZiBWSO0gLiL_x8LTzzP8v_A5tm_IkpbvJ-83OEjKVDbdrH9pitom_8DSrdwNqw92ZBlYM5Z_VE219dOWaNVHcNAgY5iPvezp-xeHj9H16qy6XzEamIZv9HginStARybbcXB3iUJN3Do9J_3WvwoIIW6YG5OdwQLlwb-LWVTxf8mrl_ABK99p_nhKb-T8WzHpwY3YLYz9RyqiZe57FVs8j_TX78hxOvvliBX9IU3mG4u6Ffi-rUKtuBvt1vUzZYBcgky_eLGmAijsg/p.jpeg" xr:uid="{6684545E-95B7-4D76-B123-007EC36D247C}"/>
+    <hyperlink ref="S76" r:id="rId34" display="https://ucc5ee67eec19705a1aa38e681bc.previews.dropboxusercontent.com/p/thumb/ABf0fZnYSwzeVbF_LH-KJA90rofrmSF-gM6aGDFrqwy7zRp9U772ygqHGU-Faouv10eyRb68Q-YyQzVtGrPeGQO0tp-FI0k7qKImzKfVypst6c1k4v4XiXjdqDtoUMYrGjDkCn1s0ADV-JkdK38o8coNuTghJoC7TaCcUztBvssEqnvWIJyk-SLhdhX2Tfvp-5QmtBnlT98NoUNS0Ag9uG88YGT7GntBejVCK7XjWfYrIJGMG8lghn8tFSaJlI7wqqpJ3E112lWeXCxE40bDOOLuIvXOlV_qjFfzcxZXyz_44LroXZyMtxrzAFLQRr6n_2KAGDb7YY0W6TnSGRQYfKkLo2xg4NTWi1YodU4Wq5hLB59QPd9eZMjx0QKUOVvdo0_HYiRUSwnAVAqutpzQ7He659CqBv70bKetuF3uB6FQ_A/p.jpeg" xr:uid="{9E89D255-5C13-4C5C-81FA-3B908D4FD707}"/>
+    <hyperlink ref="S75" r:id="rId35" display="https://ucffc5d1d3c28063252b38135a46.previews.dropboxusercontent.com/p/thumb/ABd8S709hRA9CtfqWfm9xZDyRWGDEXgAFOiC1xyTB1Z0yJ4KlmesqVmswB2NstQEK6LhzqShmeh5B5ZvNMYg3vEawPYo5XS8JcdkWHtOzb6zqEHsAEJ4yzG5NOuZezrVgHuiqQ1ntMFqP8wQ3VkWbQQmzvPTijO3KgrQo5PwIWBxzmK7g0AHTBB9-Tbrb0a6eFc_BPTnNq6WtaJjHt3TyI9i7MoyFOGJbSDtnZ9cFsrn3JxcSLZvKOhsyTO-sb4ZFpcEXufnGO5YuaX2DsVhDE_OAaQrBmNR2BVmt5R8RsjzdIJ14sc88M8wQswJPwGg9YsHJ1ZqMPvNVQgGJt_DEBU5fGqOc5bPZv7cCEUhSH82MrV8QZQB_6vq2WEGmTlRA2NVRec61djc3OccU-4WlQzNafzkq5m2jjM6SwICrdW09Q/p.jpeg" xr:uid="{5932A081-90C7-4C9E-8007-1735043537FC}"/>
+    <hyperlink ref="S73" r:id="rId36" display="https://uc83429968c20a3cc962d81543c5.previews.dropboxusercontent.com/p/thumb/ABfxmJEsKSkHKbCQuOWFGaJUHZzDebP1lzd4nvZ73ZPEyPPZyOtD0EWpoWIyG01NSg2JN_9eAaZjuYAm8rcOXRX_bUDw_T0lta6QQ0hb315P055bPhzmyVwT2FZNZbesa46nqGwxFkZffu9sr47_pY0qBXbyAY5aRM8QWetWM3MuZSoqTMly3X1O7Y-y2ywIwG_LcwaQaCZyTg-gM3-D44dtGHh65WboYM0R8oJJqbVy-gxmUw2qkwOTx086t--PazStvTTCM9Y8xUSU_3MpdGZYl2FGdIbn_kfKSGUHe8GRvIKBBgnYTI2CqLnk2R5iUMCllkgaWKuTZy61SU4EUkuBeQSOi8MuzOykRYWcinCAQ_fY5-fuEfQwcNLq5uEeN4Jd2uG6inmlX3o-cURRtYkQIFPK1zHu5RMeShXsxs02EQ/p.jpeg" xr:uid="{1D081D37-D3D6-4B6D-94E7-B150C41DB62E}"/>
+    <hyperlink ref="S72" r:id="rId37" display="https://uc7513b31a13f14f67ba48e8063d.previews.dropboxusercontent.com/p/thumb/ABed6XjhcDRDoXDMfIVjErksm_GhvHZVTcf2Ghc3LZAaTBCDal67pkj70NqxH19y6pjuvXYJxwfG8OTcVFDnVThfQ_y4u8ZIMBwCOqMpSikyOZu8K2kRDVOHHoOn-wYZ82ZKiGIn99c_8MIyJRi7Jkc4X3o8qHOmEslZATLYi42QtKo3DQ6XT2yBLQRHR1FShZESX9pnY1LUua_0OpjGuuHN3qUp4eV0y4k9NrCwJXxTgjp4Fd9cYOVQizU0qCzyJJsY7iKLaRvWph5TUL7mooXbCvKqQzKX_vVGAwYhtYBtlPPKsg4qtLfzUbUxLmkCRqWxy9g1Vb-3yMwPv7LQQrtTpXeuVjjCdSgmeYYDrTESa9OD7Ts86CuhxIz1OHkr8nQ8BH8riPQ2043WUGTyFz_CjQp8TUr54Nv4XIo7udS08w/p.jpeg" xr:uid="{D21EE40B-43F0-4267-ACCA-8410E8A90238}"/>
+    <hyperlink ref="S69" r:id="rId38" display="https://ucf9e4f04a38eddaa75371ce841a.previews.dropboxusercontent.com/p/thumb/ABfk_UYOLIgf_w2dxAXzDyqEjFn7C6JQPnfluWZzUCfwZB-TI2DZPWR2arFvigcaFpn35i2m4wL68VuSQmO60U8nEMiMvyNO2KTbjA6oJOt1Ozt1zTxrTc5Yk0qpSa_anktE1fWhhwprqPaThBxZUPMce7QJaRudPg52_7dcvMDQ1lHUVeu4GLY5x-lyhnTFsXUA53Rm4J_ituFipHzGGgt1lDD3Q9MA6HLMnlFRdl8-yGScTGohLeoTzDldSa6TnRWT2VrxmfzC3-Lw2qynb-7pqx52KosKxsAuvmf2Sk1HiiuTdyceeY7VOqyE5Ecqjf-gCgKvkxHWk5cMmB73t5f8tKCjhwnhbdbZiy_I1X-NoMRqZ8q51hTHbMVPIKY87qED3iVtbuU-8uhVht0qA0HOyGVY9WcDWGwjHpOMgTLUjg/p.jpeg" xr:uid="{3D8DCC6E-A185-4F3E-9CF0-523F4B53695D}"/>
+    <hyperlink ref="S67" r:id="rId39" display="https://uc3b2151db4e51f764f5f098b2b1.previews.dropboxusercontent.com/p/thumb/ABfE0fFqsUXHOB6ILGSY9BJXeHlJa7jNYNVXfl3Ifvjy7RQQnr_MEQ5o1RPRK6XSlKi3C7gNmIwF3cnVIwdnHQ9iQNilsoAnh8XWhXfZhdIgDlENbKPtu4B9KJVRxAMudXqWaNiA7JICgKyjbtmnuLGHxJMuc5QPaa58fpCmdsSfigzPUBn4hHxK5mBvQKbtcBQ2C12M7XGSP0iGN2c4qYa5CdhjuZLUfDo1YfFJG-gkJFB34Zz_m62t-AXdAzo0MddvI0gJwO7MG893NkjPLkCsYA8kVo5aWdmL-B7A2bAGSnyV-nfCBcXSM81pffW3PHuZR8nDFR3yuyOIxF7U1c1cY-QemPFJnqiYwQefIYBbtc1M7wt4MntOrCtEiRGzOlrQT9E-MjkA5O6Tv1szuBqwHzgWjFwxYpKlMxzm7Q94Yw/p.jpeg" xr:uid="{E2B468C6-38E2-4F50-B521-D7873935576C}"/>
+    <hyperlink ref="S66" r:id="rId40" display="https://uc868df3f7362fb41d16e17eec8c.previews.dropboxusercontent.com/p/thumb/ABeU7JGZKxbX-yq_Nv_T8MnKcWzWxSOqrxS2m9RFCCdbylPAXtpBO3EKnsvy_ycwljblQB9isyR_x68m3Q8lBVEUXlAg7YOAKA7P_haG-R2EOCePgoYWWqyl0IXwV5sZ4ezJ-WwpIUR1MgdOGyrdpOPiThkjt04lpAobOqVUIFeM4_GgeKwCZRdXY4uoOqnCAEeCYpdRKuurFJr5R9-PLhFRgV4Aae7JEtEXIDN5UqVjN4icZatYZfjiFqXjxc3UyJZdO6b8IEvXsYA77Fc9PX0yoCAC1iuWMTfzv8RBi2jbJ9eLaTsEadhPeZeBQTiozzg-KE3HOY2EOAk-_Ijt2kMD-zpwXoOeaMRR3T_zYGbyrBKfV6hvByxhB8AB-FIliCKJszAzpVbw0hlrBU-UY_aSQlYZ3A0MK8ze7MHF2R2xJQ/p.jpeg" xr:uid="{6A7AD920-F7E9-4B9C-A793-D35F4D695E6A}"/>
+    <hyperlink ref="S63" r:id="rId41" display="https://ucfd7523b16bcad4d01f1e2adbd7.previews.dropboxusercontent.com/p/thumb/ABeNL8tVlZ88lepY1u5lXFU5ocbfzmDCthEmuuYuyMUhRqIjAxVoNlOj5AMrX2cyfbrGcYQdHik25LzaS6HieLs2PSFuDBLN_g1PgBU2SSg5a2b1gInW6QRzIwphLwkA0EP2V4RssZaPEDLhQ3bx1bt8uceBPogmo4YCdh-m95RsP0FhdTiSqj8VVt-CNDy-6GvTlK10xDZkpufjoOF6yuoOj1bvq292NLRs9VnycMA1YSV_eZNlbHo94H0-hr3glqHzPJSqkzYhWp7CsmhTs50SZENEmzgXPqqjBkttIpm3SmjU2rvUpIGqsiGsyUErw7MBaKGn88UWi3e3nbXn7iCxlECQN9WyWVsNaHpiLJwVHBu5SOxPP-FF0UC6v25gD5NwChV3xrjyVEU3D1p0bfrQK8B_vtLPSg-NfETeGlPrLQ/p.jpeg" xr:uid="{27FE5FEC-D381-4D2E-BD24-B0A183EAC1D0}"/>
+    <hyperlink ref="S61" r:id="rId42" display="https://ucdf3a59536b5f7df87755759b8a.previews.dropboxusercontent.com/p/thumb/ABfC8hr1u13kCvZE9yONgSxQJJ_OOj3R9Ehii2qhaoKeFAkmDDw6S74H_notSlLTW5UknU00ECxUTHf1b4lqjLls3S2bI9Wdd4qkOODyOg4T_6PjMQY6zQYosld50s6uGsyTCWHyGCrjKwDYsKyIhcMdz3lgtqrDCQysh67hgbmkKp4VUkDNT9IgEwYDbtYg4I3PBBkvx6v1gbtzHpGt65KUI4Zm2AjiDkqK4QZadydVzPOZfAi8FJRkWQ6-ta1isyGDiYj_CqLWjFPIdDVQi7x-eTYH9mWilnCEB1u9BHQPvgUGv2XhwmrJVT6UcmK07v8JSk1Ac2AcYZq2nbvQKrJj-NDjtsLLo-IiidM3j3OAV9N6ND2wGyXoQqNeSSfmdHBBlpav-9WlLrYdwvxJSI4rhwnJVjk0T2dntLh7Vd6ulw/p.jpeg" xr:uid="{9F35053B-AFFE-47B5-A05D-216185E4DB51}"/>
+    <hyperlink ref="S62" r:id="rId43" display="https://uc7b0406223bf1daec0413cca967.previews.dropboxusercontent.com/p/thumb/ABdfMztxLH15j68nBwphpOaudt-KQehuDvZ_lIxW55GDQq5jKAntatU8nfDBLaKkTkIOCy-EKk6zbZfVvP-93hkYEOVKQ3zZYiJYA-OBwyDobkZbXH-_O2EQd8LY84HN_XgKTEn-9HSJyX622wS3zd7n9hm7sS4yk1w6dCkqq_HkqEHbGK1V9i22xhsElubbo9oI9OOpZfWU2gtcc1imtKXuvwe63FtCaVPRZZO9hNHBjWlKDjHjsu3CZatRzTfpWSHdKq28apCOGQ5uE5n9QLhRY7NBp8jHYMQc4BoN142RDsFQR7n9cc-vz0044gO090PwQ5mD2Kwo6nrXhAUzG79RalIcnzO3O1IywGPA0k7RlNvM4L-jqxRnKL7mq2CssbsECnJH1Bayb3FIwAozLISu3-BCAWOFU7YUIzdBJJReYg/p.jpeg" xr:uid="{B7BE9BE8-F682-4C1A-9B73-74956E1BFB50}"/>
+    <hyperlink ref="S60" r:id="rId44" display="https://uc3df08688d681b3b2e338c47b9d.previews.dropboxusercontent.com/p/thumb/ABfSQmyTVbrAy4ZCkFCFd5BxLUF9A1vB77IHVgc1cCjqA2W_m7IJJNzmS_h_UQ8gxfxBEJ1cUu7UzrVWGjdUKqtYa1A_1jcTi79NqH2jSepjyCQis3lPCWp5W8sFtPWxgXsigqAzyTN6MTlJTME6GTDc0y_3f0jn5IHfbgfRRJzn_ane9xOOQx2LtTuljRPwaYOzoIyvtkSh4GWZJ3sz8NA_hsxC9Gx4IwPK4sA_TkPxWfA-Yhatw9Okz2OX6sUmZRdKqge_lyvNzw7dQrReeGvlWIHEg80jUbayvtez1q4WDD22AOpQ64ZE9FYHVX5sb7yYcoJa-ZDj5jDQmIqLQiWejtIxS-DfaTfDtYkr032oOZrw0j_iO3msLaaeRsN9KFyFkIVqEuBFcC9Sh7p4_hlw1DIWDf4siM9OUZf9JT9AqA/p.jpeg" xr:uid="{8C51B5C6-E1F6-4F4D-B258-2E00C10F816D}"/>
+    <hyperlink ref="S59" r:id="rId45" display="https://uc30eec35611120bbb7c4913d0a1.previews.dropboxusercontent.com/p/thumb/ABdlzNu9zWpKNyZ8bLj7b1cBkB-qvd5IovokMHMDQrdgy6oQuRazxTRNv4QCtfRb0ia0QBbgXxbsGg4XwxyQ4l3CGVxfou7CxOZWemJnk1q8x_msQ8OClAy7Y7I_ANOJhByKTPRzpeltMrFrzCesCbn3qgb_TmX_i27eXjlK48SnGfeMWNQDvvV4-VnPBoiAM1VGOAlexn5fBV-GL6d-FztISgNt3W4-q14jQVst5lB5ivNPFOJpyCYqBbJ56pHlBjwmBJ4KFX8iomcbJCBGy1yfpMsxtXZos7M8YFz4--h5IpFP98-FuWCKdYpm2Ds5WuNbezjhAsux5TqMNTCd13vqV6LL2k3hG7inVmGT_k-vI_B1sbUe4TJ8trV8YEvPhfu3bsg4xoO7rYj6MMNfdh3yXpLhFkUhHql9wAjk5iUePA/p.jpeg" xr:uid="{36F4343C-DB8A-45A6-BBAC-0088882378A9}"/>
+    <hyperlink ref="S58" r:id="rId46" display="https://ucbf64dfc33a0d3f30fceb766e73.previews.dropboxusercontent.com/p/thumb/ABc0KNZ9jcREKi7dfJA7AJq8vlYHBjfzLpezZIOSIqIQ4ranqbWqOW1a4EQfKVhgE08W227vWrbVZgWAhzzp4BvF0f1Blzd7G-VveIzVaA2CrbJ_d69nDE7bt4Y17e2LNdCB88OANoSe7BVgjN5TeUf6xHyaI6mItxZ7YYmhCwZLw3lnOpvJhQwjageeOa64Ww8g7WKb5QS3SUj_xqbWDMAavwNxTJcOIr8axxykF2uYrPZ2cBwcf3P5ub6a71FdmMWt_jVXLjcB6EGv18EB0vpfzYq8LTAQkvPRc40NYqjMTi2yL_Ivt0rTrEHlwo9NQk7sj5Qo5xGXBeBCyicDhU77Nw0q7AOC3HhboDJ7vL55lXeVhwbD_bM80zX5xN9XPmSpnkG69kizRw7a0ugCxrnu-i4gdeKc7yQx1Tpm-tHGQA/p.jpeg" xr:uid="{820A12A8-022D-444D-981C-135311FD60C3}"/>
+    <hyperlink ref="S56" r:id="rId47" display="https://uc4b48c815b9eefb1571c0018181.previews.dropboxusercontent.com/p/thumb/ABeMJXnmSi5Dd6xaeeeKDrZB7akeJOY9tH7ZiUy70zr3RWc1fcIA9Dj02AkLsMlRi_M7kLeLK4YMcOh47HOYl142lfTMZBryzO8X7Walol4I2CNf3rfONH2WWfXynLALaRn6WmzB1Ji3SKG4F3YWQvW8eN-C5mXfs4yoyNan2LqPCzefqA_cn3ZPpzzUeuUXPpqz25ZN3UAaC9YKMxEAOdUr2J66ixtYpR8XphxDiilhHfiaHYimIIAAKTjM53U1gBQWBNJihM-TX-rcbZg-UOMz5S5rdUlIzC5Eq8NY5bBUfZj8rFTVcJTcqtJJMA_rIsZ9YWDavS7J9TNSKrhOhdxPDCi06i7pfY0ScKTFi9t41m6KWVz-Xj84ijVgHgYTeCTfkOB0z4eoFTGpQ6qNxC_bnR45yWGcQPy8aYLRLUB4IA/p.jpeg" xr:uid="{EE1E2092-AC87-468B-8185-F8CC3AACACE4}"/>
+    <hyperlink ref="S1" r:id="rId48" display="https://uc473ab1d3f024f3cbbf33edbd68.previews.dropboxusercontent.com/p/thumb/ABd35-HlKek3gYJfW_-58F--BG8ejvOla5SfBjpI3pp4JgnezXwiHyrKTOkc1XZE7R7M3wnT5VrsO3ZpV7esgIbu9F_uT1sE8XUfhESBUDx-Aocld0ab_UwEPmwM6EnA-vRVepgtGjLdWctheSViJtbXYEgnAbcVFNtV4xVXMYZGnbRe-GMOgbcudYMEe7osbUBpB_ArSTyGTNJyGeHLJF6jStD02dzStybiWaTmTus81lBPVDw71XTFkp-xplaSAP1OD4KYRJLWwjLioHbpfNf4Jh7TTMqRpHABZ8kr_KM3fYIUTX4I5kwk3rHe1Ic9EAdvCDtBdyuFP-po2IlEMDaSSmHjUVacAsHqrVVLJTQrabv_i2BaybDIiuLNRAZFrkk/p.jpeg" xr:uid="{9ECB1404-B45D-4AFC-816E-26036A3FCBBB}"/>
+    <hyperlink ref="S11" r:id="rId49" display="https://uc92cb6266affa5d3e9769dcf1fd.previews.dropboxusercontent.com/p/thumb/ABfY7l0ZYU4UOMjp5GsNhGoADEAoEL31Bp1kstAHTajUhWLGAk2tZym_3p8p2JFeFpvu3TeZccqkc0FCQsdFQNOMGhuu5_qwQgkNfeUH0ZcHCbHYWy7aTdR1bhKD7o-zWQq48ExkiI2qBqGS-oND0PRqAdCkpudaU23sL0qdha87_Q0ErZ0Wn5biWboy3JO11oUSSq87QTtCsuk3WRoy8i3hsWpXcTv-BavmQFbQw3YBeB6wigzCBxQ0fGOei1b5ZQUQSIgZikApkLs3TLmk4I1oqdiHnQMWV_eek3-o2dAIrF4XngHKhmw0qBpMAf1qIF3m9JcSj1vmihNqNkWR-mUz1zWUJALVtydoVINXTaJanN9pYETdvelkzfeMusS4Z0E/p.jpeg" xr:uid="{33D3FA1D-DC37-4FDF-A096-69C2D2324395}"/>
+    <hyperlink ref="S10" r:id="rId50" display="https://ucaef174f583543ab756e8ff877a.previews.dropboxusercontent.com/p/thumb/ABcXBicarpH7Of3YzUoWYdgdDRi4ZjzIk0YN5dLOaxy5nUjiPbMJEGOgWmOKSmfOXdYBLyuaKe-P5xF9POuBSOa_vI0RHyz_FaZzy9dGWeJa7vtz-pL8xX46EJYqz4o6KMLIDCW7e_n5d5SsKixonXnNhMybyS1jXJcH3BT9-t2c72xb2nS-rPMgP9YuP4YuW1g3lSxTG9JuHOzm3PJGR59ne7SZaeIZFLR9aAWj2PUZm8-sKyGSwznXyAvtmnbmnaC5B_SeZBfC2_WZi9ksFS7-xIHeMqv-dK-3J0ADC3IRy1lmvWmfirxltdEZnZshLbDpo5RslmHL0w2KNyNJXByN9j856Oy6eg84Df7L5IxXdOR8ax0ozB573N9UM_f9pNs/p.jpeg" xr:uid="{EC53894E-6532-4B09-861D-B6EE7DC6A583}"/>
+    <hyperlink ref="S9" r:id="rId51" display="https://uced6fd332230c3bf19d74637d1d.previews.dropboxusercontent.com/p/thumb/ABf-baCszaI5sdiapyAmAQj_wSZ8FROmDkmx2iOa2LQc_8IuKJguxLllpUc5KGbgUABdwPYkTGmjpZ3WisvoXMFNH69QZSxI_aE2bLfvZMJIG2EisIouZX9B9N0l0uWeStisI8tU0byxJG0o3AiF-_vgLBA4Za59rJeBdDZsElPeJ56nHtg68sXXU1TXucwIR3mpe89lTj5ni3h4a8psOA7XORzsOYNI8gvcteIue0jxISZWWU91oV3ofDpa9zd8OPV3OqHNDe78EPDYA_YQawKUT7tNZ_xCTCYLYwCRGeW2lCe466tAC2YXPvmq9M3udpXLRrB1RJnoMm5HGFaB7UVfsmcTVWJMrA0tY0p_d04ZwqpAc9KgwMM293oNDQ-EIRM/p.jpeg" xr:uid="{9CDDFEA1-8012-4701-BAC5-2D7225E170F5}"/>
+    <hyperlink ref="S8" r:id="rId52" display="https://uccf4644f81a66fceaf58e01db71.previews.dropboxusercontent.com/p/thumb/ABcywBm5eEC3iAqGI_6-2zXII7af5ArFqPZuJZs48yenhrrXzfvhOjEyDyWKFb6UZ8P6NqaWkcZqj8YVwOkFo_7MPdaw8u_AmzOV1ig_rbycO_k9PM7zOPEg6jMMRbqK4QJlJAph3g-e06jTT78vUjJzlsuQelTCjhmxyG8UskvZWZa4rsiae041QdACjWVky1IL2hQ7KGQpE2zpV-YrcZJj2Fo8EsdWD8UfNuwR_58dx3D9tg5TMwzPAVe5VxxuH0m2GBeCmIqMlG20fXEKBskDdTCRN2Nn4e56G7waRsLrqPauFVfVUS9BpV3sUgzMnm86yWAE019rBoA7K4bUB3ew0BVIfNpnKpkKLkXAE9Q3-8A0dQHhEhNh7LX9iMxzemE/p.jpeg" xr:uid="{4B3F45E0-42DF-4E9E-9C80-2F0C3EEEBAF8}"/>
+    <hyperlink ref="S7" r:id="rId53" display="https://uc860f724763eb5cb06b9d45f458.previews.dropboxusercontent.com/p/thumb/ABcC8X7UzVhvtB-LBC2rlqTQnbeOUXNe1CoJITGDdA-xReaPCK7GatDcmrGcRxBDKFLt4y3kk2F7bomW-OQx8b7gNC_dR3oiBreV6wrlNR0f8NygS-Sp1C6f5jBHIU1aMJvmRM4LdgKo5rMbImq3aC9zhcvN7r5wokaD0lkUH6lx9ENa01N7o9PeMcseP03BWOCzXFhht6MAmNsll1E7g_46oL6-u5l5J9NEAV7bz_8FcLbAgEjzONS2u_and9Gy7TC5Jt7jUxJ09vpFJVDgflCR7Xki8c7V-MBYupKfDQb_4x7xpylg1dtwjAkVkSg65FXiVEQMG8l0KmPHJhoxe557N-Gh1fS2r45ijMOsMD00caH4DZUUVu1y92mS_5M_VaU/p.jpeg" xr:uid="{EC8768B4-E6BE-40DD-9C77-E3A425D4B0FB}"/>
+    <hyperlink ref="S6" r:id="rId54" display="https://uc1320008bc34c5317b6b1822d2a.previews.dropboxusercontent.com/p/thumb/ABfhKXlBCJDrVdSiBn1Qh-c_4QMP7ztUIk6Q3WH5YOHS_sAEQnCNKfyS3IBf4kQIU7UabqN0xeJp8mfu4DzWanZVwG8Xr_-GR7VSZjnNMuhex7RucKykl4BtAfOez2kpZYuX0y6IyY4RoxSGcncCjnGKguFAsfy9DN6NjNnv80fGtEABFGYk2x59mjAgStzGaGPnwL0SN0UeblOgSsGPN-hzwlJPGvByuOFcKyMbpyGLrPpy1DTUh1Fsfcno8KBytzPTsdMvNnaNprrUbJ97SOegiH9SrxrOKrtACWB_1s-4A8HlhqPNPUMNkQM0g6VswNMpJBT1uxFuuZATsVbRf_NMkdWc6h2qykTDPtHymBuSRm3zKxIRmWN9CuOVxCa8A4Y/p.jpeg" xr:uid="{60261B18-2BCC-49FD-88BE-A28704D0A89F}"/>
+    <hyperlink ref="S4" r:id="rId55" display="https://ucc148df5b06313032c7e0f97ef7.previews.dropboxusercontent.com/p/thumb/ABf4uk6v6d7VKHC_Q-SubXtWRc9AXqFdJJkf0O3j-VkbjDRnHoqUsGIEIR_zMS1gxtxWoCyYJBUhLddJsGkagrPocSkMCYOO--qYyzRbjsms67klia86qCXAO3X2HFaj5LIgf8ZoW9T2WIO-CbLexc8Q8ItM4c4N8cQXu-FUZsOMA-o6rxf0SSD9fdC1ZF_UtdaGn24ceDYjOnNCBHQhfY01OqrW6SCr8wDibRcmjbjhz8EfVGEsQ2wO49hTuyB89SwzASNNRc3scK3A-DSpzpudBjghyvS-Lifun_iIL_OcYYTb-pgd9WfoZFlx15U7uw0mVEoXJbLXcV4RCmHNDXkgAQw0owElzn_Ma_2V6bi73bAmnR96vUlcBIr94-RmA_w/p.jpeg" xr:uid="{AFDBFE02-5199-40BE-901F-5A390252797D}"/>
+    <hyperlink ref="S3" r:id="rId56" display="https://uc15704c31ef47af00a5100e660e.previews.dropboxusercontent.com/p/thumb/ABfLgn4nuKS6B58Y8iha9_NP5pFYu8UE-oBUf1XLXvpznfbTyrmqGDC12dpXEjh4pDbLug0m_XY_M8PSq-Vzqs7y01_V1FQ3PNQx_DDDy4NsrfdkPMzAr3BBDRT72xZKwC8lhFw4y3Wh1vSmyh3giSVflqfNKRiJ25RUlfNqbjl9-hr0kGCdvqoTbYfMosSKm66_EyHaA6w3OurRfp0EBQJSiOCK_fFxANOON9HICGAM21Z9YVKFj1DLFL2rS-olkazswzEtrafk0ZCXs4ed_KwDkPU0gk2LQ-nvNJdONtzJBhGtKCLWaJFH0SbohwUIEyBhNHDLyjILX8uYXHtTYS8JNiP_kfHV7uRPX97nMfUx0EMbmNZHSDMR7oLeOIMinIc/p.jpeg" xr:uid="{70DEF3EC-7056-4B17-8850-C1CE31B288FB}"/>
+    <hyperlink ref="S14" r:id="rId57" display="https://ucbd6e7d45ddd17421102e97f896.previews.dropboxusercontent.com/p/thumb/ABeTYMw30DLWY9vkX7h4yC3ZxmdiCtNLTcS1NRSRZ6kk6JPrrFiMuseh2-P1INuo96aKCtbsPl4YbbG9wyET5BfwUxJQe3vOLwOEwC67_xCKaxCJ3uX8DBVz4CmbrwqbkUuX6ThHEvmWx-r0f0wftvnm6SCl0iRrGiCO8APA5gn_032gTSwT-kUlXgeRmNn97Vfc1emOkIWFi5Zp-vR-OdjnVofdGAVlf_i1cf_ceP56p8lD2axHWDR2SWTc4D-4EnqLxigWroC8QWxRBdAhNfX7ZqW9AiJpMiPtzMCeLQIa9b4cc2lgPdeUDZvo2f7EOihk_-iJKMa7iY79ZB17oE6CbElu4Jeu04b26SZ9_QLJj82EmiCRw_kcIKOM5s6NSYY/p.jpeg" xr:uid="{F80EA165-40A2-490E-B378-8667EDB1CF82}"/>
+    <hyperlink ref="S15" r:id="rId58" display="https://uc08263df58fceaa972604d388fc.previews.dropboxusercontent.com/p/thumb/ABd_I2DRoxRS8ST69OGSPeeADEXe02lMpiS45psSxyTjpICHJln8UASXGNUbQQXhfFGDHzf415QiE9E1EcE183v4x4FPBu9JxGUpjdzck24-7hEYbxmU3-qPa_vQUeTmArXygqCaMMDoe2gtoo7S4Jvw2U24xwJ1bSzKaZfIaCBYkG_2FC3-gaXYZTudlO3R3h3MXUtiS0TVVnKyDvCeo17F7t1XzsRHsW9aynSHgY9QeNxbIu-k-KKLAFTUxxWnSUmipBFQRsgBKm9sbluym2YVZA1c4J1IzdBQunxCu0wGempjH0tSyC04COtX1ETOKINWwDnfbFAmMt1chnV_Scj_QKAicbxSIYAHYf52UgpM5XYwdKQLtjf2QXKQ2c-ReFg/p.jpeg" xr:uid="{AB3D87C9-7D0F-4032-9690-F550082C465F}"/>
+    <hyperlink ref="S16" r:id="rId59" display="https://ucd9a971f66696830c6121de558c.previews.dropboxusercontent.com/p/thumb/ABcLb3fcVnGTg3daAk_e_-25Eu75E8K4fDN4LGRD_Ey8PNH1dLHojua-zwbrcr2FvA1h9WVCw6QBUoevNezeUixlCbFUB-t-lSplZbzzuZPzTby7D7PlKlsBUUKDQ7O_9l5aeVdAKPlOVseDnkhBFJbZP0GnVXoekZMeq1eO5GE-cYS39vfBwCetw9-FBwnbIZakSLcSmnzkBca25zIwdr96muQjss_Ih0kUYFjiF-SFfHyxua-sJ7stxeWAWTq5ridQDfZfbhdMAk9rBFMf_G87XXnXZYsD-9a3ycsFoifNi6m98k2J0iXn_-GOGBaYUR01qua3ii9VaXiOFEWv06EXoURVp3aZ_EwzZEwn8mPKbQOIu0TyX2oz0yO3ftVZZQE/p.jpeg" xr:uid="{5E73B485-8D4E-406B-8E01-9A24198B6989}"/>
+    <hyperlink ref="S17" r:id="rId60" display="https://uc4bb6b3c1f5228dbdb0476eebfa.previews.dropboxusercontent.com/p/thumb/ABfrkKHt4t09k2TPRjPdR44hbWooSdwJCFeG9SVmarwHBZE2eskrPCe0wTEmDm17Zugi_hK1iKWQd40HsHVUWbsny1tEtQm2KkAUd3iVPx7MNMriWrgNfIseBeVwYy2j1L11SZjwq_5OSbGnt45CNCfU1nFxHn7WwJ4RP694nTFe6if0z697J1Pb0mCPjRLPaNf8czNaFrZCBCruORTJtecpCGL7Yd676CtSAdp26tMWJrGl_ID9_6oooq7348QgoBayqVcWmzUlzNFraN2pVMIhbnY8ztBRP2QjePk1EP5KojwLtzKtWzbGjs1vXNum0TdnE9YJH1LTVV7HQ4Gxuz2MS-1Dl9b8zEU9Ae1S0oyIUlqmhf7Rjn_olkSbkXVrwWA/p.jpeg" xr:uid="{1C216117-3EA3-4DB1-9344-5A878188703E}"/>
+    <hyperlink ref="S18" r:id="rId61" display="https://uc19a682a333de699cffab6bd721.previews.dropboxusercontent.com/p/thumb/ABcr__zGSNirOGxergW7PZT4A3irfMOAMdQcLo0GM6ZTQ0QgZ2jjmmY5tFMmn5jOjyEL2tMUzwk12O464pv4GV28bFF7ZipcQRLajaM_kkn8vWJUDVM3mISTnG7Mx2g__lzFy0aicnxjy2vh6Ot0UarX1hWlGqf4Dh64stxSqFblcEv6udPMTzmveBgaeN-D5wWHwKQLQNukaliIh7FQ8mCxypsv7YNlG5hlLnEflCwm9wQj6-KWHiCOs_fCbHnfyZOsoWaD4kR4WwRx5jpAe25Y7lhQ16iOS24qWE-Jz9vf6ct23TpG8vXULEPiB0a0Euw7rUjKW-D-xrUfkaUv1Bkt0WujneReUTUkFauVtUNjd_F_fsCC0iy2GnI80YU_8GY/p.jpeg" xr:uid="{24A2721C-1EE4-4619-AF54-6A980028DC39}"/>
+    <hyperlink ref="S19" r:id="rId62" display="https://ucc6da03eaf0e3e046311b662740.previews.dropboxusercontent.com/p/thumb/ABeihBhH2xERpTg2Uz6cGsbtn4cn_RR37jnaAHzr-VQAU4RmU2DkOirJWl1HCSgHZguSgK5upQLkyufQgzKetMMgw7drIknGKWMs1VwMmRBnNgDEXOXe3TAvqyDVrPCiPvXQKuBwh55PU1FjlIiMem-ZTDinb5f9VyeWxGCI57inWrDDj82OqoRdPejJw1W_sipUdcS3Q94M67_BU1SQ6KSnl93kj20TarFR2RV6bXGS7IIDv8BHfkItN8yv6UgHmKySdo3rrDCsy2A8560LBs8YRebOC8gQ4UVPCUusU1nzVA70iwgtmlgxNdBsKE3VR_8NQCwgL6O9_rEE3EEtQxvkRXFPktCrvTsS7Rdz2L_K_JgPdizHEeVmX6wiikIdAIs/p.jpeg" xr:uid="{D14E1F61-D584-443D-B8F9-469505A35F52}"/>
+    <hyperlink ref="S20" r:id="rId63" display="https://uccd98bbaadc614b0d1c0421fcea.previews.dropboxusercontent.com/p/thumb/ABdFSqk-eHyqtI1aLWLS67Nlab4MZDJAPVc00G1CCLwUoxGuzEb3c5cfTx2RfmKovsMy3zENIkpZOqoSiNofvqfecnNP314HFxRs-pAgiGqLDSbj7_Yb0ma0C-cf8TDvDjR4iQyu-Eu3uJ2gd71u9qAG15OxbhlEZVjmpqlhbXlFQPJ3zwTQ7A5PZ8kRpMyVUCDkklr4kYeeexmMF0UMBlzcGSHEpBPux1kY2eKlROw6NpLrZT7TNuzFjhqdxxHGUHcwM9K2jO0s9q8BSMoC81z3-8aV_NsmdkUk83qv0Rgc9pxbNHB1UswNAjFq7Hol6ehn79JBRjTa2E81_Z8qYL5rIaCvDPqtF1qC18RgST4C-65o50r8JIsSbXgp355NoKM/p.jpeg" xr:uid="{BB7C0591-AED2-4C94-A813-DD979708BA14}"/>
+    <hyperlink ref="S21" r:id="rId64" display="https://uc345ed5ed39e24ffd35e7e64f65.previews.dropboxusercontent.com/p/thumb/ABfjsLapW6mM5-nbh_yGcFS8YMYkM_y3Q4GAtilBJq0qltSvXO_V2wWgKtitdICgJtn7NSpvGwuHsYMVQcsYHVSTQSEF7NNEp70eoY4yaNW_WA0I5RrlXg6TmuFvD1fVoDETfJE4qRnyGbbjopXHK-o8-ZaZ4X7D483hEDfmuSG0AaZB3MMZgVebuYpR3tyZSXnToPcAatFKd7N1NTmtBLgVtu-4nWOitk6Jvx7KS8rO98eAOyYg-8sgid3bngK_hzOkZ3FqURaIh_J7R7TNqjAPXiCXbqZSnaBjTHWu1xkm9dCkqtlQMJTsQfdmudvbJyK10l9jkLguncjPoa_Kr6-O-YiduZacKHsY1TG2GDFaPLKmkN0sCVay5Jj24G28NhM/p.jpeg" xr:uid="{F13F8704-8289-41EA-A3A6-659480185842}"/>
+    <hyperlink ref="S22" r:id="rId65" display="https://uc2b79bb46a20601ea0a9005caa3.previews.dropboxusercontent.com/p/thumb/ABcswFlE4ILcoEZ_zpUQGw7aESPpcjyf25nKwBuYh81bb-2VI9SVWsj80zwK4FKvM-Vu1bUKXdO2Ns4jkIaBPzcGBnPfeHCqtxcOouKmQXVFdc0afxLP7zta1pYKaEnMb2dfinHjHoA1ebEk_b_XHbYB4puqYZ_2Jw41KtGA_tZZPyGm7CWUPOUVu7ErcVp28iGCXfJAR-GdYgKtm3FHeqVr0wEyY2sDMHdzySy5o-M4GuUaGfOsKUyDRTgu9LVRPJkVNtEHnuZKu_hWIBkmzyfbpjQUA1wPAmWKh2DIfm5oaZP1ASVP5bZuhlyp0EytEhdnbAlkv3Ds9isjWTTDve1nxjOZB8dsW2VYi8L6S0IEn8tjkQ0IohivMzBDhzvZS0U/p.jpeg" xr:uid="{A5389021-867F-4831-B886-1C614F4D4754}"/>
+    <hyperlink ref="S23" r:id="rId66" display="https://uc592eadf8510f13e4b97074faaf.previews.dropboxusercontent.com/p/thumb/ABdTq1Do4fFrME_wh2kB_HaNfWJEUdhkZAE0hpBwBAudR4zAjhEjdh0SxpUTajGjQU8U6V8uq99kNEvNuLjqgmzr6KwZQeBzCGLe-g8dLxYbtixaV6U-CnsCRm7_BdzA0NFIWXB0Te1t29WoOHWCpNQhKKf_DeC5XBV3jrrBYGEl3-7Rq3f_ok7gLh424ODNvjuqgwjjXbGCmo4JPuX371p1HflN-PDs2OcxurgbWsHwtJHrNzXV400c38jvL4bKnBaRL06gPvyzek5zB4WoQXKqYE7W-3K0qyP1Kg4RaU5-jghQAsTEwKVi1kAaaVERXpiP4rzJN0PNTF7VLjGDBmqGu5SfQom9OInZQCUcjf7fUPeQTWk0O64yxhRJ7OFp3Jk/p.jpeg" xr:uid="{091CB816-BEA2-4F12-A75A-DD98A837D23E}"/>
+    <hyperlink ref="S24" r:id="rId67" display="https://uc10a0379f6ac2c632d278e42544.previews.dropboxusercontent.com/p/thumb/ABde3rEjudZrtHDZAy7eVJTZi1GUnyCEjx2YJ37u7iaPmO1iQkpIe1u1lp19cLwc6T09PC8lGZ3rf3q-GOiA4oqwB7m3ORQR8qS5UEvJVzQ0v29_J3wVV8o7M2Uqg4yETeW3tfMK8OjuixxuCXnKg2zuwY1F9kLIlAE5oy2GraFxSvEAdpwxDCkvK7Qj2fl7bhT4eMHyJhmSxnzXOvtoXp1LCjzR4K44dZ6YfxVI52Nh9Nb3ejV8pTZRnrStFaDFd_guolUrKdQfE1iFxwo--T8pi4DI2XVufjS-YMlJvvUhhIkcaa3dzQEACJT1ND1vBkaKK4bETx3K5mu8sUeNV0TU0BKVeL7K6IEK_6WuAl3EgfFkq0RaPmXEPP7pCml3Hr4/p.jpeg" xr:uid="{384C6749-AB5C-4DBD-B525-B4C6D8B88403}"/>
+    <hyperlink ref="S25" r:id="rId68" display="https://uc2d44ad4a301a2ef92ff0739f7d.previews.dropboxusercontent.com/p/thumb/ABdHeAJj97hKkkZHg9NfbaDynhGw60VpuSLK-eZD9ZWdqGFuh1FfwojBAlDdq6nDlcaTZADWzihL3XR9q5jFfxC3VAFouFQpYu5HqiJ1Y_dS7cge-bKByJHZ2vuRdTtMmdQ_Xu2fQPK2twYqqB283ym1Z76zdi1-HzaAaJI9OvdlTQfJFgeixzC9Y_lXSW0cbIcIIZAAbnP_XNAALKUVY7WN7bnNKANhJ5uR4XOJ6K4e8xC9Vg-T9c03WLIoe6UYYN4Q4IopsyA4veroabFg9uzPcvDtnWq2SevNYUR7ZlYSoyTzU3qfLY7dmT3VEGSNXHgRRepG_FhpZDHMKJLC353XOF0YgVVUaY7sNNYdn0CctR1X3PKPpo8_9Wb0tsjyZOk/p.jpeg" xr:uid="{22333AE4-0388-4368-B086-4E3B48650CD3}"/>
+    <hyperlink ref="S26" r:id="rId69" display="https://uc5f9904111d3ea55b60b4143c79.previews.dropboxusercontent.com/p/thumb/ABfH8e1ccMfimWukD7g2Ahk8gAFcEJp-X6zPDSD17spYlpTT_vDzPs9YHsaUTKTr2M3iaYo3AGI6G_riBQqumy6YVZJCHavjD5Hbt9YV8UhiRv_Zu7Iah8fJY9FOqJ902mFlc5onL9mN1vJcsgqjw9qWL8jhJAi-ZxoUvxccIYwfrMptzLO6OK2zwPF5zvIJ2qUUkjNNvuybjrE1gsWjB5Q1NJJmyRpblNj0k0cAE7kryDEB9T7yhpXoRWt3sRsE8yJGVTtlPBbQqwWSey6k-8CIuI6dVsBbfIVzbPGAJfUzTfuaAbzjhX6_nRjhTUD89aqFdLATvY_PqJ3OCy-vTnKsUlsnItxQuhtOcSq1pqFFRw70tDThF-OqWr6QqBLww08/p.jpeg" xr:uid="{827731C5-3AE8-40B2-BC57-FE841C69DAEF}"/>
+    <hyperlink ref="S29" r:id="rId70" display="https://uc015a5380f769f4855e21c2ee41.previews.dropboxusercontent.com/p/thumb/ABeHsHXtDdx-su1lpGhhok6ZUK8fotSjBBfvH-ONfS8Vbr-t7IAO1QYGyAZ2lDOVyeAgnEVX4aB6vrDaaw1p1JXGAceCuYQkpK_v3YQY_ssBIBXKLQxW60mILiLkbuY2F5Z05RNp8bLjyd3gr8GrZocd575bSwLj9uqn_RJuYCbKP8hPHK4YmQKeFm2oY2hVRDNVAuz1EIyMRLx7WL2EwvxoePthxQ1cqyn9v0JlOTu8LwuoTiZBSK0VFc_yCJgRDaED4VmiPQ8H6GT_sdnsMu5Bux6WD54ItYPZ5LtMP55lU01YiNkNYz4_etBLCJnfimulEV_IZxTJG1swNZjLz4x0X9Jg-qiYGtjlWF0-XiDf5j_Qn4USPvmTX_iZhKFCzvs/p.jpeg" xr:uid="{A7E47F32-F209-4CDF-ABEA-539DA5D4A66C}"/>
+    <hyperlink ref="S30" r:id="rId71" display="https://uc12acb66874afec202097dd4591.previews.dropboxusercontent.com/p/thumb/ABfTT9ii_MHe5YrmU_uiGP-J7ezlghj__KhpuCZZhFwnEgFjwqwhu_StH18j0Q41_uuq69AZDa11Xjpd8oxbmc8LXoX6VlAwu1LBj2EYe2bESts0xu2EA_e0QPap4oLgvbV-hochpepcCWCpzREyFu1b46tY9wThBGfaqX6YRYjNxtIwzxyOHN_1QXo4ZynPjPPvc0TD8D-kSrNM3aVkAam2gpZVhNqRx9hMDNZNtRMoXfB3DpiezxyUrSRQO_evT_RKp6MZwe6mpY_LSBfX8_X7I97JmaMAnw64zMERXWZqvMW7gGXWJZsdLhoU4auYsZlJrPrQ_tKDEVC50YbR8HJ4hhRO3JnkLgB-upREdf8__oWqtBZ4ISjfQQmSdObWynE/p.jpeg" xr:uid="{D9B893A6-989C-40E2-BD5D-FD5F18683B13}"/>
+    <hyperlink ref="S31" r:id="rId72" display="https://uc9d070795294239004b99a90d4a.previews.dropboxusercontent.com/p/thumb/ABen-JYsStSoO1-ysZ5YNeXxwu9wt8d2LpQPC_DNSvBXY7W_sclPq7qW_XW1X8aPvvSQhhdSrvrrJVBRykOvHTcqJHJwA_6mahaMlGPJQMEU6E2S-Aj1E4V8eADkB7gj7i06RlzDCPvqV_4JbyTMik8hrGed7Bm101hNe9lJn3IDQz_l25UjEjpWG_gZhKcKkJEEBM8f3E8FvprPfCwwbBNvD8c4XPbIFeCZyLGm0tavByEltpwZZLc419RZOB-M2UFARoksOotjBLeOIDPBU5a7FoCsknhZzPAq0WYs3D7Z-lBt6LRJlCs8Yo4gWQAPMweHdGBOpU2ufxuHCuiIEqxR8Wp_t_u0_ba4qgUbDrCyIy_Ni_I-sK6JxQOzNmiEhEk/p.jpeg" xr:uid="{504959EF-916C-4300-8F03-4AC31162701F}"/>
+    <hyperlink ref="S32" r:id="rId73" display="https://uc5653b21c4bc4c0a5559d6f0a6e.previews.dropboxusercontent.com/p/thumb/ABdgl2zQ373P1oZbyF0DD1gaHUZQV74_VaLHkpZYP8i9KMLxnQjc_ti9lylW1szmqSVfryr9dBsHVwQYsRRR6u8MOcFdG5_7EVaamMk1Cq9MCRcx0VINATJvp6JdZG2CETm0AVIY0soFBKO5Webmtu_hLyLIYiU5LMiRcfbnUHWigI9a8sdu7H1CnA4OtsyNxUMfZgCT1KJPxg5DzhrzUGJ9R4eSYqyS-XyeKrT14N4VNajYTTp8VEaqNxFblyU1mxEgSf00IJeu8EghFz8cVqR2PM9gPp6HQwLJ7gjNx4cXnZJOB0g7O2BCrXP2ivkqSSoRKsGE5uSQOuHerd9Qovz7zkgLhIIjura582tyae3uFkjr1VQeQ2vJbq8tIhuZ56Y/p.jpeg" xr:uid="{2EEEAE0B-6781-49AD-AC40-A5610FF1DAA4}"/>
+    <hyperlink ref="S33" r:id="rId74" display="https://uc78db1fd14f1d1206fe0cc7167b.previews.dropboxusercontent.com/p/thumb/ABdBe2OTfsoASkyiEA8EMjaFblapWk_0Z6DVP29u1hWaSdRX3xJZrSF9rUfQX0i--QysFcuzeSxdul835MzMOoleum_dbNRPUJ3GRWRNeDrJQZglyBQIBEScLtVbevsUPUNIv-8laLRi1Q0nMpeI_kATW36XhbboTDA9kMXNrc3O5ykIxD91dnUPjtjb7-sxLvrM6RTCj96p8mfOml-pLeHzkyJD6WFBn5ABqZV3Sf1aPtOZlQ7huqqNfbB8wSukgqhr6BBTwIf69n8BPVhc-jQ1zzEcPeInqdEZqwhtybTfcpFcrIn84LBfv1f5PtkAHVtt7iatoZMXXuvijovOkc3VG0lvJ_tdAO5SkrSF548lHkS7llTHti5AujvzE24TyKA/p.jpeg" xr:uid="{4177EAB0-9D3C-4DB2-943A-C88B49F0A04E}"/>
+    <hyperlink ref="S36" r:id="rId75" display="https://uc072b77bbb7522d0e1bae4e7a26.previews.dropboxusercontent.com/p/thumb/ABfMj6D5GnSlUv8zI7xmTY80DoA8D4-1C2KxlRqlEHLRfvx1dDJv1ujBqFNiKGN85vAE17TFN-XsfJixbjitWHNETuU2MyULJG6Yw5L1vSS0jMPkqVsbZfusnuzJ6MGJdmyRZnREPOdc6VdMdjqiJmwaN8n4o9usTFMoojYbgjfvTWgP2jlBopTNGX6vdBHbW98rmG_HFI_fhONfJs69aIzH8rSJYgmIHYOCQjmu21tgtsyNtXfXNPR3Fs-BzQCO5gqrlPwXSek2V3QCpTU10tWojQ9NrEguu5zuUGTU8qVJYWFFdgWISrgQt9FKTidSTGnKIQGrtduyPPD2zY3m16zoY58h3qcE3uU8ycTgtTUkk_yVtyFlqR3OaFYCcC3BQ6A/p.jpeg" xr:uid="{FDAC5791-2B05-4B1F-B329-E7A655CECDC6}"/>
+    <hyperlink ref="S37" r:id="rId76" display="https://uc96bbf2f337f688b574d6febbf1.previews.dropboxusercontent.com/p/thumb/ABc1TGuKocmlGAVpcMfBDsabwfjk7aHcgy6uy6KAE_W_aDoDxYLwBpw1U0IEkgy_9zUOEdXbIDe0JNOSlO1pGKZQ4kW9cw3AdNio5tToHa-t-UWzbtm-hOO-Cg32A5H8cckAGHYGnnAZ3_HHDwE-Hl5tQORjnvXklwJKEBN_qSzGleVdVf-jffvmnNVXZ1fkvwIbSg4pqEAO-k_Af9vq9DW8apkRA6xoLyALzvs7qLmRUscIeI2c0I_hWSwW-km8oN-WOVMEtUewb5O0aGBcyUf_3dtykWehNcF5UAwJfWRsP7KZXEEOiBMW5G5AUPcrXHBKmXN58jE_uS5I2gx1RIS6OEBx65JjR8Ij5Md2B-Ei_1NOa1MBDbLasUHdT97to9k/p.jpeg" xr:uid="{03628202-D11F-4A5F-BE71-DE2A5AD97B71}"/>
+    <hyperlink ref="S39" r:id="rId77" display="https://uc11168f70a2fa011cec3f4582d2.previews.dropboxusercontent.com/p/thumb/ABfDJCFK_xjFZSJAI7sDp0tA1jUiKBGMJAt-xo9BN1YIbW0HnAr6Od0Mw-ME7zRwV3xyCI5qD4vCsJ-7n67V26SL5EMSs9wcz4KvKHYzLfdZI1aEr4VsVHSls-EeusRkUlKCjfflJvuCvRv1xslYpFfQVd4w9RqEc1XBjHBeT3OKRtyKylrMc49PklkJOf8TlhnWcJRQAWOwqCZFjT8WhAW3I3oF-oUi_rgD6fZGQui6SGMzCmpwkXh8Qgmu1FSR6L3MePtDprKQqq5Dj4sTd5tV53c04PorL7lev8kvtCnDVhoBegdiT5OOWEyHaWH7zCdDV4HLrzumCBB06CQF4HyCI7FITlLK3EOhT-vJOsy9c2L86KOrzOxgx3DEPQbt-5c/p.jpeg" xr:uid="{6C294763-D096-4B9C-B1FD-4DB5E5C9934A}"/>
+    <hyperlink ref="S40" r:id="rId78" display="https://ucb66a69016ce41e67c5795cfe57.previews.dropboxusercontent.com/p/thumb/ABfFC--DxJBVzIH7Om8iMME502BsMIshfLOoVNByRYyyq6HbbYaYoJZdldu8XBQ-dVzQ__RymodHLPGZRQTq47qk-DF4EwfZlheDdz1-4a1n_4HLPAY4s4y7xznXsnQ6qbSznA1kE5F5Jf_v9695uIcaqIFbVZWXPF8nVweLMxSieoxGIXtcPnbLZOVyABmMJKhik3ETSV9EJcCHHgmugvxaWg4UbaISAEj37_i22CB613cysLZPfD79mit-HvjvLHfKqH4Q2Q5cA_ylSV2Bx5ikuN4q5Q2Mz2lKN25gKcl7Oj_xc9t15ah9i52DRJOy9XPZnhikf3EOrWjll7poJOD1sFQhie3grxWfGwAVw-93V3Pgr1gCQz0EHy4iFGZq_rM6AJVKKfGIgn3Ax_xnT4kaLyE6ACZjZLkjDqgX9_vl9w/p.jpeg" xr:uid="{DC7E5C5D-3291-4BE2-A97F-B05603CB0686}"/>
+    <hyperlink ref="S41" r:id="rId79" display="https://ucaf3dbc0a0373492005231719aa.previews.dropboxusercontent.com/p/thumb/ABdVP3WaxiQr5i7gh_2CAOhkwRiUiZxVOF9ktpTf2URKwTQvqW1JmKon_cEu06epgleWN1MdOeEEY9HW9nkwo413Fajjzp6JZFP3u2o_BoE6sK2C0aQC15DmCA3ulAsGSNg_Z4Eci7pZ0-GF6ZhTumP_h3Efx4sQzefPXWo3I-cEJsxgFk1sdQdku2AgGxlfmIcOfrvWBxs1cc43R-tz9xOZdIJgQroTN0O3v5caQMFrtdObThpBdZLyyhTiPh9dWOYkZXsmjbWIS3Fk47O5uw2-LqUfqeN1UViIQZo2Bg7xzlasLKxawnO9ZwgGIW9UwL64TiJ4dmhOHDTtJ4GxBR-ocqx0Zzuw_H6Y8nc3GawqqsGs2mrPSKWW-U16mHXI797IKrSLmt_FvquJY9UaCKplMBv4j7cIFQELWdqSKHX3zA/p.jpeg" xr:uid="{91D38BF0-A6C2-4871-BCD4-69E399FCFB24}"/>
+    <hyperlink ref="S42" r:id="rId80" display="https://uc03d661ef846c2bc7cbbd75b435.previews.dropboxusercontent.com/p/thumb/ABcpNW9qaHSUHPw3Zf8H6xod8-NzabIzD7uL_zT5jHAlBEMBGthan886y3f8pGbwFp9wMcIzVkAfo6QqKyQ5dMfl0HdthnPCFVUUnhd-CxEicCZ-oe7SWwd4Imu1HfK4DxKx2nwjYq9XmcV5rroHQyTF84Zh2rCl10og-tRZdgiNjZgPnLKWUhJuby-DV2975uzjaI4WBsvoE7yRxeqlMFz1gn8fw0Yl6jL2yZUnyzwrMpGFzaTAthjeMGJqOap_G5366FJtl-3gIL_vV2gqFAo4kdoXRINWOd8vpz_TJmYo5Vw-TnO38cGYznb51yL1dIpcFGjHM1L7djcJj7jctXa-kVO93aNGMscAgv899tTC1WFFVXofXn7oNNxJDdN7z1cdelQ5aoT3V_2PwzAYjT8JSZgUYWtZgF2QHz0XSLGPlA/p.jpeg" xr:uid="{E9D4D0E1-8BFE-4EF4-89B8-0FDDEEAE3BCF}"/>
+    <hyperlink ref="S43" r:id="rId81" display="https://uc032a835146610322780cc5f186.previews.dropboxusercontent.com/p/thumb/ABfmtClbUKIZ8VqeZDpxXG5yDfb_XyIcm3lQgqB7eNaU6dQ2mv-0CSEgHbK-V-249_4DkQqIY1N7deGVWfGIeS63ZNOrYZIRLu8sSCMdDKN4D28zWgHbu-xphMcDAvsJuHmPkFU-JQuvv4A0TaiBHfPWu3noN54yXWKuA-VIsX3JbbVSPEO1zDSKVexV0G3RMIWCLHI2O1qsSNI_tcfQujRdvf8KRM95zWI3kuispy4lFEWdmjrYnoFe8slplMciUcBxTgcCXuUvtc8SFQjkc7775B53NSuE-Jw9qC7_3-I1bXI1YPLEjH9R2WlGb15vncwUJk7-wol0W5vqjr0R9Nxw0jOnkWNZtPUdcee9bkKqGU6Uz-mQgT8p_C28PQWeGku-9RJnep2OW6weOlC3g7CtnA8DvUmceB5TTqaCUmq93A/p.jpeg" xr:uid="{DA64F217-2099-46D6-8846-3DF0D87ED1C2}"/>
+    <hyperlink ref="S44" r:id="rId82" display="https://uc1f33a6f358eb8cb4fb479fdaec.previews.dropboxusercontent.com/p/thumb/ABchfz0joiYPxR6wzc0xUaQZm2sgs0D4o-ujq1MRjxcdmapkM0w_T2svIEy-XeEGAeA5T1WwsxoJEFNPqzCDg0izXPlee5mxEMT60OX3B2M1YNJj6xBvjXx7cBnj_F5rqgfD6xhaBrjMPD8us-6Ha2wRiE2d1lBKL-BWF7OObQXbo_S1HLm-nfq30bXm0Qv9u39T9xNwdukWbMoP88bAgU14ZB8vzYEVMwNcKmkht0_E6VPkjQentV1O7n76H3z8TS3vSe_VV6-7Ch4Fg9TYCmx5fnvak9VWzrNKJKvY1XQYMAUDj8mxUo-W-oacRBtlux12QUfzb13VAe7NejgR0IO7rfelr47R1kqDCBhkEl-fThc7Mbr8KUBoCNso2ouAPr4vcL_OBlTJltjGEy7yXFttcErr84vjECSVOxRpQWtOdQ/p.jpeg" xr:uid="{45A27B6B-B9EC-4F35-84B7-CE9A211662C0}"/>
+    <hyperlink ref="S45" r:id="rId83" display="https://ucec514f2625e7a4aba72b101c7f.previews.dropboxusercontent.com/p/thumb/ABeSpvtqHI0zqtgulFq0rYChM-_ampMAgUGpgr8pwrg-3iVIBdfIMT2J9uT46-ZJc9vUM66HHLRM9EoHsPdj9iL2YOTmHseY7jMOG8U5EuBQRoj-pBKPPpIWG_UHsjWU2814f7q__61AWNECXk-Q74imXeEEiZvs27t8SU2ntz9CCTXtS8xzRTCcX_VmdZBVUa3NN1-lG5pIzgf9_4qDj_PVtZtyp7IXxnJszFWNEIJIQjedlS8F9fRkGoFGCT9w_tecgnXBQeHAO8f60jn2YTrMy1VxeooesBImTc7ecQXoSEY8lR63Q7rTIX8xYQONCF24LHUCcP7fw4rA7AXNAxo11cL9GbqkftDG3gGFmRg1CsJ33023TaONJb4hEbaSHA3EbdTKFyG_BDar4VqjGM-bWvNayx6EUzuQ2lH-h-iuLg/p.jpeg" xr:uid="{2F4D4E24-8D85-4DC3-A68F-C8835A8C8CC8}"/>
+    <hyperlink ref="S46" r:id="rId84" display="https://uc034b5b8de8b2771327a68b2ff4.previews.dropboxusercontent.com/p/thumb/ABejOCRrQW2VG9yOfC1IyZv6ovfjmviwOMuY5qw3r2uMlmCxw50dT_5RH1Dgm5SZL8oanu35EhcrTakf8Uq8CePgGTPGn98UxxnQ2U4k38htTUTBvE9n8NbVVgeMJfBIx0edDssRwvKgEiQqI7FYGvW3hwCOdsQmRGvVcOjHCivSCc3HD6dg0woGylc_fsp4EqW7vcA88JojMTBNzyLwhrXbr2lz8WDXHIdkhhVOJlFH5yGR0GJV4LmvMKQ5E5ZYaa_kHbTD3cywOits-Lu-vu-TQHAAI-stNs2lPoP4_otl-Yer4jWjHaDnBp-6YvEIutYR06iYxxRtI73EV6P9iyJgKDdTh9TaYmSItwQSAD39nkfn8xkWLNNhtHI49XUpdp0-gYw-okzjY4FU3FMNd3CHCZUkzJd1RmjWuKPtf4x5_Q/p.jpeg" xr:uid="{9A9466B3-7C2C-4C04-9C42-C6F95183D15A}"/>
+    <hyperlink ref="S47" r:id="rId85" display="https://uc4c1ddbc7cd58ae881d4fd284b9.previews.dropboxusercontent.com/p/thumb/ABd9QpLsOOMxRZqhuSpbY_KZDxOay5CdrC5buopt1llrFDQE52ZCH6LM4jH0MFb1x77azVkA8yzv5tJV4_C6c8wws-hDwDoHTK74_BSye70368Bf4k69VTGRkND6s2d0s6I_5aB0deM4MY1e_BRLCNq7UG0_bMNuMhyocTfqLvR28UhqMPDF3v0toaj7zB7iGL6SUFRTAPIK5rfa1NtSzZ3a0YkQC6ClY9QDDJhkGH30gjLQPdSNvweT-ZkE2wTqxZ5_gssOdymGu_kOhSowSAmMf5BU5-6gv4ofzPutBrVy_BMq4DPkF-DnK_dDzDK8PRpF9Xw0yv30byZBz-sm8SVbaxKOp_hBQFfsaD_-v-5MmrLHVqp2mHKtiUBQzYo5ga24NjxRgImoQpGz2k5SWOoPd50xap1UHcTwQE4rA2ZOQg/p.jpeg" xr:uid="{42A7F6EA-BA09-490B-AEA0-932EB36AECAB}"/>
+    <hyperlink ref="S48" r:id="rId86" display="https://uc0e3e8967bf06a15c3fa3773d43.previews.dropboxusercontent.com/p/thumb/ABdc5-k1PIbBaEjEvNdW5FO1AJ8GfQSg9JIfouEyzhnGwugP1EAiLX53nED6Dt5GFGWTSHWOaiQnTE_gV6kjDaSZSFiFJ8F-W_PTtM2EuFlHuwT0dmBy9XUykwlWDSkYK9dKNa_-YPTY--h7cGNLhs4e1fW_pCX79JeLC1zYB30tIEk8DZVHODMfhkxq2-bS15gD_11DINOk8a6MVyLPjDGShkr9bRRXrvy2MPJBYCCnJJgYft3uBMSqaWQXtQBkmdkZaJSOgcY6gDnG6Zk7C32reZgS55M2OjPqd-JVcSYAaDbi5uSdVwX224cgfHWQeIJHHjo_56c0c55wTMrnhabQkbG3HWyIi1gy5Edm2KVf3PIOOhA5kp7NEEgzSFPCSMfU4UtjcKDpoEWI-EFgksG7UBY7r7avdfvDj11nx21a7Q/p.jpeg" xr:uid="{EB6BF247-0D37-4FEE-B8BB-3FD000029744}"/>
+    <hyperlink ref="S49" r:id="rId87" display="https://uc656b29d690f8216279c80811d0.previews.dropboxusercontent.com/p/thumb/ABcdyCdBMjehqr7JUqoXAUzZliwX-4LBiYsIxL6YXvze2g_8QFSsB9ti8e-MKv9hnp3wHMd49i6vImtIObrb77ZWiBgXpxxG-B1JJEhAZuFgU61HbphcHQGRvWB3PaA65x09qSsSUhkQS1YXtrW3Usi4tnglYysuMdrJe0_nUvoPEBz6mimK4BNf3IgphbfE4l2MCtl3Rqr8rgQCphu0KfJkURf-Jed07XQTaGDdlSf1-6n9BZtRSYLP7Hxz-Yj-At3X1zs5ZDbCm_rF3tFZIcPqhGGPv5ULSckOAn-YneftIgYYmnqr_ev8XOhq2qD3y7XH6J3qbLso6D5tpY13kSQ7aI56LbhTObPJ8tFx3yG0vw_25LCxTX7VA6ipalXYHiUumXRWwlkZWRGRDNJLf5n-vyjxqgCFeXqWnkxP4KUd6w/p.jpeg" xr:uid="{CBB9CFE0-32A8-4560-A6E6-23C5B2B59FAD}"/>
+    <hyperlink ref="S52" r:id="rId88" display="https://ucb4fbc484a655eef8c73cbf7c30.previews.dropboxusercontent.com/p/thumb/ABcZDNLim83J0K-hVA_vWZoiqrDgpmkXdNNR2QIpwCa1YOxCmva8G_yjzM03zTyVt73NptDzOnUyKvnhxv62g3_aYkVd_gLU4il_yaO057hCrqKcynFTFSZqtMfHrtoN1DRudiY_-GvkYytKNBOVkLnST8Kw4dtLBTYG-NE6TT-otto8Nj-yWGy-S4gqwTYkqlQwZXZ_XhoGqB1HlaUSoMQV957-6h1DReGfBz7Ry63J3b4zR60OAoKAlnQh4Iz3vE8O4Cf5bygKEBmcedtruGEwwwpN5f6W__85LISxc0lJFf485_oZ1j8hWGtqgsCUnkIo8fyqaew3fjQT8fLHWhwdTSA7s8kKQYOvSPfpomjJJWfOe9ZHu0ohYU25EhTP2epplyUo4kzJCZ5zuOqvVkWCVE7t8eaLU4uE4Fa1QxuchQ/p.jpeg" xr:uid="{7932744B-D63D-4C1F-844E-6D281C4BBBD3}"/>
+    <hyperlink ref="S53" r:id="rId89" display="https://ucc78c6e58bdebc65eb75b4a15f9.previews.dropboxusercontent.com/p/thumb/ABeGuajVtgU7dybJwHogODzIMUhS0eHT4bw4tX_reFiPGvcDCLQpHheZIt-OdOF2CDMVmKpCl6XbE5dyYBC-ES96zuUfxLLAkbctGQBUGh2XlW5nHnuezoiItQdEulwkDS0N_TgmVa-U4ZeavJT2fjWHhVXHoKQo3WUNLhp3YlDQ7g1O9mBY3GhjnHoJtEDyjiYk0hLbJmYFbQfl2DUsQ-CkyWfDNK_26ckb14CPbIVzOI8H7TlP8sn2VokJ9tt9WRKW349JzAQ6M2NTQwp3A0kN27oEiynUMp2Xv8xckzDxgDx-dB6v4G3qgk8Q2PPitC1aIHogYOGhppw28L4WLtPdQpkJTs6KJIbN0YkK5QuS5nIZRXkCFz8xYR52SWdqKaVIWxQj_6HhPLugDOhk8MYLU2SINGeZkEfr18yq0d6NMA/p.jpeg" xr:uid="{B4543D33-6DE6-48F7-BF92-D2ED31FFFF12}"/>
+    <hyperlink ref="S55" r:id="rId90" display="https://uc13cc8d5a399d899796296d326c.previews.dropboxusercontent.com/p/thumb/ABe6DU0UGxC02G73DIkI0PWQj7pOR26NvgF1rHvkDf9uKA1sRH7ZcHYjEJ_ij7bhCrljskpNdyhB6loEny_XMj0A12mso2goCjcm5XbLbNzlQvJyl-pn0kktj3QIpZfm_Br20edmV9eCdyj1ZJF7bViD1y88bA4KzDtd-08BJ5I4iJRg2C1hz2hxR8XItBhebkAoiYpu1K7WJHpNycF3br9QkDmZfm2zwSemBB0pKf5WHfWFdFMD-F9K3Pig2QHfZEwpP_neNdZSp9uQng9MNDTg1HzJodQjwzV8JNr6zi0koymkEcHX08eCWOLLMpaYngxeak-LuP-4G6JJVqfqnyxmsU-QsMRIkxnjrYKQLrVAKmDf-U8BD_NhVnabBgRAVVMTtj-nOEGfEZ9AoeIMu69mY9HGFGr1k6ExIoQVlpVBAg/p.jpeg" xr:uid="{31F44A9D-D9C5-4F49-B2D2-2FB243B3B396}"/>
+    <hyperlink ref="S64" r:id="rId91" display="https://uc7b0406223bf1daec0413cca967.previews.dropboxusercontent.com/p/thumb/ABdfMztxLH15j68nBwphpOaudt-KQehuDvZ_lIxW55GDQq5jKAntatU8nfDBLaKkTkIOCy-EKk6zbZfVvP-93hkYEOVKQ3zZYiJYA-OBwyDobkZbXH-_O2EQd8LY84HN_XgKTEn-9HSJyX622wS3zd7n9hm7sS4yk1w6dCkqq_HkqEHbGK1V9i22xhsElubbo9oI9OOpZfWU2gtcc1imtKXuvwe63FtCaVPRZZO9hNHBjWlKDjHjsu3CZatRzTfpWSHdKq28apCOGQ5uE5n9QLhRY7NBp8jHYMQc4BoN142RDsFQR7n9cc-vz0044gO090PwQ5mD2Kwo6nrXhAUzG79RalIcnzO3O1IywGPA0k7RlNvM4L-jqxRnKL7mq2CssbsECnJH1Bayb3FIwAozLISu3-BCAWOFU7YUIzdBJJReYg/p.jpeg" xr:uid="{2DDF491D-2026-47BB-9E85-949DF05C3A0F}"/>
+    <hyperlink ref="S51" r:id="rId92" display="https://uc3c868bf0f6f47a0eea0eb045c8.previews.dropboxusercontent.com/p/thumb/ABfvKyncm0ZMnbXO0KlzkATSYszJrVT1PKESgPrSQX6W-dqCRjCyM4tFTUISjMbUcbo7KJ19dNJj3UCjqeQ_OPGbrDyHGm6w48QzLsYpl4sYcosjZLFZdn6Y4xLRCIXiSliFc2-QgWLYTN3MYm00Gb-7lpRMfOtuuuOPY8_arTzkz1uDJ7mC8sSbLrKnIknCQqB9uu81oWtXdESEwyyOr7oSMsTQzSts9p4If9iIJZAJm3pR9-SQqdERj21yWSYFL3-EcpYGEnypXggItMZy73d_d0PK56o0KRoZthnJ3XOgv6p2ANvCKJoGM_2HUIc5XSFdqyAqu66IFTwaU1LiRQGhbKSsV3yEImDP-qnMAXis1NXS6vVc7ZtjQM4Ecwl_pmy7RxejHr3aPGlqsOVA3BW-BcAoruVW1aIc2MpicXrx8A/p.jpeg" xr:uid="{638ADFD7-425E-4B69-B8F4-37E94BCDF139}"/>
+    <hyperlink ref="S117" r:id="rId93" display="https://uc0c68e868d69f568916df4f9c30.previews.dropboxusercontent.com/p/thumb/ABdadMC-x1JdIQE6azcIAnUZxoHQfS7DLvWVp_TG-CYvSWhO7mxYUAWvRjLTvPNtwet5zTvcWxSHIqHZThrF7C7uNZFEA0bb9xnhn9NM4UXlMs4sN6yGwkjmTqKyMXkhedfseiT1h3FfQIeGHwND8N9_G1AoKryRlBL29SJbrQcb0VauWEaeAhy5wQS0ZKKN-VpGLv6jm64kByGsCxnxvPj_mE4zg94e071cAO-55WTXgYWj58gOwls9oFJy9uvBvgkEA2fktpI58AF5jVilDZNR4YJhNU4-UdgJdjZXwZQoZQCFNuGq-fidKh5bsPrUzBuUpX272pE61eOlaI7jCDRx5oEMWdqpvK_T0R7h2Ras8sK7UlGBst59CxFjQMi_nT9koBAHvtd7vexzlF0rWJXQAWtoJ1Z7cYdP6ijrMR0pow/p.jpeg" xr:uid="{233E40D3-C952-4139-9875-BF236C471D7E}"/>
+    <hyperlink ref="X118" r:id="rId94" display="https://uc0c68e868d69f568916df4f9c30.previews.dropboxusercontent.com/p/thumb/ABdadMC-x1JdIQE6azcIAnUZxoHQfS7DLvWVp_TG-CYvSWhO7mxYUAWvRjLTvPNtwet5zTvcWxSHIqHZThrF7C7uNZFEA0bb9xnhn9NM4UXlMs4sN6yGwkjmTqKyMXkhedfseiT1h3FfQIeGHwND8N9_G1AoKryRlBL29SJbrQcb0VauWEaeAhy5wQS0ZKKN-VpGLv6jm64kByGsCxnxvPj_mE4zg94e071cAO-55WTXgYWj58gOwls9oFJy9uvBvgkEA2fktpI58AF5jVilDZNR4YJhNU4-UdgJdjZXwZQoZQCFNuGq-fidKh5bsPrUzBuUpX272pE61eOlaI7jCDRx5oEMWdqpvK_T0R7h2Ras8sK7UlGBst59CxFjQMi_nT9koBAHvtd7vexzlF0rWJXQAWtoJ1Z7cYdP6ijrMR0pow/p.jpeg" xr:uid="{1E09B404-F835-432C-BC76-8E2DFE1AA86D}"/>
+    <hyperlink ref="X116" r:id="rId95" display="https://uc18f08d002c9a613a28a0086fad.previews.dropboxusercontent.com/p/thumb/ABfd58-PPmiYUdNAlDEe6h_B6IiaQf-oEHlirhQvWpX-XKGSgCDDuDKtOoCxJOPRdu7xvqUL_erXsTKizY6z17GZL1x_teTKqjTEJZkaNxemRCKNT04YurJnLG2vu_M45BvRdKE2bQfFrkxkLmYjzPjlww8mnvF5xyEEotaHy8BjossG4W17EvII383240-B5YjOaDkrpQv04tHxXpNLNyGmPbes2icuc7oanqagd8eQzgrnL72v0qa4kpS7vkpZ4T5fHAiYrJlEWb73Fnm-S-oVKbfV72NuLw7tXv3Dq8SqSs1Y_rtdVVK6WiSj10iKMZw6ZVsvC4rk9DOAbGunSFGea9m20NOm4SxPS_Rp4jjD26BmgrhSHWG5i_D1LUS9tCqlA-VAOPIQFA4NR1IyGWrgQivItcfAAg2ox9luhuo2uQ/p.jpeg" xr:uid="{8B363293-87E8-4EF6-9BB1-0BFA8BF9C5D7}"/>
+    <hyperlink ref="X115" r:id="rId96" display="https://uc9b2ddc0c78a7155fb0ed01917b.previews.dropboxusercontent.com/p/thumb/ABdEGLF7egd0G2pM5dX7AGfo5FHhA9z3-BeHeQ5MOL8t-21T0VP5sDaixagumCtk_MlBgdy_0tvf9MaX1YNQA7EABMowbeo-rHDQMw9VgpgKGD1xDY3bZhWOqbtQ738Spy4x19ptCkfO4Wwv43oW7XqBbFtm9Tm6sKDl-NBbrD7_4x7-Gh8fS8xiQfcME881MUrn7D66XfSMy22Tq94cFhoJ651n-QK0aojgxLnRs2_Ti0mEzcEqomrUfZhUvQ2XVBb9nXBP-hS9-adzeododwbM6rJhdyn7p-C5vhZbKcZ87E4JfOPqa6toQLyV-VjMSJXlDeRY-PoV1RTgfcj1JG0ntpZfDkGH156rOgqUYUQEmczkiSRIEkPaHEwia9v7BDNPXtd5pwLTOayDvO_jhv8-QaWnwEiF65Nr7rlEuooG1w/p.jpeg" xr:uid="{53EAB55B-D96A-431A-AC4B-5DD2D24D29EE}"/>
+    <hyperlink ref="X2" r:id="rId97" display="https://ucf31c780d390a8cb66bb83d4002.previews.dropboxusercontent.com/p/thumb/ABfvSNrt2wHEshyUXbzezFx4rof0ejdFSFgV3ucUEcHYVL-kJPI_XjqCFth0gVnM3YQubDyS-roI5UiHGWUlGdCKW-VnXe4KI91oEoshW90C4hhImFx2TtHAOVo7R4AwKeDgAcAEUK8_X0YkjUN4AsMmDgDSrbRVOBiK04A-ynnOGLBBXaG1tFVdQ5OAB3PE8VLgHWG_CzG8g6B56-dxta-Gi29OU39D_5qoi-rtnt2dKBmFDF_PMuetx6oKWUss1N_73rWo08JJvQoIeLFt81jphaZAaYnZwm-_77q0AwqJRnp2LZra6BNIYw73wgmKPju7be6iKMcq_CvfoXaNiTQ23b4Dv976oSxfKZPMVhribnnMLRaI829RwExIgvU1e98/p.jpeg" xr:uid="{6D583A22-3501-40FC-A3CC-1CB4C40B20D4}"/>
+    <hyperlink ref="X114" r:id="rId98" display="https://uc589611219f1960daf2097896e7.previews.dropboxusercontent.com/p/thumb/ABcsSMMY8yQn0SebALghdta5kA1G93Hz_K9oAb4gsspClegxItpTOnrP5MbR57w8_pdOysunCj-_ajn0rZkPJfYxBM3tfxxJraj7vthDMtCFwxxk3OK3naNqM3jvSbwzz1TwdP9_b85G-ZsCaI66LO_bP62Hbgz9Whnt1ScO8enHCNi2GD2kvcZayYZ4qPmXVIcSeqZ-7Bq5H5C_hmruj7SFdypbNw4FP83tJ8nM8Lfjy-leBC5MKjaRRLDw9tsqmQBOVhFjFhMQWUfCH5I4Qif-b7FqEKG94zsMW7wwv1XNmis1cd83hjKaUSOdQ16ZczrRSgsiF4uVVaLiS5iI7OKAw5nbIP5fF9D8_DetkPmUsVM_j7rNP9QPcHHMmGtorLdid0eF9g9E5v7y18i9BzYtMiJbpx-k7Joit2OAmJxHvg/p.jpeg" xr:uid="{44F2EE1B-227B-4F53-B6B8-827226EC2C75}"/>
+    <hyperlink ref="X113" r:id="rId99" display="https://uc49fa0cbdb0be62073bcd6f37ec.previews.dropboxusercontent.com/p/thumb/ABf1Kpuxlbn7Dhd1H6AA0ahGqFH0aBb-uk7Vhpg4P3HihaiexEvfZo1mKOs20Fp0OVN8Q3llsC0_XnNU94t5oWA-c3hXGhmBYo5HHPRzyt3LXmd5myqUdXosEC4wrWVkzLcz2aIHTeR2-WKlK9V0LCiucUmU2kKA9EXnlYdJJ0AUmc91BDWXB-7rewc4qy9483DUOZPizK3DL91m7pGct7oMW51fIReNeJ4-ebMMt3PrVr3A5-P-EEQ84FmvQJfVRzRxOODyhpaCEFDI6MS9_wsplbW5W4ZAk5tKKk822uVfZZBevrp2F0BvgDim9LpDVhkitvEjLxMPO3c6f1LpLi1iJKy56WAdNH5aOQskOXcm4s1OBlQwIzU-7su3t6xEn93jGMlIGHLfNx0IPvCCKi6Ci78EjszHJnq8JdBQ4v5QFw/p.jpeg" xr:uid="{95A8ED3E-26D1-4F67-91A0-7E857BC23063}"/>
+    <hyperlink ref="X112" r:id="rId100" display="https://uc468eb4491bea3902454a023f08.previews.dropboxusercontent.com/p/thumb/ABcCz1iBA6elQb5edj2fL_x9MUyPj2UJ6wglAaeZ8mB0Zq9byVrsSwOzSjoRrGcciZ6vFx1BWrdAbpAzUgfrx1FYKulqaMpwdpMvU7HIyB-SVotjad5RxEXqGuh2Z_ohPXVZbttSdVaf0fsU8IFiHo110O3cWrX13ZF6VNT_NJgkRPiqosJvLfmKx-vqe6JXF7gEaseB-hOEDTFwWtbwXUQylqz4GIR61YHyEHbdWLWxBJ3MbUIsZCKa2VygdD5hSRwfK43g3biT3L9PZDujVlZgVo7CAxQOpkNw7UXgruTJjYndQwAyWkqEGe-nPpDxhtcbFGUUddOspw-_g19NeXk5I2o2qtnUxDmzRiVqKbswps12B_4dpeH0JKObFJnQvZ544l8S_IDRpAlDkrUeDkVYv-C4oUeasN-sgQAkPw7-5A/p.jpeg" xr:uid="{C7FD054F-99BD-48B7-B51E-0D75FDBF434B}"/>
+    <hyperlink ref="X109" r:id="rId101" display="https://uc7e58b0df394520ffb96a31b712.previews.dropboxusercontent.com/p/thumb/ABcgkRnFag0DXx0Tnjz_7wga1u9AmYLrMBNGmPROP8pu9NU0LZ0TD8dCEH6iuZsvmWUlyFx08hjXGJ-lUEWl_E4be0xivy5qDGHI-w6sxEbN6BaiHHhVdSw_mB5ObS-tES6kj2zDK5MfWUwgFhSub8qJ-YXynF4ltFsnxemxiulknjGzspsVyuyk89dclXz90pjZ-g0dlTLz6DgYoInb_WBhZcnIWjrwgMCTllM-1Jh9YyZ_Pu561dmnHESg6Jr3gLIcXbRpvZcx1HBsJshpsIcbfAQ8eBNg-iKPinio7VpXJma5HDEwekDRPtjC1FXeW8Z04TioftDh0SDStNavOzfAwHl6rhpz3O5U4nGu-96H6uJHToM1FWspqicnv87VPRBmkaKDiMR-bCjSmjH8t3hzeTDZSIZxWKpYU7wa-oWTsQ/p.jpeg" xr:uid="{6A0F2329-70A9-4B1B-B1C9-F073435951B3}"/>
+    <hyperlink ref="X108" r:id="rId102" display="https://ucc3f474c2861fb01650641440dc.previews.dropboxusercontent.com/p/thumb/ABcHtE7dOTUZJkWRd_6zz9qXsxHQf4_0ubdFjeNJdTMVr4hsdGkmDc5NweRXSgsFAPD_aAiKeeus4RaLNW7CCdMaHMxskCaSyZve2r_DAQT9opYKoRo5gPHL3mBhwcz1BTnSNR6uVqwiQ4GndVoZjaNm6OC3A_xnyLY9MZvfN7nKns66ufXhzTM1q4oyFxXxlCFG6VUZLwDX3GormtTj_0KCEXEwmxVRCyLmyYLzVw-uDx29tTgG1TwGH5c4lEv21kxJGtoruY0tENqfUUz4M0IzM5zH3p5fyrcqU2gKT-23MGi_CgdTtwT9MHF8G2cvkaMM0LInIloson-Qu5ZKp5k-ebPWXYiqAatPFIb6kTWyaNR1NvWQ-wyK3sOCEX5gNWGsjR0xmsgNoabu7-ZeWWTlfUoEAm0ghcuDv1pklw6z5Q/p.jpeg" xr:uid="{D95ED270-27DD-4F4F-BF58-0397A6FC413B}"/>
+    <hyperlink ref="X107" r:id="rId103" display="https://uc214cd81079fa3f5be4ee0e0fdb.previews.dropboxusercontent.com/p/thumb/ABc2cU7FcMIc31ShVHnOM8Sf7TKr35brVrCwYH4-mbALsQxhL5g1u-qJbYtnNCa57eyTqKo8TWOQGd3lEhmdJYwfSJKgUBAmUwlVOioksNoNlUj82WHG6JdihgVfUR4nFtOI08nCBJ_UOia4-bfChHt3VfBwbXtP76etO5JiJjBJpvJ5ab_bnABbSdLMJYiTtdpm8lkCfjifWQhxqZcLMjdhmFrqg4p8fpK4Ip_mIGxz3DX19aK8idMyy0hcAZr49EMa45sJ5Y1ZaMOXIYM_eDRGXoPfRgGSgvgbMzh1o-PPoIEDcvnkp12txpvB-h72AdmJhZFNtJNLo729M4ySQ-d1hc9qjZ8f1yb6tCVBLrVgaVyacoy9V4InNcw8mHPmJ_IkzxvF6lXkxD1vR5bulWNgayGBGsTfgdMIpro41SNW8w/p.jpeg" xr:uid="{E09F9CC1-A019-481A-BC8E-233B66BC4CA2}"/>
+    <hyperlink ref="X106" r:id="rId104" display="https://uca556c15aacf9c2baf478338fc7.previews.dropboxusercontent.com/p/thumb/ABd0UCMWdNhEgmzdJ3-vL3p79Rt3CLIYmTJ7a-va9Ptz4LYEIgLJ2XZiCi1CgI01vdmYE1RiafNJaJdkO3dK10s0h5BiGf-H5Z-fx0YRmQqLNPClgrTY_EHrZ7j2DT5clyM6NBrTmnwQMZSWepx6mjsFW16XriLSZYnxor9Lrj8CX2LYh6iK88IzMRkxKGjMvK-eD32xLbOHxzzzBoFeJnEmSPpN0jx7xMqbzMCuzdZczuwepfK2yavxHWUxjmrXUxky59F7gGhUTrUr-JYfPCQp7zIKVS-06qgYzt6G1lumzNnHtTI0xRVgqKdhIzSHSdY87kmMcsIv0zmPb6bnzwbap_nKHkBZYHqFAiNNNpuymCy14anOYkrZKKMtvSAg7r1YqnxCwVdBMz6AdDUmehcGvzOhp15wBqimlsiV6RIw5Q/p.jpeg" xr:uid="{607F734E-29AC-4892-B314-DCF981A5731B}"/>
+    <hyperlink ref="X104" r:id="rId105" display="https://uc940cf153674f0ce4aefd03eeca.previews.dropboxusercontent.com/p/thumb/ABe9r_X4Q8puGuNyktisc-OtZjdiygrZzSvPlWEpSef9P0zU_aZjAhC-6YjGqlJO74kluz-uhMTaFWfcX3tMT2yjqqAuUaN1dDPs5HM6T8iUt-buoIdnGrHf31HtzS_3otRNdNXtoFOwTVrpbNItHGg7a8AInPEi2lmHEA5EwO-WRCzL5Yu328rVeAFKnjdVKZaDK3Ea0aaDM_FEgltUPQp7UtfSz7U_KOLiwsngvW2BURdU1p4TkC5nHkfdJXpZdLgsO1_uNIBM_Dmcl3tBRfH_0Sd-1lAmlA5Ki4CfT2gfTVDRuX1Qjm38OefRiyi0iiey3i4QpAor3bMYkymVHVAqB1Zdg7yw1YzeunMJBSAiqQ9j-Zpqfu12uGNMRIVkYCUWW1CoNCaPjAMV7eCTIADtJdHngFqG-MFnA49yN6zvAw/p.jpeg" xr:uid="{B1928CCD-3AE7-4360-97AD-49A6713CA5AA}"/>
+    <hyperlink ref="X103" r:id="rId106" display="https://uc24ee82e6b0dd0b3f1a452135ac.previews.dropboxusercontent.com/p/thumb/ABdwNaEKHKUmrs0LphOhNJCwnhiGqTmBDsZPYFp_sLo3WsQWVk-_ZuFH-uRGsNHhgfHau73xC8xngYWnSvajBnj9hzVO2kqEw2F2Igm2V8QXPqb11eHOiT2i9LCdNOxp91Xupa4MnOab7jZqzhjFDkNfTU28Kp7g1-GcxxzScYcslI8dIUeK6Jaip39Y1ES-JxUnynLKgBJmzMFoHU8um6mjTBm9vZiOsdUFRO4a8JY0iqx96Du2_7rg2S3vto3Zx2nkEtkIZiN6rSIq-xt-7CyPOwutJ4F6lGDTDJNwLgvXflhSlpbph1wfIboVyo0kFbAf2Nt6UBo452CSs7CJ5dVO-A18LC6jt6ufg4O8EEIRMmB7TPU7x7VTnhAuJh7Q1h1iglNn6vGrrsvbwjgE5iWVxEXlDaVjnQLouXJ_Z5kR8w/p.jpeg" xr:uid="{A8D5721F-D5F4-40B2-A234-ABFC9D663090}"/>
+    <hyperlink ref="X102" r:id="rId107" display="https://uc561b3ba606cb2a8e43f284220c.previews.dropboxusercontent.com/p/thumb/ABc5kFfI1d6Rr09uwi4UpPZ1HHBk-n1A8yCctr7gv1E_wk63KfT8nBu-JsUsAbgq_Pet0REKr51ixL0qyCRS0FulRc2ldfLl4yGHovv4aTDao4mpBRW03LWSQMuOgLLHi5hyfZKrbdgLbd6LkxswOM4S4I9WRaHenc4ZuZojgaA2TE0IIPlwaHoQgm_uQlCb5Isfshu_jksD8K94TXjarfpcjjbVbOZEyT5svUc9p5NsvPRcvK69O9w0WQJBS9PJlJLMq2CyDmfcDJt-2adrVGkOJD9D_TW5wyCbKipSbnos8w8bzjPDMX6eZix_MR0wHT3FoY9Dj0kSCnItW8lXSzPYwmGsYeHloho8NnpXZT_D0xy2UdhACKOQw3iTGCJCANFrGNvwEW2zmYPQjmOVmB35mBqfQOhsu1xpckn7aqkbxw/p.jpeg" xr:uid="{6776C090-F277-46CB-818B-5B19E587F7C4}"/>
+    <hyperlink ref="X101" r:id="rId108" display="https://uc7cbaa023146e7d14fc365bf5fd.previews.dropboxusercontent.com/p/thumb/ABfwTQkaNioWE1_B5dKGm7WWjXQspOw0CJFvSL0A9t8yVQHOFuTwyUvxahluqW7llo_iB-6TJEhZGWnIuGiE70J7j_A7MEzZNs0V5KrP_NrcuPlkyA0Yy7Cr_sVo_b_O6c1RYJnEEHFcA3QDgzYrptgnc7_w3nxukkN412DDKouFvuJ561-R7drOexSwwA8hB6FWRVi9f7O6fugIGsY2Ss8rzsOtDVA6EvEiK_Ykjl3xEK3YoP_Hhn9tUDOCz9PchhA688AH-kn3rqQKWgJd8JRssWJFeP9_PFFfmLdy352e6UCqEqooAu2sxo5ijrgu8rspYt38SGy8MOPtjcCwvimHwuvoIJosHrUd3IyziBDJv5iFj_1WQOXpJ0EEPUb9dB1i_3fMMeLe0oOmdGc5OPBmn2LWr2Z-CWK0n8Qbkm9x8g/p.jpeg" xr:uid="{92A8FD57-60FC-469D-80B0-B2DAA5502680}"/>
+    <hyperlink ref="X100" r:id="rId109" display="https://uc0450cdde5830db8d628e12afa1.previews.dropboxusercontent.com/p/thumb/ABeLYrLuMZxMKXbR7rHoBxX_pqEPJ-q1cn6adAb-qINNp-4JrioC-FDLhQqzNriEr-hkgzONFVdFBD3dM_PTX9Tf3FbNWMB5ZeYxItSuNEGs-zA8Fdwma0if8mTcxdCQRZzIWx4s8Qoke1hw9TX1fCclSzUnRfi6BBCbhuqmx1vzDX5ykDTri3X34P43R4acMZZ1JeqZ2ZDMMK51paT3SgNQZrGDTNH19A9Ftba4Cah41YPZA-oVUXL57HNpsPMrNodnTGsyE1zb2zj-lHokTmJvxHZBgqjwmukBJjzpi34bM9cuWIdr7vY-xtWd-KPGN3G6HkRHM5GUawllUYYvkdsLSnXgbh54tf8PmcYG818EtrL63kX4VauW18YfVH8xviu5GTs1gNLHQAsk6JlAG5npe8euvhjv94hNyPAsSRvZ1g/p.jpeg" xr:uid="{B74A7BA9-1E71-451E-A543-8242737897ED}"/>
+    <hyperlink ref="X99" r:id="rId110" display="https://uccc3a26dca8001df60984dd46e0.previews.dropboxusercontent.com/p/thumb/ABdHyIJdJWfVK1QfIBOTkE6g1iw-P41KDeuYrpTaWVKyvIogoBI1-NcnCOQczF8FjGGWqrb66vAlS3n1WfRNJi8U3QsBDg7BtO9m6k4cq3Igq0rQH-IT1gy6_2V9x_vCUsAc4VjWqETZWUoJQHTluLek_lCcwhzaxCSmYsg4Y5uVsMnzbVYW4Z2gq202hfULKV2TZJ65HIVg0930WeAU8QqDaS13f1k_-CT9Tt43Ze-ul27oEq9LiJC7gJaRwMUYylBfhd6bejvt6A7eK8yU6GjXG-xlGHBOViI9FwXmUyvihKzNOcTv0Lnr6rrB-bXW2mH5CSnVPeETILpNg--0PkZ5ODm22IO4HP0iorBdniRqehpvKFpte6sdUB0msVJVYtOVyjQn_uiYnIWwcIq5KUpY3j8rLOlq7dblJISc6Gi7qQ/p.jpeg" xr:uid="{5EF8E0C1-2877-463D-9FBC-8D1168B812B9}"/>
+    <hyperlink ref="X97" r:id="rId111" display="https://uc7e90520245e3c6974300e8e7cf.previews.dropboxusercontent.com/p/thumb/ABfQJwjz0ndBca77lwbHjTw6CXW7n34JlZYOK-2NLX13NKEdVQuOlqcf_jCFl21M1y0D-JGoB14nnI_XWv4OjzaoW64dpHwAADKrMW3imdPjapxQCIswFqqO03PDsDYNihEjp0krNKZ9bt6kDfrpBcSpgWrX7fbpWx8xAbYLnioZht53R9AgAbBQmwnfHmz-U-zQq0LTrE2jVMIsFelQVxaGjtLcIe8oLznIL97KHSGEfh_jh-2M_XeXbH7OaF0ywA6WPtbk_XH8gwRqaI3ls30DSS7_FdqcZzCZuC5zwQBtPh7IINEOrnFFZPhKwgvCleRZ0EiHKP6-cHlyRUwjV7g7sQPcM_Fe0uMqX-RRQgvC53kVzrKLXwq0NSPv9iXC0wvMJ6RmGxt8i-g3oj_RCEaoZgdycE1rfgiMtsXN5EnGwA/p.jpeg" xr:uid="{CF4026EB-754D-41F0-B7CD-EBC39F3D2EA7}"/>
+    <hyperlink ref="X96" r:id="rId112" display="https://uc74fba5b81091e184fb23167601.previews.dropboxusercontent.com/p/thumb/ABfG-qciPGtY3e4C91HIEHOtHDxP3gSugijkd-ZWYfbg5hFRpvDbxJSMsf7Vai1fYhUX0By4t4aiZWZi67x4iq-vE30dYCMhlrLPgE_1GkmHqTfIV_hK2vwgosycysm7sZ1FH_atnsnlALqQ9MEyVMnqvNHm64WlQilZqqP1FAXAKHh85VE1wiXQb2CNqVqIk7XZhDvlsShsQqhw3TmOBM2GnkB_QquayV3TrrcQFYHAHDJYx2lmovJOpX-0wTBw3pqSbkttXtY7PVlBrcO1kgIDaTXTlEBjiMTXaIksApjuKgui6sPTjB2EYA7E0cbKR2ZUNvZjJD67WgS11vmISZgV7sw1sLt6WbhreFoUPWDfRNEZRQpPAiGuOZlYIs3j4VkqpClm_oprTkS3BdzolZGr1eckzWGfPVmBCBnDLALs1A/p.jpeg" xr:uid="{C054D084-38F1-4239-8EB1-235F88AAF0D9}"/>
+    <hyperlink ref="X95" r:id="rId113" display="https://uc8bd7896662a8fbe079bbcb02c5.previews.dropboxusercontent.com/p/thumb/ABfbKWCtZazIAAxFUR-JbHcmfj8bJBKRb5UkRTEaiaHdSDKitydpPb4RL9cP9rBugCSum0XRqO2Xbd34gd_g64pSYH9oSjw9MT03AqHU8-wr63kO8r86ba2TM77IgAK9cb0Kb4m8f1SgSiO1iP1KoNEUsfAX55oEfMccTBU2za5KmfX1LhwFQrl6-zRoeAxWmynC-5dJlAli0COpKn9eQe2eGlvhAXhweOVJFMiMPrIp4rDeUJRSVHQXzGQ1A03sAxsDbNG0eDOWYf9OKXvwCXMT1ig7iqLGxvD-UYA4tJdd2ZmEJWIqR0ZpFHJrWbCVVDyNCyzmdiy8Nii9VdBEdtidRwTvgY-fJrND-tzP2FEiZJU4eVZXPGHumGQLrBsKf9K6NM9KJnngJsVwwBCPSjsqqeQ8IYxllnMqTFUGg6NPKQ/p.jpeg" xr:uid="{7726A98C-C1C4-4308-8D8B-0E3E81DF8B04}"/>
+    <hyperlink ref="X91" r:id="rId114" display="https://uc96b9aff1e347771330ddb7d5d5.previews.dropboxusercontent.com/p/thumb/ABcrKpRblMJ1LAhez72-JeBwtjwp8tLEUgy6Rwe9Hr21TIe38GAcD5PsvdTPNWSDYWIcuqt-4_JQEXQd4Uv9IbPBFY-52NnzuKW7NY2Zh9GwaQbB4ydnJgqM_bB2dltIBH3mf_XX3x3a4NWwjLICcegFnVtmmLYm630PxQ7rAnkI5QlGmNvHsn6Fo4bZzqTogolXvArSx3sGr6AO6FCdzqh2jv34YMIvbD2fIIOpR7HXIDwDIRrfZOHuqzejnuS32-miv5uUNkoGF-5fH08kE5e3dxQ7O20urvKJkrnf7U2Wow9C37K1IQAcEIFBzjHvdQHyzyPSABE7IiIb8qVQ3VLMeiEa67oAVzlMsfdOsAuZLVa9KM4W1DuFHZw_-7-_DgylXnd9jRRau8WTkc5STI8ZfGFKWAuXZqHnQLr_idG1hQ/p.jpeg" xr:uid="{85AB384F-6C80-4043-9D67-C3A2A2446ACC}"/>
+    <hyperlink ref="X89" r:id="rId115" display="https://ucd000e2a95820e6afc400d76825.previews.dropboxusercontent.com/p/thumb/ABdjM1ehD_u320U9zM9FDKMtdLF9q9S2pVERjmoLxjcHn1bM8tqIWo8GpCHkEL2uvKbtsEcR38nLKmWF_E2awuqfCrAp6jHHS46M8S8iL0NpzkA-u5aTGkXEke4zyoxQFpLainG1afM5N_Cwm7YAZBYSL0g8EpyaESDbdsa39If2luFE5l39puCJ4_bBb8AqYOvqUjCF0xhGLmZv7wD9a4XW5JhofsXGs8stQMM1Z0jkUEjylpNZ6sVTYEhyQDSE_-aP8WQZkBR7T21hEwF8S1sRdVc_z-_50nACvjFe3D_eF9JIPOun54ExtLSU6q6rinySL36N09xXDsbJyGylo2io6X3SXIW7clRhtSEPT4lTQwS9pfkPrYEePsUQnsCsfuXUkIcHeQR9nZs7deYIWU075GdsPT63TjjOKUpEafJ8hw/p.jpeg" xr:uid="{4D07E9F4-7ADC-48E6-8FEB-EC358E349BF1}"/>
+    <hyperlink ref="X88" r:id="rId116" display="https://uc39ace3b8238f7870dda6fe3546.previews.dropboxusercontent.com/p/thumb/ABeZbrg-gwG7sh_59zcmQ4WSVsPeU8sEKZ-K4MsurCtuxbVcTBIgFh_15o2F67B1q7SoX5El57eQ96-ntdLuvPiIeSkd4pvr8s39VPaioBmLGEiJoYiSzJu0n5PpInGidp35Ob-UHSdBykNp_g_g5H6i5JLd3F4SkQABSlttlygwi9dHqz7kYW2FBw-yd2dzD7Gf6diIpo6hopuHoCPDk6b2CI1TnKScF9Kp9r47f2x5FJA-ZK0_DT7u8lwD-cVBVRPYQnVs-nNiAURCnVPXhMJD0pkzPlDU8DjEQ3zYjka0n_bjYH35D669TVF_XeTvQlpp6kdgRRqXYS2qBOPdppRv_Y2asj3llI6vofRqGo85Gq8VZm7sGCo4Mq3l4GZ1mS-0CYKZb77ypSOhJ4mYUcP65TYk2S3AZjltvkivaNHIIA/p.jpeg" xr:uid="{ECE7F08E-319E-4786-B9C1-55A08CCBCE3F}"/>
+    <hyperlink ref="X87" r:id="rId117" display="https://ucb53aa7d567a677ff7621919f85.previews.dropboxusercontent.com/p/thumb/ABcRp9azTRbl07Aw7DfUmyJOaiF9j_siFqhDAYCal9_Ri2S9zXth_vxjNPendvdFlrZORvxVPeuBgbYj3Vng1dOHGtuw-pWkl5uZUfS7G_avlj-5xLVf368_R4FhAc-cjjwx8JcumFyNUA-FVSx4vzffdVv801d41POGYM-9gnUYKy6iysg5OsEebjmx43qJrrbazitMgUCQrrRt0H43m3EYjLzkQ4zrscwgfKxmQh_UT5x9lVOJTMyIE6C-viMDmLqQXcIUHkq_Dnjl7aCra7qxipj0Wpfzo9_CzhobygwvT8vkqswFh9mJIHHIyt54bue4UHdXBUnI0MQH1hMK6GZLN01tzlYNmClWe5ESFG7VDpuYkMiNkM0xUPVVWhum36Dc2OwsHEHbP4Mi_5GUexhM4IOOa9Lswq3Av_1O58-73Q/p.jpeg" xr:uid="{2F08C331-F85B-433A-B111-272D17CA1EE4}"/>
+    <hyperlink ref="X86" r:id="rId118" display="https://uc4e9f43815ce453f6302cace789.previews.dropboxusercontent.com/p/thumb/ABeiv-O7IOLMwziwR6zBgbiKUsC92D-ktVaPoUM4UoKmpDchvtJnub4HAHt2NKgHgl-3Jsmc53-cgr3kB0ooRz1_yx0MtYSQqulAqjboUpkXrMSk9g0KqAVLpN8WNlGEuaaxU6VJfX9hz3xKSRow4Qd4sosWpWVU7fUaKMjby3pt8EXYkor7VoW7srpIJwzOS894xoRfO3_R7bXeH5hhwSAAkKVpUAuI9I7sdh9RZsD0HynTtr5dv9l_Lxk5egxdwPbV9NU4BPmGtje535lE4Om4qieDGMSycHF8CaOS_3ic3tM2FbhC6T5iznVHeIr7Gk97IsoKWPq47Fuv-T3ZGkPxYLxmzMJcHKbRytDxTVjibJBXtJ1mL9TL_qMXa8q8wEecwI-bIuPVom__hnQXMYFXOD2mGDqkS4VBUBUBdcitIg/p.jpeg" xr:uid="{3B932A81-0ACE-4CBF-8998-9499220AD805}"/>
+    <hyperlink ref="X85" r:id="rId119" display="https://ucee90d2ec2fcd89db947f4786ff.previews.dropboxusercontent.com/p/thumb/ABcEYrLFQ5tiU_cXBC_x660m-i2mbuVy9oNi8jPbXL7vx5Qvza2V-4x1MKrNfLVA3VdtybHgOC5fECT6f7BXzxBCz7iM7TI18dn2BkncCdxJLFUUsa9_QsxOzCoEnxI3ArkESr7JxI10mtkO24dqOZWXanX-33-ZkmFrjdLYOrt5zrs6W17kBC0hML_tKLcOeygbefF8YPswO2SvxHEvdOhPaIpQSQJEPWWy8FU6FjDUsRR-IiLTEjy5djdztd3CrrcLnTSZ0L-vRWedDQAayPR4GF-BZu7cc_8a6c2Dyi5o0NLI-gDAU1hjGOgRxJzsmss92RqiCT2LWws-wTmIXoGZUSPpOaI6mVtNBq2tYuasQ6dp87xEpx2DTDvYej68I1aCQgMdFyYsnchvETDpgfF01qMYhCDUKf3OOrQEJlYzTQ/p.jpeg" xr:uid="{1DF1DD02-055B-431A-AE11-7B8AA1E86EAE}"/>
+    <hyperlink ref="X84" r:id="rId120" display="https://uc8469c499b4878b9ba8a6a46aa1.previews.dropboxusercontent.com/p/thumb/ABf7mn6t39xyvDMWdhHGUJ8ZRHFtUFWi5BUieJMNa7pq8I1g7Gu2cyRMZJ6Vp9cLlo6Lqwt9yJdTqSeTHVuO8Ix-icIoz0d20XyTS2EsqpjwR6xSku_tYJP3s5wgM10_ljE5pjcLD-x-OjZmYoLXoYhR85L7UW6X0isoD-SzBRmrWSGCMTVjrwpo-DYwPVloLHfRqRNXBLvY90fEsVM6wmrjjQLsYyC8MLQ0f-ot6GuWgYLbQNuRgfRvc-pbJ_yaK-5JJewd0e1zl8geEGbj0aaC9Ve40OWf3_o3U9n8cnQIFjxAwSNf_YRTV0xIImtHEBHJjpitaewEKys6mGAOmMjdytBHWattQGUikO_u5w3UZNVSqW4benEHmaISoCncipNTyiN9jx5Ez5N4S8RE66xaGJZIidyMRnBMz-zT-Xj6JA/p.jpeg" xr:uid="{B559C6F5-7266-40BE-B767-5EE379D010E1}"/>
+    <hyperlink ref="X83" r:id="rId121" display="https://uc29275d8d46bb13a1594645a0f5.previews.dropboxusercontent.com/p/thumb/ABfQEjwNklcgoQhRMZE_EUyzxzcj_q1HmnIclR3K7g5nuD_9SZ5WwdAQC4_-mjw8aP1Y9DBFCGIR5SVSLYVOE2ZF3-Gzf4y0zc9HR6XBbvy-zo72KOBp_4sKRTAIGO6jsh2ODxGWu32N-zjaRpukAlRR3wY4wxMErZgh7DfoTSEMbxfBhUHCnr9REtkJ2r8TjSdcSsYRJ54Ajkp4YNxbO3Y7nu01Mh1iufmY8VmGF8xAafJOFva_B8w-mBhVnRR1fHnnP8uW1R--_fKFxgbKhTLRkRSgFspf_jIQ-U63ht_vLxVbPoHJ3pIykGmOQT4w8xm5B-klR55rYCbq_-QriJsGkWvTlS4eR5JNYY4ntt2bKzjev05pvnYFKj_nrJanWbGCeHuXm42wpNR8akbfwzayCpw9m9uR0r2MASaBTSUr5Q/p.jpeg" xr:uid="{1B33A65C-8757-491D-8EE4-2D1A7248B626}"/>
+    <hyperlink ref="X82" r:id="rId122" display="https://uc21c0d12b07380bacad6c136c4c.previews.dropboxusercontent.com/p/thumb/ABef8aEkanJmpzSbx9kzrBCtjeQutvQvi2p_1xFVw92WTqRaw7XkECXgSjd34kocghctzYH5jWQGHjMDKVyl_5xLfVeNEOxpK3ZktPeD6epWfiKTlSldGhGHycSdOcNVfgdZzAAtM1bmFRIgdkuuDSckKbce2TM-W5Bu_bgsLCFLW4z5DcBJTtpEquxVrio0BTFE2OzdsAPTzprmhhQzDjWmqG-0QDH2lzXMY0QvFdVYjHyk_gZZhq_fAhdQ1AYDjRxhm_0b09z95lpCA6VgJM5YYol4x_uxuQKjPcTuiwz8nAAzKV_P25js2A-BBznbReeYCym7zZby-O1IVeQ70IOxXV0S55f4fBFi5BERB3x4q1ou15h-E7CE6XFTol1t-NEe6zvgstyjZjVMlB_cY05FtziJ173_UTptFvSAwGQjnQ/p.jpeg" xr:uid="{07082072-035A-4F41-A0F9-6BC2F01C87CE}"/>
+    <hyperlink ref="X80" r:id="rId123" display="https://ucbc454bf97b12d7ceb293031874.previews.dropboxusercontent.com/p/thumb/ABejEvOrfugnqEOOcEyGcUm22-EILJ2zaSSFdhaRkYQAcn8ueCMXci5SxjyGzZkLwbSdsT38-vbtKnMTaDb0VR7tah3GD2PL2aATxLxJdNh7xmR2g-Wvjtfwo2tGoPfHNbW0vKKdCidL3nrq-0RufqtTs2rjXUwonsHlCx0YmQugIDNPFjJehAKZvmTQtRWaBfvHLa5a5UNM_F3jedcIKXMv-qs5XcwzFS0kIYtrZhsA58FD6Ov5MseY2cgIcrL4EIBpO0mzkjPrULXKmbyOthcKCB0Q3cJltK2RaJBs-creg7Nfzk7b_j9OI_1JtbIYdJSL_jb75cdEIUvMeVfNON3kkUZbNIyhUAo6gUauKas7rOYQtLxWgmeegqm0divORPwv8tU--JU06FOwC60oIyQoY6Ck2VkcUTD6ibZKR_o-1w/p.jpeg" xr:uid="{F871C301-D7C8-4FDB-A755-6F037136C6FF}"/>
+    <hyperlink ref="X79" r:id="rId124" display="https://uce2b7795785b131a9a6b15b4b6c.previews.dropboxusercontent.com/p/thumb/ABdWPwp7XVja9_siOWp6A3EsFIDGBPyiTy93pj9ZuXiJFK910QOkliRPYzSdqCmArcJURZ9iEBnOlG2DT4DO4q26s2MtRWn3Cd3pKzYhAGZ3Q38YcnLfWwnVkXeuUeFvQNOWhKqfTzMxaympAP5nalOrwGFVmqrslXT9mC8lA_p0gh6f5J_mef6lrpKkOyS6Xzn3kiiPR1w9XUStt10cnH2HEduu_nS8WGv1Ov6HTSQvBiRxI0oY0e9zqxxzIms_BSu50DiISTIqZ-vSenmaTzGVty2fHYeTwrDFY7ng5GlWhyHQUF5AUUPX5OWa1KqKCXbViyga5ZSGJ62QXr4CFkG7ymR06kNNYQURiJdjyFoe7dq6F_tkrzFLFo7IN5o_oEmn24SRU2QFiov0gY2IjW32CcoVjV9kl7dAHwuoBk9jnw/p.jpeg" xr:uid="{FAFF5DBE-1BCA-4405-B3D9-23A027A154E2}"/>
+    <hyperlink ref="X78" r:id="rId125" display="https://uc29275d8d46bb13a1594645a0f5.previews.dropboxusercontent.com/p/thumb/ABfQEjwNklcgoQhRMZE_EUyzxzcj_q1HmnIclR3K7g5nuD_9SZ5WwdAQC4_-mjw8aP1Y9DBFCGIR5SVSLYVOE2ZF3-Gzf4y0zc9HR6XBbvy-zo72KOBp_4sKRTAIGO6jsh2ODxGWu32N-zjaRpukAlRR3wY4wxMErZgh7DfoTSEMbxfBhUHCnr9REtkJ2r8TjSdcSsYRJ54Ajkp4YNxbO3Y7nu01Mh1iufmY8VmGF8xAafJOFva_B8w-mBhVnRR1fHnnP8uW1R--_fKFxgbKhTLRkRSgFspf_jIQ-U63ht_vLxVbPoHJ3pIykGmOQT4w8xm5B-klR55rYCbq_-QriJsGkWvTlS4eR5JNYY4ntt2bKzjev05pvnYFKj_nrJanWbGCeHuXm42wpNR8akbfwzayCpw9m9uR0r2MASaBTSUr5Q/p.jpeg" xr:uid="{4330ECA5-B44B-4903-BE70-E3752F764C5A}"/>
+    <hyperlink ref="X77" r:id="rId126" display="https://uc788feaa3a8a2b39def5a66043e.previews.dropboxusercontent.com/p/thumb/ABdkZuoZ-OKV2d-EkXZlAU6-XX6qDOk63QBaNAzXEQGNJryviIG826oPvh66KRDyaTZvJiPKLJ9jwoAqG9zSAg1hbKMzhQJRU8bUU_JX8fjTbzN-3rjvMNNGWK6vaoNkWkxCvcxLNae11S242bYUBhvaKVT-tTTW3ZiBWSO0gLiL_x8LTzzP8v_A5tm_IkpbvJ-83OEjKVDbdrH9pitom_8DSrdwNqw92ZBlYM5Z_VE219dOWaNVHcNAgY5iPvezp-xeHj9H16qy6XzEamIZv9HginStARybbcXB3iUJN3Do9J_3WvwoIIW6YG5OdwQLlwb-LWVTxf8mrl_ABK99p_nhKb-T8WzHpwY3YLYz9RyqiZe57FVs8j_TX78hxOvvliBX9IU3mG4u6Ffi-rUKtuBvt1vUzZYBcgky_eLGmAijsg/p.jpeg" xr:uid="{E6A63257-EC00-47D9-A37A-9F9CADD41EE3}"/>
+    <hyperlink ref="X76" r:id="rId127" display="https://ucc5ee67eec19705a1aa38e681bc.previews.dropboxusercontent.com/p/thumb/ABf0fZnYSwzeVbF_LH-KJA90rofrmSF-gM6aGDFrqwy7zRp9U772ygqHGU-Faouv10eyRb68Q-YyQzVtGrPeGQO0tp-FI0k7qKImzKfVypst6c1k4v4XiXjdqDtoUMYrGjDkCn1s0ADV-JkdK38o8coNuTghJoC7TaCcUztBvssEqnvWIJyk-SLhdhX2Tfvp-5QmtBnlT98NoUNS0Ag9uG88YGT7GntBejVCK7XjWfYrIJGMG8lghn8tFSaJlI7wqqpJ3E112lWeXCxE40bDOOLuIvXOlV_qjFfzcxZXyz_44LroXZyMtxrzAFLQRr6n_2KAGDb7YY0W6TnSGRQYfKkLo2xg4NTWi1YodU4Wq5hLB59QPd9eZMjx0QKUOVvdo0_HYiRUSwnAVAqutpzQ7He659CqBv70bKetuF3uB6FQ_A/p.jpeg" xr:uid="{BE033589-F894-4688-9277-AA10FD6329BB}"/>
+    <hyperlink ref="X75" r:id="rId128" display="https://ucffc5d1d3c28063252b38135a46.previews.dropboxusercontent.com/p/thumb/ABd8S709hRA9CtfqWfm9xZDyRWGDEXgAFOiC1xyTB1Z0yJ4KlmesqVmswB2NstQEK6LhzqShmeh5B5ZvNMYg3vEawPYo5XS8JcdkWHtOzb6zqEHsAEJ4yzG5NOuZezrVgHuiqQ1ntMFqP8wQ3VkWbQQmzvPTijO3KgrQo5PwIWBxzmK7g0AHTBB9-Tbrb0a6eFc_BPTnNq6WtaJjHt3TyI9i7MoyFOGJbSDtnZ9cFsrn3JxcSLZvKOhsyTO-sb4ZFpcEXufnGO5YuaX2DsVhDE_OAaQrBmNR2BVmt5R8RsjzdIJ14sc88M8wQswJPwGg9YsHJ1ZqMPvNVQgGJt_DEBU5fGqOc5bPZv7cCEUhSH82MrV8QZQB_6vq2WEGmTlRA2NVRec61djc3OccU-4WlQzNafzkq5m2jjM6SwICrdW09Q/p.jpeg" xr:uid="{5EF50DFE-BFE5-4F87-94D3-A0E894F0105D}"/>
+    <hyperlink ref="X73" r:id="rId129" display="https://uc83429968c20a3cc962d81543c5.previews.dropboxusercontent.com/p/thumb/ABfxmJEsKSkHKbCQuOWFGaJUHZzDebP1lzd4nvZ73ZPEyPPZyOtD0EWpoWIyG01NSg2JN_9eAaZjuYAm8rcOXRX_bUDw_T0lta6QQ0hb315P055bPhzmyVwT2FZNZbesa46nqGwxFkZffu9sr47_pY0qBXbyAY5aRM8QWetWM3MuZSoqTMly3X1O7Y-y2ywIwG_LcwaQaCZyTg-gM3-D44dtGHh65WboYM0R8oJJqbVy-gxmUw2qkwOTx086t--PazStvTTCM9Y8xUSU_3MpdGZYl2FGdIbn_kfKSGUHe8GRvIKBBgnYTI2CqLnk2R5iUMCllkgaWKuTZy61SU4EUkuBeQSOi8MuzOykRYWcinCAQ_fY5-fuEfQwcNLq5uEeN4Jd2uG6inmlX3o-cURRtYkQIFPK1zHu5RMeShXsxs02EQ/p.jpeg" xr:uid="{4D80B73B-B9E4-497F-96A1-A5D9B54E10C5}"/>
+    <hyperlink ref="X72" r:id="rId130" display="https://uc7513b31a13f14f67ba48e8063d.previews.dropboxusercontent.com/p/thumb/ABed6XjhcDRDoXDMfIVjErksm_GhvHZVTcf2Ghc3LZAaTBCDal67pkj70NqxH19y6pjuvXYJxwfG8OTcVFDnVThfQ_y4u8ZIMBwCOqMpSikyOZu8K2kRDVOHHoOn-wYZ82ZKiGIn99c_8MIyJRi7Jkc4X3o8qHOmEslZATLYi42QtKo3DQ6XT2yBLQRHR1FShZESX9pnY1LUua_0OpjGuuHN3qUp4eV0y4k9NrCwJXxTgjp4Fd9cYOVQizU0qCzyJJsY7iKLaRvWph5TUL7mooXbCvKqQzKX_vVGAwYhtYBtlPPKsg4qtLfzUbUxLmkCRqWxy9g1Vb-3yMwPv7LQQrtTpXeuVjjCdSgmeYYDrTESa9OD7Ts86CuhxIz1OHkr8nQ8BH8riPQ2043WUGTyFz_CjQp8TUr54Nv4XIo7udS08w/p.jpeg" xr:uid="{4C98B7AB-1FF5-4254-A3E1-8A9EA4ADFC6B}"/>
+    <hyperlink ref="X69" r:id="rId131" display="https://ucf9e4f04a38eddaa75371ce841a.previews.dropboxusercontent.com/p/thumb/ABfk_UYOLIgf_w2dxAXzDyqEjFn7C6JQPnfluWZzUCfwZB-TI2DZPWR2arFvigcaFpn35i2m4wL68VuSQmO60U8nEMiMvyNO2KTbjA6oJOt1Ozt1zTxrTc5Yk0qpSa_anktE1fWhhwprqPaThBxZUPMce7QJaRudPg52_7dcvMDQ1lHUVeu4GLY5x-lyhnTFsXUA53Rm4J_ituFipHzGGgt1lDD3Q9MA6HLMnlFRdl8-yGScTGohLeoTzDldSa6TnRWT2VrxmfzC3-Lw2qynb-7pqx52KosKxsAuvmf2Sk1HiiuTdyceeY7VOqyE5Ecqjf-gCgKvkxHWk5cMmB73t5f8tKCjhwnhbdbZiy_I1X-NoMRqZ8q51hTHbMVPIKY87qED3iVtbuU-8uhVht0qA0HOyGVY9WcDWGwjHpOMgTLUjg/p.jpeg" xr:uid="{98270D36-7AB5-4A5C-A8EF-372D179F230E}"/>
+    <hyperlink ref="X67" r:id="rId132" display="https://uc3b2151db4e51f764f5f098b2b1.previews.dropboxusercontent.com/p/thumb/ABfE0fFqsUXHOB6ILGSY9BJXeHlJa7jNYNVXfl3Ifvjy7RQQnr_MEQ5o1RPRK6XSlKi3C7gNmIwF3cnVIwdnHQ9iQNilsoAnh8XWhXfZhdIgDlENbKPtu4B9KJVRxAMudXqWaNiA7JICgKyjbtmnuLGHxJMuc5QPaa58fpCmdsSfigzPUBn4hHxK5mBvQKbtcBQ2C12M7XGSP0iGN2c4qYa5CdhjuZLUfDo1YfFJG-gkJFB34Zz_m62t-AXdAzo0MddvI0gJwO7MG893NkjPLkCsYA8kVo5aWdmL-B7A2bAGSnyV-nfCBcXSM81pffW3PHuZR8nDFR3yuyOIxF7U1c1cY-QemPFJnqiYwQefIYBbtc1M7wt4MntOrCtEiRGzOlrQT9E-MjkA5O6Tv1szuBqwHzgWjFwxYpKlMxzm7Q94Yw/p.jpeg" xr:uid="{CC120B57-3596-4FCA-BB22-D676F114F29D}"/>
+    <hyperlink ref="X66" r:id="rId133" display="https://uc868df3f7362fb41d16e17eec8c.previews.dropboxusercontent.com/p/thumb/ABeU7JGZKxbX-yq_Nv_T8MnKcWzWxSOqrxS2m9RFCCdbylPAXtpBO3EKnsvy_ycwljblQB9isyR_x68m3Q8lBVEUXlAg7YOAKA7P_haG-R2EOCePgoYWWqyl0IXwV5sZ4ezJ-WwpIUR1MgdOGyrdpOPiThkjt04lpAobOqVUIFeM4_GgeKwCZRdXY4uoOqnCAEeCYpdRKuurFJr5R9-PLhFRgV4Aae7JEtEXIDN5UqVjN4icZatYZfjiFqXjxc3UyJZdO6b8IEvXsYA77Fc9PX0yoCAC1iuWMTfzv8RBi2jbJ9eLaTsEadhPeZeBQTiozzg-KE3HOY2EOAk-_Ijt2kMD-zpwXoOeaMRR3T_zYGbyrBKfV6hvByxhB8AB-FIliCKJszAzpVbw0hlrBU-UY_aSQlYZ3A0MK8ze7MHF2R2xJQ/p.jpeg" xr:uid="{B721B94B-B2C1-43FE-9A12-D7DC7524AAD5}"/>
+    <hyperlink ref="X63" r:id="rId134" display="https://ucfd7523b16bcad4d01f1e2adbd7.previews.dropboxusercontent.com/p/thumb/ABeNL8tVlZ88lepY1u5lXFU5ocbfzmDCthEmuuYuyMUhRqIjAxVoNlOj5AMrX2cyfbrGcYQdHik25LzaS6HieLs2PSFuDBLN_g1PgBU2SSg5a2b1gInW6QRzIwphLwkA0EP2V4RssZaPEDLhQ3bx1bt8uceBPogmo4YCdh-m95RsP0FhdTiSqj8VVt-CNDy-6GvTlK10xDZkpufjoOF6yuoOj1bvq292NLRs9VnycMA1YSV_eZNlbHo94H0-hr3glqHzPJSqkzYhWp7CsmhTs50SZENEmzgXPqqjBkttIpm3SmjU2rvUpIGqsiGsyUErw7MBaKGn88UWi3e3nbXn7iCxlECQN9WyWVsNaHpiLJwVHBu5SOxPP-FF0UC6v25gD5NwChV3xrjyVEU3D1p0bfrQK8B_vtLPSg-NfETeGlPrLQ/p.jpeg" xr:uid="{0448023F-CDCC-47E9-9DD8-E559CB138298}"/>
+    <hyperlink ref="X61" r:id="rId135" display="https://ucdf3a59536b5f7df87755759b8a.previews.dropboxusercontent.com/p/thumb/ABfC8hr1u13kCvZE9yONgSxQJJ_OOj3R9Ehii2qhaoKeFAkmDDw6S74H_notSlLTW5UknU00ECxUTHf1b4lqjLls3S2bI9Wdd4qkOODyOg4T_6PjMQY6zQYosld50s6uGsyTCWHyGCrjKwDYsKyIhcMdz3lgtqrDCQysh67hgbmkKp4VUkDNT9IgEwYDbtYg4I3PBBkvx6v1gbtzHpGt65KUI4Zm2AjiDkqK4QZadydVzPOZfAi8FJRkWQ6-ta1isyGDiYj_CqLWjFPIdDVQi7x-eTYH9mWilnCEB1u9BHQPvgUGv2XhwmrJVT6UcmK07v8JSk1Ac2AcYZq2nbvQKrJj-NDjtsLLo-IiidM3j3OAV9N6ND2wGyXoQqNeSSfmdHBBlpav-9WlLrYdwvxJSI4rhwnJVjk0T2dntLh7Vd6ulw/p.jpeg" xr:uid="{CDA6CC84-E3E1-449F-9F4F-372B29F62FB1}"/>
+    <hyperlink ref="X62" r:id="rId136" display="https://uc7b0406223bf1daec0413cca967.previews.dropboxusercontent.com/p/thumb/ABdfMztxLH15j68nBwphpOaudt-KQehuDvZ_lIxW55GDQq5jKAntatU8nfDBLaKkTkIOCy-EKk6zbZfVvP-93hkYEOVKQ3zZYiJYA-OBwyDobkZbXH-_O2EQd8LY84HN_XgKTEn-9HSJyX622wS3zd7n9hm7sS4yk1w6dCkqq_HkqEHbGK1V9i22xhsElubbo9oI9OOpZfWU2gtcc1imtKXuvwe63FtCaVPRZZO9hNHBjWlKDjHjsu3CZatRzTfpWSHdKq28apCOGQ5uE5n9QLhRY7NBp8jHYMQc4BoN142RDsFQR7n9cc-vz0044gO090PwQ5mD2Kwo6nrXhAUzG79RalIcnzO3O1IywGPA0k7RlNvM4L-jqxRnKL7mq2CssbsECnJH1Bayb3FIwAozLISu3-BCAWOFU7YUIzdBJJReYg/p.jpeg" xr:uid="{8224C24E-B1CF-49E7-B6FA-7FF7F532398A}"/>
+    <hyperlink ref="X60" r:id="rId137" display="https://uc3df08688d681b3b2e338c47b9d.previews.dropboxusercontent.com/p/thumb/ABfSQmyTVbrAy4ZCkFCFd5BxLUF9A1vB77IHVgc1cCjqA2W_m7IJJNzmS_h_UQ8gxfxBEJ1cUu7UzrVWGjdUKqtYa1A_1jcTi79NqH2jSepjyCQis3lPCWp5W8sFtPWxgXsigqAzyTN6MTlJTME6GTDc0y_3f0jn5IHfbgfRRJzn_ane9xOOQx2LtTuljRPwaYOzoIyvtkSh4GWZJ3sz8NA_hsxC9Gx4IwPK4sA_TkPxWfA-Yhatw9Okz2OX6sUmZRdKqge_lyvNzw7dQrReeGvlWIHEg80jUbayvtez1q4WDD22AOpQ64ZE9FYHVX5sb7yYcoJa-ZDj5jDQmIqLQiWejtIxS-DfaTfDtYkr032oOZrw0j_iO3msLaaeRsN9KFyFkIVqEuBFcC9Sh7p4_hlw1DIWDf4siM9OUZf9JT9AqA/p.jpeg" xr:uid="{0B8EA285-D80F-4EED-9A2A-ABB70C4F5492}"/>
+    <hyperlink ref="X59" r:id="rId138" display="https://uc30eec35611120bbb7c4913d0a1.previews.dropboxusercontent.com/p/thumb/ABdlzNu9zWpKNyZ8bLj7b1cBkB-qvd5IovokMHMDQrdgy6oQuRazxTRNv4QCtfRb0ia0QBbgXxbsGg4XwxyQ4l3CGVxfou7CxOZWemJnk1q8x_msQ8OClAy7Y7I_ANOJhByKTPRzpeltMrFrzCesCbn3qgb_TmX_i27eXjlK48SnGfeMWNQDvvV4-VnPBoiAM1VGOAlexn5fBV-GL6d-FztISgNt3W4-q14jQVst5lB5ivNPFOJpyCYqBbJ56pHlBjwmBJ4KFX8iomcbJCBGy1yfpMsxtXZos7M8YFz4--h5IpFP98-FuWCKdYpm2Ds5WuNbezjhAsux5TqMNTCd13vqV6LL2k3hG7inVmGT_k-vI_B1sbUe4TJ8trV8YEvPhfu3bsg4xoO7rYj6MMNfdh3yXpLhFkUhHql9wAjk5iUePA/p.jpeg" xr:uid="{2D49F5A0-59CD-4CDC-9395-2AC9402B01B8}"/>
+    <hyperlink ref="X58" r:id="rId139" display="https://ucbf64dfc33a0d3f30fceb766e73.previews.dropboxusercontent.com/p/thumb/ABc0KNZ9jcREKi7dfJA7AJq8vlYHBjfzLpezZIOSIqIQ4ranqbWqOW1a4EQfKVhgE08W227vWrbVZgWAhzzp4BvF0f1Blzd7G-VveIzVaA2CrbJ_d69nDE7bt4Y17e2LNdCB88OANoSe7BVgjN5TeUf6xHyaI6mItxZ7YYmhCwZLw3lnOpvJhQwjageeOa64Ww8g7WKb5QS3SUj_xqbWDMAavwNxTJcOIr8axxykF2uYrPZ2cBwcf3P5ub6a71FdmMWt_jVXLjcB6EGv18EB0vpfzYq8LTAQkvPRc40NYqjMTi2yL_Ivt0rTrEHlwo9NQk7sj5Qo5xGXBeBCyicDhU77Nw0q7AOC3HhboDJ7vL55lXeVhwbD_bM80zX5xN9XPmSpnkG69kizRw7a0ugCxrnu-i4gdeKc7yQx1Tpm-tHGQA/p.jpeg" xr:uid="{C6E7008D-49CD-4758-AFBA-4B313601996C}"/>
+    <hyperlink ref="X56" r:id="rId140" display="https://uc4b48c815b9eefb1571c0018181.previews.dropboxusercontent.com/p/thumb/ABeMJXnmSi5Dd6xaeeeKDrZB7akeJOY9tH7ZiUy70zr3RWc1fcIA9Dj02AkLsMlRi_M7kLeLK4YMcOh47HOYl142lfTMZBryzO8X7Walol4I2CNf3rfONH2WWfXynLALaRn6WmzB1Ji3SKG4F3YWQvW8eN-C5mXfs4yoyNan2LqPCzefqA_cn3ZPpzzUeuUXPpqz25ZN3UAaC9YKMxEAOdUr2J66ixtYpR8XphxDiilhHfiaHYimIIAAKTjM53U1gBQWBNJihM-TX-rcbZg-UOMz5S5rdUlIzC5Eq8NY5bBUfZj8rFTVcJTcqtJJMA_rIsZ9YWDavS7J9TNSKrhOhdxPDCi06i7pfY0ScKTFi9t41m6KWVz-Xj84ijVgHgYTeCTfkOB0z4eoFTGpQ6qNxC_bnR45yWGcQPy8aYLRLUB4IA/p.jpeg" xr:uid="{80EE5416-E322-4DCE-8218-57A8551B7FFB}"/>
+    <hyperlink ref="X1" r:id="rId141" display="https://uc473ab1d3f024f3cbbf33edbd68.previews.dropboxusercontent.com/p/thumb/ABd35-HlKek3gYJfW_-58F--BG8ejvOla5SfBjpI3pp4JgnezXwiHyrKTOkc1XZE7R7M3wnT5VrsO3ZpV7esgIbu9F_uT1sE8XUfhESBUDx-Aocld0ab_UwEPmwM6EnA-vRVepgtGjLdWctheSViJtbXYEgnAbcVFNtV4xVXMYZGnbRe-GMOgbcudYMEe7osbUBpB_ArSTyGTNJyGeHLJF6jStD02dzStybiWaTmTus81lBPVDw71XTFkp-xplaSAP1OD4KYRJLWwjLioHbpfNf4Jh7TTMqRpHABZ8kr_KM3fYIUTX4I5kwk3rHe1Ic9EAdvCDtBdyuFP-po2IlEMDaSSmHjUVacAsHqrVVLJTQrabv_i2BaybDIiuLNRAZFrkk/p.jpeg" xr:uid="{B7EE33F5-2EE3-4F92-B76B-E4BDD4E7FFF2}"/>
+    <hyperlink ref="X11" r:id="rId142" display="https://uc92cb6266affa5d3e9769dcf1fd.previews.dropboxusercontent.com/p/thumb/ABfY7l0ZYU4UOMjp5GsNhGoADEAoEL31Bp1kstAHTajUhWLGAk2tZym_3p8p2JFeFpvu3TeZccqkc0FCQsdFQNOMGhuu5_qwQgkNfeUH0ZcHCbHYWy7aTdR1bhKD7o-zWQq48ExkiI2qBqGS-oND0PRqAdCkpudaU23sL0qdha87_Q0ErZ0Wn5biWboy3JO11oUSSq87QTtCsuk3WRoy8i3hsWpXcTv-BavmQFbQw3YBeB6wigzCBxQ0fGOei1b5ZQUQSIgZikApkLs3TLmk4I1oqdiHnQMWV_eek3-o2dAIrF4XngHKhmw0qBpMAf1qIF3m9JcSj1vmihNqNkWR-mUz1zWUJALVtydoVINXTaJanN9pYETdvelkzfeMusS4Z0E/p.jpeg" xr:uid="{738AB59F-8CB0-4D31-AB63-38EB01BD1900}"/>
+    <hyperlink ref="X10" r:id="rId143" display="https://ucaef174f583543ab756e8ff877a.previews.dropboxusercontent.com/p/thumb/ABcXBicarpH7Of3YzUoWYdgdDRi4ZjzIk0YN5dLOaxy5nUjiPbMJEGOgWmOKSmfOXdYBLyuaKe-P5xF9POuBSOa_vI0RHyz_FaZzy9dGWeJa7vtz-pL8xX46EJYqz4o6KMLIDCW7e_n5d5SsKixonXnNhMybyS1jXJcH3BT9-t2c72xb2nS-rPMgP9YuP4YuW1g3lSxTG9JuHOzm3PJGR59ne7SZaeIZFLR9aAWj2PUZm8-sKyGSwznXyAvtmnbmnaC5B_SeZBfC2_WZi9ksFS7-xIHeMqv-dK-3J0ADC3IRy1lmvWmfirxltdEZnZshLbDpo5RslmHL0w2KNyNJXByN9j856Oy6eg84Df7L5IxXdOR8ax0ozB573N9UM_f9pNs/p.jpeg" xr:uid="{CE2DEC51-D12F-4DB7-B7BD-85479D5B3F18}"/>
+    <hyperlink ref="X9" r:id="rId144" display="https://uced6fd332230c3bf19d74637d1d.previews.dropboxusercontent.com/p/thumb/ABf-baCszaI5sdiapyAmAQj_wSZ8FROmDkmx2iOa2LQc_8IuKJguxLllpUc5KGbgUABdwPYkTGmjpZ3WisvoXMFNH69QZSxI_aE2bLfvZMJIG2EisIouZX9B9N0l0uWeStisI8tU0byxJG0o3AiF-_vgLBA4Za59rJeBdDZsElPeJ56nHtg68sXXU1TXucwIR3mpe89lTj5ni3h4a8psOA7XORzsOYNI8gvcteIue0jxISZWWU91oV3ofDpa9zd8OPV3OqHNDe78EPDYA_YQawKUT7tNZ_xCTCYLYwCRGeW2lCe466tAC2YXPvmq9M3udpXLRrB1RJnoMm5HGFaB7UVfsmcTVWJMrA0tY0p_d04ZwqpAc9KgwMM293oNDQ-EIRM/p.jpeg" xr:uid="{7452294D-B302-415C-8693-BAE3CE8669E0}"/>
+    <hyperlink ref="X8" r:id="rId145" display="https://uccf4644f81a66fceaf58e01db71.previews.dropboxusercontent.com/p/thumb/ABcywBm5eEC3iAqGI_6-2zXII7af5ArFqPZuJZs48yenhrrXzfvhOjEyDyWKFb6UZ8P6NqaWkcZqj8YVwOkFo_7MPdaw8u_AmzOV1ig_rbycO_k9PM7zOPEg6jMMRbqK4QJlJAph3g-e06jTT78vUjJzlsuQelTCjhmxyG8UskvZWZa4rsiae041QdACjWVky1IL2hQ7KGQpE2zpV-YrcZJj2Fo8EsdWD8UfNuwR_58dx3D9tg5TMwzPAVe5VxxuH0m2GBeCmIqMlG20fXEKBskDdTCRN2Nn4e56G7waRsLrqPauFVfVUS9BpV3sUgzMnm86yWAE019rBoA7K4bUB3ew0BVIfNpnKpkKLkXAE9Q3-8A0dQHhEhNh7LX9iMxzemE/p.jpeg" xr:uid="{FF3D0E82-337F-4CCB-904F-AA627E46725D}"/>
+    <hyperlink ref="X7" r:id="rId146" display="https://uc860f724763eb5cb06b9d45f458.previews.dropboxusercontent.com/p/thumb/ABcC8X7UzVhvtB-LBC2rlqTQnbeOUXNe1CoJITGDdA-xReaPCK7GatDcmrGcRxBDKFLt4y3kk2F7bomW-OQx8b7gNC_dR3oiBreV6wrlNR0f8NygS-Sp1C6f5jBHIU1aMJvmRM4LdgKo5rMbImq3aC9zhcvN7r5wokaD0lkUH6lx9ENa01N7o9PeMcseP03BWOCzXFhht6MAmNsll1E7g_46oL6-u5l5J9NEAV7bz_8FcLbAgEjzONS2u_and9Gy7TC5Jt7jUxJ09vpFJVDgflCR7Xki8c7V-MBYupKfDQb_4x7xpylg1dtwjAkVkSg65FXiVEQMG8l0KmPHJhoxe557N-Gh1fS2r45ijMOsMD00caH4DZUUVu1y92mS_5M_VaU/p.jpeg" xr:uid="{1330D882-4455-4F2D-9B81-2B41D87FA10E}"/>
+    <hyperlink ref="X6" r:id="rId147" display="https://uc1320008bc34c5317b6b1822d2a.previews.dropboxusercontent.com/p/thumb/ABfhKXlBCJDrVdSiBn1Qh-c_4QMP7ztUIk6Q3WH5YOHS_sAEQnCNKfyS3IBf4kQIU7UabqN0xeJp8mfu4DzWanZVwG8Xr_-GR7VSZjnNMuhex7RucKykl4BtAfOez2kpZYuX0y6IyY4RoxSGcncCjnGKguFAsfy9DN6NjNnv80fGtEABFGYk2x59mjAgStzGaGPnwL0SN0UeblOgSsGPN-hzwlJPGvByuOFcKyMbpyGLrPpy1DTUh1Fsfcno8KBytzPTsdMvNnaNprrUbJ97SOegiH9SrxrOKrtACWB_1s-4A8HlhqPNPUMNkQM0g6VswNMpJBT1uxFuuZATsVbRf_NMkdWc6h2qykTDPtHymBuSRm3zKxIRmWN9CuOVxCa8A4Y/p.jpeg" xr:uid="{A934C2C9-29DA-4A47-9F30-431DDD46E7B2}"/>
+    <hyperlink ref="X4" r:id="rId148" display="https://ucc148df5b06313032c7e0f97ef7.previews.dropboxusercontent.com/p/thumb/ABf4uk6v6d7VKHC_Q-SubXtWRc9AXqFdJJkf0O3j-VkbjDRnHoqUsGIEIR_zMS1gxtxWoCyYJBUhLddJsGkagrPocSkMCYOO--qYyzRbjsms67klia86qCXAO3X2HFaj5LIgf8ZoW9T2WIO-CbLexc8Q8ItM4c4N8cQXu-FUZsOMA-o6rxf0SSD9fdC1ZF_UtdaGn24ceDYjOnNCBHQhfY01OqrW6SCr8wDibRcmjbjhz8EfVGEsQ2wO49hTuyB89SwzASNNRc3scK3A-DSpzpudBjghyvS-Lifun_iIL_OcYYTb-pgd9WfoZFlx15U7uw0mVEoXJbLXcV4RCmHNDXkgAQw0owElzn_Ma_2V6bi73bAmnR96vUlcBIr94-RmA_w/p.jpeg" xr:uid="{3376C9CB-6471-4274-95DF-4DC16A1BAD2B}"/>
+    <hyperlink ref="X3" r:id="rId149" display="https://uc15704c31ef47af00a5100e660e.previews.dropboxusercontent.com/p/thumb/ABfLgn4nuKS6B58Y8iha9_NP5pFYu8UE-oBUf1XLXvpznfbTyrmqGDC12dpXEjh4pDbLug0m_XY_M8PSq-Vzqs7y01_V1FQ3PNQx_DDDy4NsrfdkPMzAr3BBDRT72xZKwC8lhFw4y3Wh1vSmyh3giSVflqfNKRiJ25RUlfNqbjl9-hr0kGCdvqoTbYfMosSKm66_EyHaA6w3OurRfp0EBQJSiOCK_fFxANOON9HICGAM21Z9YVKFj1DLFL2rS-olkazswzEtrafk0ZCXs4ed_KwDkPU0gk2LQ-nvNJdONtzJBhGtKCLWaJFH0SbohwUIEyBhNHDLyjILX8uYXHtTYS8JNiP_kfHV7uRPX97nMfUx0EMbmNZHSDMR7oLeOIMinIc/p.jpeg" xr:uid="{67B970D4-B8F0-4BF7-94E4-4D90CD154DD2}"/>
+    <hyperlink ref="X14" r:id="rId150" display="https://ucbd6e7d45ddd17421102e97f896.previews.dropboxusercontent.com/p/thumb/ABeTYMw30DLWY9vkX7h4yC3ZxmdiCtNLTcS1NRSRZ6kk6JPrrFiMuseh2-P1INuo96aKCtbsPl4YbbG9wyET5BfwUxJQe3vOLwOEwC67_xCKaxCJ3uX8DBVz4CmbrwqbkUuX6ThHEvmWx-r0f0wftvnm6SCl0iRrGiCO8APA5gn_032gTSwT-kUlXgeRmNn97Vfc1emOkIWFi5Zp-vR-OdjnVofdGAVlf_i1cf_ceP56p8lD2axHWDR2SWTc4D-4EnqLxigWroC8QWxRBdAhNfX7ZqW9AiJpMiPtzMCeLQIa9b4cc2lgPdeUDZvo2f7EOihk_-iJKMa7iY79ZB17oE6CbElu4Jeu04b26SZ9_QLJj82EmiCRw_kcIKOM5s6NSYY/p.jpeg" xr:uid="{6421C14D-A736-49F9-B1CB-0ADAA7B810B8}"/>
+    <hyperlink ref="X15" r:id="rId151" display="https://uc08263df58fceaa972604d388fc.previews.dropboxusercontent.com/p/thumb/ABd_I2DRoxRS8ST69OGSPeeADEXe02lMpiS45psSxyTjpICHJln8UASXGNUbQQXhfFGDHzf415QiE9E1EcE183v4x4FPBu9JxGUpjdzck24-7hEYbxmU3-qPa_vQUeTmArXygqCaMMDoe2gtoo7S4Jvw2U24xwJ1bSzKaZfIaCBYkG_2FC3-gaXYZTudlO3R3h3MXUtiS0TVVnKyDvCeo17F7t1XzsRHsW9aynSHgY9QeNxbIu-k-KKLAFTUxxWnSUmipBFQRsgBKm9sbluym2YVZA1c4J1IzdBQunxCu0wGempjH0tSyC04COtX1ETOKINWwDnfbFAmMt1chnV_Scj_QKAicbxSIYAHYf52UgpM5XYwdKQLtjf2QXKQ2c-ReFg/p.jpeg" xr:uid="{5D9E6322-4007-4D52-A800-E155EA70F992}"/>
+    <hyperlink ref="X16" r:id="rId152" display="https://ucd9a971f66696830c6121de558c.previews.dropboxusercontent.com/p/thumb/ABcLb3fcVnGTg3daAk_e_-25Eu75E8K4fDN4LGRD_Ey8PNH1dLHojua-zwbrcr2FvA1h9WVCw6QBUoevNezeUixlCbFUB-t-lSplZbzzuZPzTby7D7PlKlsBUUKDQ7O_9l5aeVdAKPlOVseDnkhBFJbZP0GnVXoekZMeq1eO5GE-cYS39vfBwCetw9-FBwnbIZakSLcSmnzkBca25zIwdr96muQjss_Ih0kUYFjiF-SFfHyxua-sJ7stxeWAWTq5ridQDfZfbhdMAk9rBFMf_G87XXnXZYsD-9a3ycsFoifNi6m98k2J0iXn_-GOGBaYUR01qua3ii9VaXiOFEWv06EXoURVp3aZ_EwzZEwn8mPKbQOIu0TyX2oz0yO3ftVZZQE/p.jpeg" xr:uid="{8138BDC5-CF94-4573-95BB-5AEC05F38AA1}"/>
+    <hyperlink ref="X17" r:id="rId153" display="https://uc4bb6b3c1f5228dbdb0476eebfa.previews.dropboxusercontent.com/p/thumb/ABfrkKHt4t09k2TPRjPdR44hbWooSdwJCFeG9SVmarwHBZE2eskrPCe0wTEmDm17Zugi_hK1iKWQd40HsHVUWbsny1tEtQm2KkAUd3iVPx7MNMriWrgNfIseBeVwYy2j1L11SZjwq_5OSbGnt45CNCfU1nFxHn7WwJ4RP694nTFe6if0z697J1Pb0mCPjRLPaNf8czNaFrZCBCruORTJtecpCGL7Yd676CtSAdp26tMWJrGl_ID9_6oooq7348QgoBayqVcWmzUlzNFraN2pVMIhbnY8ztBRP2QjePk1EP5KojwLtzKtWzbGjs1vXNum0TdnE9YJH1LTVV7HQ4Gxuz2MS-1Dl9b8zEU9Ae1S0oyIUlqmhf7Rjn_olkSbkXVrwWA/p.jpeg" xr:uid="{F9E03A31-42C9-4992-AF44-D9E8F9FC3A4B}"/>
+    <hyperlink ref="X18" r:id="rId154" display="https://uc19a682a333de699cffab6bd721.previews.dropboxusercontent.com/p/thumb/ABcr__zGSNirOGxergW7PZT4A3irfMOAMdQcLo0GM6ZTQ0QgZ2jjmmY5tFMmn5jOjyEL2tMUzwk12O464pv4GV28bFF7ZipcQRLajaM_kkn8vWJUDVM3mISTnG7Mx2g__lzFy0aicnxjy2vh6Ot0UarX1hWlGqf4Dh64stxSqFblcEv6udPMTzmveBgaeN-D5wWHwKQLQNukaliIh7FQ8mCxypsv7YNlG5hlLnEflCwm9wQj6-KWHiCOs_fCbHnfyZOsoWaD4kR4WwRx5jpAe25Y7lhQ16iOS24qWE-Jz9vf6ct23TpG8vXULEPiB0a0Euw7rUjKW-D-xrUfkaUv1Bkt0WujneReUTUkFauVtUNjd_F_fsCC0iy2GnI80YU_8GY/p.jpeg" xr:uid="{B6A0F97A-2A2E-4731-8DDB-DB5A054C2531}"/>
+    <hyperlink ref="X19" r:id="rId155" display="https://ucc6da03eaf0e3e046311b662740.previews.dropboxusercontent.com/p/thumb/ABeihBhH2xERpTg2Uz6cGsbtn4cn_RR37jnaAHzr-VQAU4RmU2DkOirJWl1HCSgHZguSgK5upQLkyufQgzKetMMgw7drIknGKWMs1VwMmRBnNgDEXOXe3TAvqyDVrPCiPvXQKuBwh55PU1FjlIiMem-ZTDinb5f9VyeWxGCI57inWrDDj82OqoRdPejJw1W_sipUdcS3Q94M67_BU1SQ6KSnl93kj20TarFR2RV6bXGS7IIDv8BHfkItN8yv6UgHmKySdo3rrDCsy2A8560LBs8YRebOC8gQ4UVPCUusU1nzVA70iwgtmlgxNdBsKE3VR_8NQCwgL6O9_rEE3EEtQxvkRXFPktCrvTsS7Rdz2L_K_JgPdizHEeVmX6wiikIdAIs/p.jpeg" xr:uid="{B330420B-12FD-4222-A6E4-12E7B8DE1484}"/>
+    <hyperlink ref="X20" r:id="rId156" display="https://uccd98bbaadc614b0d1c0421fcea.previews.dropboxusercontent.com/p/thumb/ABdFSqk-eHyqtI1aLWLS67Nlab4MZDJAPVc00G1CCLwUoxGuzEb3c5cfTx2RfmKovsMy3zENIkpZOqoSiNofvqfecnNP314HFxRs-pAgiGqLDSbj7_Yb0ma0C-cf8TDvDjR4iQyu-Eu3uJ2gd71u9qAG15OxbhlEZVjmpqlhbXlFQPJ3zwTQ7A5PZ8kRpMyVUCDkklr4kYeeexmMF0UMBlzcGSHEpBPux1kY2eKlROw6NpLrZT7TNuzFjhqdxxHGUHcwM9K2jO0s9q8BSMoC81z3-8aV_NsmdkUk83qv0Rgc9pxbNHB1UswNAjFq7Hol6ehn79JBRjTa2E81_Z8qYL5rIaCvDPqtF1qC18RgST4C-65o50r8JIsSbXgp355NoKM/p.jpeg" xr:uid="{9C078962-F19F-4819-A088-EBA7E63F1EFD}"/>
+    <hyperlink ref="X21" r:id="rId157" display="https://uc345ed5ed39e24ffd35e7e64f65.previews.dropboxusercontent.com/p/thumb/ABfjsLapW6mM5-nbh_yGcFS8YMYkM_y3Q4GAtilBJq0qltSvXO_V2wWgKtitdICgJtn7NSpvGwuHsYMVQcsYHVSTQSEF7NNEp70eoY4yaNW_WA0I5RrlXg6TmuFvD1fVoDETfJE4qRnyGbbjopXHK-o8-ZaZ4X7D483hEDfmuSG0AaZB3MMZgVebuYpR3tyZSXnToPcAatFKd7N1NTmtBLgVtu-4nWOitk6Jvx7KS8rO98eAOyYg-8sgid3bngK_hzOkZ3FqURaIh_J7R7TNqjAPXiCXbqZSnaBjTHWu1xkm9dCkqtlQMJTsQfdmudvbJyK10l9jkLguncjPoa_Kr6-O-YiduZacKHsY1TG2GDFaPLKmkN0sCVay5Jj24G28NhM/p.jpeg" xr:uid="{C397F06E-4B3D-4386-B979-42D89D925403}"/>
+    <hyperlink ref="X22" r:id="rId158" display="https://uc2b79bb46a20601ea0a9005caa3.previews.dropboxusercontent.com/p/thumb/ABcswFlE4ILcoEZ_zpUQGw7aESPpcjyf25nKwBuYh81bb-2VI9SVWsj80zwK4FKvM-Vu1bUKXdO2Ns4jkIaBPzcGBnPfeHCqtxcOouKmQXVFdc0afxLP7zta1pYKaEnMb2dfinHjHoA1ebEk_b_XHbYB4puqYZ_2Jw41KtGA_tZZPyGm7CWUPOUVu7ErcVp28iGCXfJAR-GdYgKtm3FHeqVr0wEyY2sDMHdzySy5o-M4GuUaGfOsKUyDRTgu9LVRPJkVNtEHnuZKu_hWIBkmzyfbpjQUA1wPAmWKh2DIfm5oaZP1ASVP5bZuhlyp0EytEhdnbAlkv3Ds9isjWTTDve1nxjOZB8dsW2VYi8L6S0IEn8tjkQ0IohivMzBDhzvZS0U/p.jpeg" xr:uid="{5E6EA57F-2CB8-488C-85A7-0C4E4E7AA5CA}"/>
+    <hyperlink ref="X23" r:id="rId159" display="https://uc592eadf8510f13e4b97074faaf.previews.dropboxusercontent.com/p/thumb/ABdTq1Do4fFrME_wh2kB_HaNfWJEUdhkZAE0hpBwBAudR4zAjhEjdh0SxpUTajGjQU8U6V8uq99kNEvNuLjqgmzr6KwZQeBzCGLe-g8dLxYbtixaV6U-CnsCRm7_BdzA0NFIWXB0Te1t29WoOHWCpNQhKKf_DeC5XBV3jrrBYGEl3-7Rq3f_ok7gLh424ODNvjuqgwjjXbGCmo4JPuX371p1HflN-PDs2OcxurgbWsHwtJHrNzXV400c38jvL4bKnBaRL06gPvyzek5zB4WoQXKqYE7W-3K0qyP1Kg4RaU5-jghQAsTEwKVi1kAaaVERXpiP4rzJN0PNTF7VLjGDBmqGu5SfQom9OInZQCUcjf7fUPeQTWk0O64yxhRJ7OFp3Jk/p.jpeg" xr:uid="{89241415-35C1-4E21-A6F9-D2ECDE2E5272}"/>
+    <hyperlink ref="X24" r:id="rId160" display="https://uc10a0379f6ac2c632d278e42544.previews.dropboxusercontent.com/p/thumb/ABde3rEjudZrtHDZAy7eVJTZi1GUnyCEjx2YJ37u7iaPmO1iQkpIe1u1lp19cLwc6T09PC8lGZ3rf3q-GOiA4oqwB7m3ORQR8qS5UEvJVzQ0v29_J3wVV8o7M2Uqg4yETeW3tfMK8OjuixxuCXnKg2zuwY1F9kLIlAE5oy2GraFxSvEAdpwxDCkvK7Qj2fl7bhT4eMHyJhmSxnzXOvtoXp1LCjzR4K44dZ6YfxVI52Nh9Nb3ejV8pTZRnrStFaDFd_guolUrKdQfE1iFxwo--T8pi4DI2XVufjS-YMlJvvUhhIkcaa3dzQEACJT1ND1vBkaKK4bETx3K5mu8sUeNV0TU0BKVeL7K6IEK_6WuAl3EgfFkq0RaPmXEPP7pCml3Hr4/p.jpeg" xr:uid="{53F15031-845D-4AC8-A140-32A5CAB1E681}"/>
+    <hyperlink ref="X25" r:id="rId161" display="https://uc2d44ad4a301a2ef92ff0739f7d.previews.dropboxusercontent.com/p/thumb/ABdHeAJj97hKkkZHg9NfbaDynhGw60VpuSLK-eZD9ZWdqGFuh1FfwojBAlDdq6nDlcaTZADWzihL3XR9q5jFfxC3VAFouFQpYu5HqiJ1Y_dS7cge-bKByJHZ2vuRdTtMmdQ_Xu2fQPK2twYqqB283ym1Z76zdi1-HzaAaJI9OvdlTQfJFgeixzC9Y_lXSW0cbIcIIZAAbnP_XNAALKUVY7WN7bnNKANhJ5uR4XOJ6K4e8xC9Vg-T9c03WLIoe6UYYN4Q4IopsyA4veroabFg9uzPcvDtnWq2SevNYUR7ZlYSoyTzU3qfLY7dmT3VEGSNXHgRRepG_FhpZDHMKJLC353XOF0YgVVUaY7sNNYdn0CctR1X3PKPpo8_9Wb0tsjyZOk/p.jpeg" xr:uid="{9270680A-1B25-4EFD-8167-345651E4C62F}"/>
+    <hyperlink ref="X26" r:id="rId162" display="https://uc5f9904111d3ea55b60b4143c79.previews.dropboxusercontent.com/p/thumb/ABfH8e1ccMfimWukD7g2Ahk8gAFcEJp-X6zPDSD17spYlpTT_vDzPs9YHsaUTKTr2M3iaYo3AGI6G_riBQqumy6YVZJCHavjD5Hbt9YV8UhiRv_Zu7Iah8fJY9FOqJ902mFlc5onL9mN1vJcsgqjw9qWL8jhJAi-ZxoUvxccIYwfrMptzLO6OK2zwPF5zvIJ2qUUkjNNvuybjrE1gsWjB5Q1NJJmyRpblNj0k0cAE7kryDEB9T7yhpXoRWt3sRsE8yJGVTtlPBbQqwWSey6k-8CIuI6dVsBbfIVzbPGAJfUzTfuaAbzjhX6_nRjhTUD89aqFdLATvY_PqJ3OCy-vTnKsUlsnItxQuhtOcSq1pqFFRw70tDThF-OqWr6QqBLww08/p.jpeg" xr:uid="{CBC74483-74BC-4E30-B2B6-B7C0F5656497}"/>
+    <hyperlink ref="X29" r:id="rId163" display="https://uc015a5380f769f4855e21c2ee41.previews.dropboxusercontent.com/p/thumb/ABeHsHXtDdx-su1lpGhhok6ZUK8fotSjBBfvH-ONfS8Vbr-t7IAO1QYGyAZ2lDOVyeAgnEVX4aB6vrDaaw1p1JXGAceCuYQkpK_v3YQY_ssBIBXKLQxW60mILiLkbuY2F5Z05RNp8bLjyd3gr8GrZocd575bSwLj9uqn_RJuYCbKP8hPHK4YmQKeFm2oY2hVRDNVAuz1EIyMRLx7WL2EwvxoePthxQ1cqyn9v0JlOTu8LwuoTiZBSK0VFc_yCJgRDaED4VmiPQ8H6GT_sdnsMu5Bux6WD54ItYPZ5LtMP55lU01YiNkNYz4_etBLCJnfimulEV_IZxTJG1swNZjLz4x0X9Jg-qiYGtjlWF0-XiDf5j_Qn4USPvmTX_iZhKFCzvs/p.jpeg" xr:uid="{FC98300C-42D0-429D-880D-48E91974FCF8}"/>
+    <hyperlink ref="X30" r:id="rId164" display="https://uc12acb66874afec202097dd4591.previews.dropboxusercontent.com/p/thumb/ABfTT9ii_MHe5YrmU_uiGP-J7ezlghj__KhpuCZZhFwnEgFjwqwhu_StH18j0Q41_uuq69AZDa11Xjpd8oxbmc8LXoX6VlAwu1LBj2EYe2bESts0xu2EA_e0QPap4oLgvbV-hochpepcCWCpzREyFu1b46tY9wThBGfaqX6YRYjNxtIwzxyOHN_1QXo4ZynPjPPvc0TD8D-kSrNM3aVkAam2gpZVhNqRx9hMDNZNtRMoXfB3DpiezxyUrSRQO_evT_RKp6MZwe6mpY_LSBfX8_X7I97JmaMAnw64zMERXWZqvMW7gGXWJZsdLhoU4auYsZlJrPrQ_tKDEVC50YbR8HJ4hhRO3JnkLgB-upREdf8__oWqtBZ4ISjfQQmSdObWynE/p.jpeg" xr:uid="{A1AAD653-FD3B-4A60-838C-336157071A4D}"/>
+    <hyperlink ref="X31" r:id="rId165" display="https://uc9d070795294239004b99a90d4a.previews.dropboxusercontent.com/p/thumb/ABen-JYsStSoO1-ysZ5YNeXxwu9wt8d2LpQPC_DNSvBXY7W_sclPq7qW_XW1X8aPvvSQhhdSrvrrJVBRykOvHTcqJHJwA_6mahaMlGPJQMEU6E2S-Aj1E4V8eADkB7gj7i06RlzDCPvqV_4JbyTMik8hrGed7Bm101hNe9lJn3IDQz_l25UjEjpWG_gZhKcKkJEEBM8f3E8FvprPfCwwbBNvD8c4XPbIFeCZyLGm0tavByEltpwZZLc419RZOB-M2UFARoksOotjBLeOIDPBU5a7FoCsknhZzPAq0WYs3D7Z-lBt6LRJlCs8Yo4gWQAPMweHdGBOpU2ufxuHCuiIEqxR8Wp_t_u0_ba4qgUbDrCyIy_Ni_I-sK6JxQOzNmiEhEk/p.jpeg" xr:uid="{8416CBF6-3642-4AB2-A9B9-8B7F7B9D3089}"/>
+    <hyperlink ref="X32" r:id="rId166" display="https://uc5653b21c4bc4c0a5559d6f0a6e.previews.dropboxusercontent.com/p/thumb/ABdgl2zQ373P1oZbyF0DD1gaHUZQV74_VaLHkpZYP8i9KMLxnQjc_ti9lylW1szmqSVfryr9dBsHVwQYsRRR6u8MOcFdG5_7EVaamMk1Cq9MCRcx0VINATJvp6JdZG2CETm0AVIY0soFBKO5Webmtu_hLyLIYiU5LMiRcfbnUHWigI9a8sdu7H1CnA4OtsyNxUMfZgCT1KJPxg5DzhrzUGJ9R4eSYqyS-XyeKrT14N4VNajYTTp8VEaqNxFblyU1mxEgSf00IJeu8EghFz8cVqR2PM9gPp6HQwLJ7gjNx4cXnZJOB0g7O2BCrXP2ivkqSSoRKsGE5uSQOuHerd9Qovz7zkgLhIIjura582tyae3uFkjr1VQeQ2vJbq8tIhuZ56Y/p.jpeg" xr:uid="{47305F10-DEF2-429B-8A74-550DE010CACD}"/>
+    <hyperlink ref="X33" r:id="rId167" display="https://uc78db1fd14f1d1206fe0cc7167b.previews.dropboxusercontent.com/p/thumb/ABdBe2OTfsoASkyiEA8EMjaFblapWk_0Z6DVP29u1hWaSdRX3xJZrSF9rUfQX0i--QysFcuzeSxdul835MzMOoleum_dbNRPUJ3GRWRNeDrJQZglyBQIBEScLtVbevsUPUNIv-8laLRi1Q0nMpeI_kATW36XhbboTDA9kMXNrc3O5ykIxD91dnUPjtjb7-sxLvrM6RTCj96p8mfOml-pLeHzkyJD6WFBn5ABqZV3Sf1aPtOZlQ7huqqNfbB8wSukgqhr6BBTwIf69n8BPVhc-jQ1zzEcPeInqdEZqwhtybTfcpFcrIn84LBfv1f5PtkAHVtt7iatoZMXXuvijovOkc3VG0lvJ_tdAO5SkrSF548lHkS7llTHti5AujvzE24TyKA/p.jpeg" xr:uid="{F1616D9E-4E88-4750-A235-D075904BCD23}"/>
+    <hyperlink ref="X36" r:id="rId168" display="https://uc072b77bbb7522d0e1bae4e7a26.previews.dropboxusercontent.com/p/thumb/ABfMj6D5GnSlUv8zI7xmTY80DoA8D4-1C2KxlRqlEHLRfvx1dDJv1ujBqFNiKGN85vAE17TFN-XsfJixbjitWHNETuU2MyULJG6Yw5L1vSS0jMPkqVsbZfusnuzJ6MGJdmyRZnREPOdc6VdMdjqiJmwaN8n4o9usTFMoojYbgjfvTWgP2jlBopTNGX6vdBHbW98rmG_HFI_fhONfJs69aIzH8rSJYgmIHYOCQjmu21tgtsyNtXfXNPR3Fs-BzQCO5gqrlPwXSek2V3QCpTU10tWojQ9NrEguu5zuUGTU8qVJYWFFdgWISrgQt9FKTidSTGnKIQGrtduyPPD2zY3m16zoY58h3qcE3uU8ycTgtTUkk_yVtyFlqR3OaFYCcC3BQ6A/p.jpeg" xr:uid="{F3AA85B5-43D4-4ADD-8151-7CE7FC3D292B}"/>
+    <hyperlink ref="X37" r:id="rId169" display="https://uc96bbf2f337f688b574d6febbf1.previews.dropboxusercontent.com/p/thumb/ABc1TGuKocmlGAVpcMfBDsabwfjk7aHcgy6uy6KAE_W_aDoDxYLwBpw1U0IEkgy_9zUOEdXbIDe0JNOSlO1pGKZQ4kW9cw3AdNio5tToHa-t-UWzbtm-hOO-Cg32A5H8cckAGHYGnnAZ3_HHDwE-Hl5tQORjnvXklwJKEBN_qSzGleVdVf-jffvmnNVXZ1fkvwIbSg4pqEAO-k_Af9vq9DW8apkRA6xoLyALzvs7qLmRUscIeI2c0I_hWSwW-km8oN-WOVMEtUewb5O0aGBcyUf_3dtykWehNcF5UAwJfWRsP7KZXEEOiBMW5G5AUPcrXHBKmXN58jE_uS5I2gx1RIS6OEBx65JjR8Ij5Md2B-Ei_1NOa1MBDbLasUHdT97to9k/p.jpeg" xr:uid="{46A6B72A-3B71-4F00-B440-9761567FE166}"/>
+    <hyperlink ref="X39" r:id="rId170" display="https://uc11168f70a2fa011cec3f4582d2.previews.dropboxusercontent.com/p/thumb/ABfDJCFK_xjFZSJAI7sDp0tA1jUiKBGMJAt-xo9BN1YIbW0HnAr6Od0Mw-ME7zRwV3xyCI5qD4vCsJ-7n67V26SL5EMSs9wcz4KvKHYzLfdZI1aEr4VsVHSls-EeusRkUlKCjfflJvuCvRv1xslYpFfQVd4w9RqEc1XBjHBeT3OKRtyKylrMc49PklkJOf8TlhnWcJRQAWOwqCZFjT8WhAW3I3oF-oUi_rgD6fZGQui6SGMzCmpwkXh8Qgmu1FSR6L3MePtDprKQqq5Dj4sTd5tV53c04PorL7lev8kvtCnDVhoBegdiT5OOWEyHaWH7zCdDV4HLrzumCBB06CQF4HyCI7FITlLK3EOhT-vJOsy9c2L86KOrzOxgx3DEPQbt-5c/p.jpeg" xr:uid="{4DA4F55C-90E9-4708-9A82-6850AD55A48C}"/>
+    <hyperlink ref="X40" r:id="rId171" display="https://ucb66a69016ce41e67c5795cfe57.previews.dropboxusercontent.com/p/thumb/ABfFC--DxJBVzIH7Om8iMME502BsMIshfLOoVNByRYyyq6HbbYaYoJZdldu8XBQ-dVzQ__RymodHLPGZRQTq47qk-DF4EwfZlheDdz1-4a1n_4HLPAY4s4y7xznXsnQ6qbSznA1kE5F5Jf_v9695uIcaqIFbVZWXPF8nVweLMxSieoxGIXtcPnbLZOVyABmMJKhik3ETSV9EJcCHHgmugvxaWg4UbaISAEj37_i22CB613cysLZPfD79mit-HvjvLHfKqH4Q2Q5cA_ylSV2Bx5ikuN4q5Q2Mz2lKN25gKcl7Oj_xc9t15ah9i52DRJOy9XPZnhikf3EOrWjll7poJOD1sFQhie3grxWfGwAVw-93V3Pgr1gCQz0EHy4iFGZq_rM6AJVKKfGIgn3Ax_xnT4kaLyE6ACZjZLkjDqgX9_vl9w/p.jpeg" xr:uid="{1AE6DC36-A001-43E9-8330-3DF9ECF31A9B}"/>
+    <hyperlink ref="X41" r:id="rId172" display="https://ucaf3dbc0a0373492005231719aa.previews.dropboxusercontent.com/p/thumb/ABdVP3WaxiQr5i7gh_2CAOhkwRiUiZxVOF9ktpTf2URKwTQvqW1JmKon_cEu06epgleWN1MdOeEEY9HW9nkwo413Fajjzp6JZFP3u2o_BoE6sK2C0aQC15DmCA3ulAsGSNg_Z4Eci7pZ0-GF6ZhTumP_h3Efx4sQzefPXWo3I-cEJsxgFk1sdQdku2AgGxlfmIcOfrvWBxs1cc43R-tz9xOZdIJgQroTN0O3v5caQMFrtdObThpBdZLyyhTiPh9dWOYkZXsmjbWIS3Fk47O5uw2-LqUfqeN1UViIQZo2Bg7xzlasLKxawnO9ZwgGIW9UwL64TiJ4dmhOHDTtJ4GxBR-ocqx0Zzuw_H6Y8nc3GawqqsGs2mrPSKWW-U16mHXI797IKrSLmt_FvquJY9UaCKplMBv4j7cIFQELWdqSKHX3zA/p.jpeg" xr:uid="{EE303EDE-FD78-4DE9-8C2E-BCE1C5DE250E}"/>
+    <hyperlink ref="X42" r:id="rId173" display="https://uc03d661ef846c2bc7cbbd75b435.previews.dropboxusercontent.com/p/thumb/ABcpNW9qaHSUHPw3Zf8H6xod8-NzabIzD7uL_zT5jHAlBEMBGthan886y3f8pGbwFp9wMcIzVkAfo6QqKyQ5dMfl0HdthnPCFVUUnhd-CxEicCZ-oe7SWwd4Imu1HfK4DxKx2nwjYq9XmcV5rroHQyTF84Zh2rCl10og-tRZdgiNjZgPnLKWUhJuby-DV2975uzjaI4WBsvoE7yRxeqlMFz1gn8fw0Yl6jL2yZUnyzwrMpGFzaTAthjeMGJqOap_G5366FJtl-3gIL_vV2gqFAo4kdoXRINWOd8vpz_TJmYo5Vw-TnO38cGYznb51yL1dIpcFGjHM1L7djcJj7jctXa-kVO93aNGMscAgv899tTC1WFFVXofXn7oNNxJDdN7z1cdelQ5aoT3V_2PwzAYjT8JSZgUYWtZgF2QHz0XSLGPlA/p.jpeg" xr:uid="{84623BF5-32A1-4B3E-A290-0F69B53D5006}"/>
+    <hyperlink ref="X43" r:id="rId174" display="https://uc032a835146610322780cc5f186.previews.dropboxusercontent.com/p/thumb/ABfmtClbUKIZ8VqeZDpxXG5yDfb_XyIcm3lQgqB7eNaU6dQ2mv-0CSEgHbK-V-249_4DkQqIY1N7deGVWfGIeS63ZNOrYZIRLu8sSCMdDKN4D28zWgHbu-xphMcDAvsJuHmPkFU-JQuvv4A0TaiBHfPWu3noN54yXWKuA-VIsX3JbbVSPEO1zDSKVexV0G3RMIWCLHI2O1qsSNI_tcfQujRdvf8KRM95zWI3kuispy4lFEWdmjrYnoFe8slplMciUcBxTgcCXuUvtc8SFQjkc7775B53NSuE-Jw9qC7_3-I1bXI1YPLEjH9R2WlGb15vncwUJk7-wol0W5vqjr0R9Nxw0jOnkWNZtPUdcee9bkKqGU6Uz-mQgT8p_C28PQWeGku-9RJnep2OW6weOlC3g7CtnA8DvUmceB5TTqaCUmq93A/p.jpeg" xr:uid="{FE44FD91-F56B-489E-A636-2003865FFFDD}"/>
+    <hyperlink ref="X44" r:id="rId175" display="https://uc1f33a6f358eb8cb4fb479fdaec.previews.dropboxusercontent.com/p/thumb/ABchfz0joiYPxR6wzc0xUaQZm2sgs0D4o-ujq1MRjxcdmapkM0w_T2svIEy-XeEGAeA5T1WwsxoJEFNPqzCDg0izXPlee5mxEMT60OX3B2M1YNJj6xBvjXx7cBnj_F5rqgfD6xhaBrjMPD8us-6Ha2wRiE2d1lBKL-BWF7OObQXbo_S1HLm-nfq30bXm0Qv9u39T9xNwdukWbMoP88bAgU14ZB8vzYEVMwNcKmkht0_E6VPkjQentV1O7n76H3z8TS3vSe_VV6-7Ch4Fg9TYCmx5fnvak9VWzrNKJKvY1XQYMAUDj8mxUo-W-oacRBtlux12QUfzb13VAe7NejgR0IO7rfelr47R1kqDCBhkEl-fThc7Mbr8KUBoCNso2ouAPr4vcL_OBlTJltjGEy7yXFttcErr84vjECSVOxRpQWtOdQ/p.jpeg" xr:uid="{1C3DB7C7-CD31-44D3-9B51-972C11210060}"/>
+    <hyperlink ref="X45" r:id="rId176" display="https://ucec514f2625e7a4aba72b101c7f.previews.dropboxusercontent.com/p/thumb/ABeSpvtqHI0zqtgulFq0rYChM-_ampMAgUGpgr8pwrg-3iVIBdfIMT2J9uT46-ZJc9vUM66HHLRM9EoHsPdj9iL2YOTmHseY7jMOG8U5EuBQRoj-pBKPPpIWG_UHsjWU2814f7q__61AWNECXk-Q74imXeEEiZvs27t8SU2ntz9CCTXtS8xzRTCcX_VmdZBVUa3NN1-lG5pIzgf9_4qDj_PVtZtyp7IXxnJszFWNEIJIQjedlS8F9fRkGoFGCT9w_tecgnXBQeHAO8f60jn2YTrMy1VxeooesBImTc7ecQXoSEY8lR63Q7rTIX8xYQONCF24LHUCcP7fw4rA7AXNAxo11cL9GbqkftDG3gGFmRg1CsJ33023TaONJb4hEbaSHA3EbdTKFyG_BDar4VqjGM-bWvNayx6EUzuQ2lH-h-iuLg/p.jpeg" xr:uid="{437CA099-1E2B-484A-9D33-1DAB82823C80}"/>
+    <hyperlink ref="X46" r:id="rId177" display="https://uc034b5b8de8b2771327a68b2ff4.previews.dropboxusercontent.com/p/thumb/ABejOCRrQW2VG9yOfC1IyZv6ovfjmviwOMuY5qw3r2uMlmCxw50dT_5RH1Dgm5SZL8oanu35EhcrTakf8Uq8CePgGTPGn98UxxnQ2U4k38htTUTBvE9n8NbVVgeMJfBIx0edDssRwvKgEiQqI7FYGvW3hwCOdsQmRGvVcOjHCivSCc3HD6dg0woGylc_fsp4EqW7vcA88JojMTBNzyLwhrXbr2lz8WDXHIdkhhVOJlFH5yGR0GJV4LmvMKQ5E5ZYaa_kHbTD3cywOits-Lu-vu-TQHAAI-stNs2lPoP4_otl-Yer4jWjHaDnBp-6YvEIutYR06iYxxRtI73EV6P9iyJgKDdTh9TaYmSItwQSAD39nkfn8xkWLNNhtHI49XUpdp0-gYw-okzjY4FU3FMNd3CHCZUkzJd1RmjWuKPtf4x5_Q/p.jpeg" xr:uid="{28739378-A4BD-4F8E-9728-7578780591C0}"/>
+    <hyperlink ref="X47" r:id="rId178" display="https://uc4c1ddbc7cd58ae881d4fd284b9.previews.dropboxusercontent.com/p/thumb/ABd9QpLsOOMxRZqhuSpbY_KZDxOay5CdrC5buopt1llrFDQE52ZCH6LM4jH0MFb1x77azVkA8yzv5tJV4_C6c8wws-hDwDoHTK74_BSye70368Bf4k69VTGRkND6s2d0s6I_5aB0deM4MY1e_BRLCNq7UG0_bMNuMhyocTfqLvR28UhqMPDF3v0toaj7zB7iGL6SUFRTAPIK5rfa1NtSzZ3a0YkQC6ClY9QDDJhkGH30gjLQPdSNvweT-ZkE2wTqxZ5_gssOdymGu_kOhSowSAmMf5BU5-6gv4ofzPutBrVy_BMq4DPkF-DnK_dDzDK8PRpF9Xw0yv30byZBz-sm8SVbaxKOp_hBQFfsaD_-v-5MmrLHVqp2mHKtiUBQzYo5ga24NjxRgImoQpGz2k5SWOoPd50xap1UHcTwQE4rA2ZOQg/p.jpeg" xr:uid="{CF7313E7-C303-4936-9EF0-FC830697C94B}"/>
+    <hyperlink ref="X48" r:id="rId179" display="https://uc0e3e8967bf06a15c3fa3773d43.previews.dropboxusercontent.com/p/thumb/ABdc5-k1PIbBaEjEvNdW5FO1AJ8GfQSg9JIfouEyzhnGwugP1EAiLX53nED6Dt5GFGWTSHWOaiQnTE_gV6kjDaSZSFiFJ8F-W_PTtM2EuFlHuwT0dmBy9XUykwlWDSkYK9dKNa_-YPTY--h7cGNLhs4e1fW_pCX79JeLC1zYB30tIEk8DZVHODMfhkxq2-bS15gD_11DINOk8a6MVyLPjDGShkr9bRRXrvy2MPJBYCCnJJgYft3uBMSqaWQXtQBkmdkZaJSOgcY6gDnG6Zk7C32reZgS55M2OjPqd-JVcSYAaDbi5uSdVwX224cgfHWQeIJHHjo_56c0c55wTMrnhabQkbG3HWyIi1gy5Edm2KVf3PIOOhA5kp7NEEgzSFPCSMfU4UtjcKDpoEWI-EFgksG7UBY7r7avdfvDj11nx21a7Q/p.jpeg" xr:uid="{50FA09B7-ED50-446E-AE91-0DA86B3FE243}"/>
+    <hyperlink ref="X49" r:id="rId180" display="https://uc656b29d690f8216279c80811d0.previews.dropboxusercontent.com/p/thumb/ABcdyCdBMjehqr7JUqoXAUzZliwX-4LBiYsIxL6YXvze2g_8QFSsB9ti8e-MKv9hnp3wHMd49i6vImtIObrb77ZWiBgXpxxG-B1JJEhAZuFgU61HbphcHQGRvWB3PaA65x09qSsSUhkQS1YXtrW3Usi4tnglYysuMdrJe0_nUvoPEBz6mimK4BNf3IgphbfE4l2MCtl3Rqr8rgQCphu0KfJkURf-Jed07XQTaGDdlSf1-6n9BZtRSYLP7Hxz-Yj-At3X1zs5ZDbCm_rF3tFZIcPqhGGPv5ULSckOAn-YneftIgYYmnqr_ev8XOhq2qD3y7XH6J3qbLso6D5tpY13kSQ7aI56LbhTObPJ8tFx3yG0vw_25LCxTX7VA6ipalXYHiUumXRWwlkZWRGRDNJLf5n-vyjxqgCFeXqWnkxP4KUd6w/p.jpeg" xr:uid="{B74845AD-03AB-49A0-965C-E387973626C3}"/>
+    <hyperlink ref="X52" r:id="rId181" display="https://ucb4fbc484a655eef8c73cbf7c30.previews.dropboxusercontent.com/p/thumb/ABcZDNLim83J0K-hVA_vWZoiqrDgpmkXdNNR2QIpwCa1YOxCmva8G_yjzM03zTyVt73NptDzOnUyKvnhxv62g3_aYkVd_gLU4il_yaO057hCrqKcynFTFSZqtMfHrtoN1DRudiY_-GvkYytKNBOVkLnST8Kw4dtLBTYG-NE6TT-otto8Nj-yWGy-S4gqwTYkqlQwZXZ_XhoGqB1HlaUSoMQV957-6h1DReGfBz7Ry63J3b4zR60OAoKAlnQh4Iz3vE8O4Cf5bygKEBmcedtruGEwwwpN5f6W__85LISxc0lJFf485_oZ1j8hWGtqgsCUnkIo8fyqaew3fjQT8fLHWhwdTSA7s8kKQYOvSPfpomjJJWfOe9ZHu0ohYU25EhTP2epplyUo4kzJCZ5zuOqvVkWCVE7t8eaLU4uE4Fa1QxuchQ/p.jpeg" xr:uid="{F7BB6CD6-6652-4DDC-8FA6-2BE8AC9FD1A0}"/>
+    <hyperlink ref="X53" r:id="rId182" display="https://ucc78c6e58bdebc65eb75b4a15f9.previews.dropboxusercontent.com/p/thumb/ABeGuajVtgU7dybJwHogODzIMUhS0eHT4bw4tX_reFiPGvcDCLQpHheZIt-OdOF2CDMVmKpCl6XbE5dyYBC-ES96zuUfxLLAkbctGQBUGh2XlW5nHnuezoiItQdEulwkDS0N_TgmVa-U4ZeavJT2fjWHhVXHoKQo3WUNLhp3YlDQ7g1O9mBY3GhjnHoJtEDyjiYk0hLbJmYFbQfl2DUsQ-CkyWfDNK_26ckb14CPbIVzOI8H7TlP8sn2VokJ9tt9WRKW349JzAQ6M2NTQwp3A0kN27oEiynUMp2Xv8xckzDxgDx-dB6v4G3qgk8Q2PPitC1aIHogYOGhppw28L4WLtPdQpkJTs6KJIbN0YkK5QuS5nIZRXkCFz8xYR52SWdqKaVIWxQj_6HhPLugDOhk8MYLU2SINGeZkEfr18yq0d6NMA/p.jpeg" xr:uid="{AA602F52-8E31-47EC-8ABC-EC0C7F0734C0}"/>
+    <hyperlink ref="X55" r:id="rId183" display="https://uc13cc8d5a399d899796296d326c.previews.dropboxusercontent.com/p/thumb/ABe6DU0UGxC02G73DIkI0PWQj7pOR26NvgF1rHvkDf9uKA1sRH7ZcHYjEJ_ij7bhCrljskpNdyhB6loEny_XMj0A12mso2goCjcm5XbLbNzlQvJyl-pn0kktj3QIpZfm_Br20edmV9eCdyj1ZJF7bViD1y88bA4KzDtd-08BJ5I4iJRg2C1hz2hxR8XItBhebkAoiYpu1K7WJHpNycF3br9QkDmZfm2zwSemBB0pKf5WHfWFdFMD-F9K3Pig2QHfZEwpP_neNdZSp9uQng9MNDTg1HzJodQjwzV8JNr6zi0koymkEcHX08eCWOLLMpaYngxeak-LuP-4G6JJVqfqnyxmsU-QsMRIkxnjrYKQLrVAKmDf-U8BD_NhVnabBgRAVVMTtj-nOEGfEZ9AoeIMu69mY9HGFGr1k6ExIoQVlpVBAg/p.jpeg" xr:uid="{58A09EF5-31AD-4C04-B472-76E692E7CC30}"/>
+    <hyperlink ref="X64" r:id="rId184" display="https://uc7b0406223bf1daec0413cca967.previews.dropboxusercontent.com/p/thumb/ABdfMztxLH15j68nBwphpOaudt-KQehuDvZ_lIxW55GDQq5jKAntatU8nfDBLaKkTkIOCy-EKk6zbZfVvP-93hkYEOVKQ3zZYiJYA-OBwyDobkZbXH-_O2EQd8LY84HN_XgKTEn-9HSJyX622wS3zd7n9hm7sS4yk1w6dCkqq_HkqEHbGK1V9i22xhsElubbo9oI9OOpZfWU2gtcc1imtKXuvwe63FtCaVPRZZO9hNHBjWlKDjHjsu3CZatRzTfpWSHdKq28apCOGQ5uE5n9QLhRY7NBp8jHYMQc4BoN142RDsFQR7n9cc-vz0044gO090PwQ5mD2Kwo6nrXhAUzG79RalIcnzO3O1IywGPA0k7RlNvM4L-jqxRnKL7mq2CssbsECnJH1Bayb3FIwAozLISu3-BCAWOFU7YUIzdBJJReYg/p.jpeg" xr:uid="{2D2A5EAA-E27C-4378-B500-BCD520ACDE60}"/>
+    <hyperlink ref="X51" r:id="rId185" display="https://uc3c868bf0f6f47a0eea0eb045c8.previews.dropboxusercontent.com/p/thumb/ABfvKyncm0ZMnbXO0KlzkATSYszJrVT1PKESgPrSQX6W-dqCRjCyM4tFTUISjMbUcbo7KJ19dNJj3UCjqeQ_OPGbrDyHGm6w48QzLsYpl4sYcosjZLFZdn6Y4xLRCIXiSliFc2-QgWLYTN3MYm00Gb-7lpRMfOtuuuOPY8_arTzkz1uDJ7mC8sSbLrKnIknCQqB9uu81oWtXdESEwyyOr7oSMsTQzSts9p4If9iIJZAJm3pR9-SQqdERj21yWSYFL3-EcpYGEnypXggItMZy73d_d0PK56o0KRoZthnJ3XOgv6p2ANvCKJoGM_2HUIc5XSFdqyAqu66IFTwaU1LiRQGhbKSsV3yEImDP-qnMAXis1NXS6vVc7ZtjQM4Ecwl_pmy7RxejHr3aPGlqsOVA3BW-BcAoruVW1aIc2MpicXrx8A/p.jpeg" xr:uid="{B6965E7D-D6C4-492A-A0AA-E7EDEBD14558}"/>
+    <hyperlink ref="X117" r:id="rId186" display="https://uc0c68e868d69f568916df4f9c30.previews.dropboxusercontent.com/p/thumb/ABdadMC-x1JdIQE6azcIAnUZxoHQfS7DLvWVp_TG-CYvSWhO7mxYUAWvRjLTvPNtwet5zTvcWxSHIqHZThrF7C7uNZFEA0bb9xnhn9NM4UXlMs4sN6yGwkjmTqKyMXkhedfseiT1h3FfQIeGHwND8N9_G1AoKryRlBL29SJbrQcb0VauWEaeAhy5wQS0ZKKN-VpGLv6jm64kByGsCxnxvPj_mE4zg94e071cAO-55WTXgYWj58gOwls9oFJy9uvBvgkEA2fktpI58AF5jVilDZNR4YJhNU4-UdgJdjZXwZQoZQCFNuGq-fidKh5bsPrUzBuUpX272pE61eOlaI7jCDRx5oEMWdqpvK_T0R7h2Ras8sK7UlGBst59CxFjQMi_nT9koBAHvtd7vexzlF0rWJXQAWtoJ1Z7cYdP6ijrMR0pow/p.jpeg" xr:uid="{A49E3E07-37B9-4CAC-9489-7A1D862306A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>